<commit_message>
Implemented first correct calculation of required crest height
</commit_message>
<xml_diff>
--- a/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
+++ b/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JY6\github\breakwater\Notebooks\Constanta Phase III\Input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27E325B5-5A48-4DBD-9AEB-E3C8EAF7A721}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2206A65-4F63-4948-AB34-616349ED67DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{06ED436A-2CC0-4489-A506-29F94518B839}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{06ED436A-2CC0-4489-A506-29F94518B839}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="input_hydrotechnical" sheetId="5" r:id="rId5"/>
     <sheet name="Input_Cross section" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="256">
   <si>
     <t>Input</t>
   </si>
@@ -907,12 +907,24 @@
   <si>
     <t>Overtopping limit restricted access</t>
   </si>
+  <si>
+    <t>Structure normal</t>
+  </si>
+  <si>
+    <t>Safety for overtopping</t>
+  </si>
+  <si>
+    <t>safety</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="174" formatCode="0.0000000000000"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -968,6 +980,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1076,10 +1094,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1127,57 +1146,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{FADF3455-3E5D-4FF3-B5C3-EF436E5E06DA}"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="42">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="174" formatCode="0.0000000000000"/>
     </dxf>
     <dxf>
       <font>
@@ -1187,7 +1164,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color auto="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1226,6 +1203,20 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1350,6 +1341,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1369,6 +1367,16 @@
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1468,6 +1476,16 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1605,6 +1623,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1673,6 +1701,16 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1687,7 +1725,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{128A59F9-895D-4C60-8954-4F77FF691FFB}" name="Overview" displayName="Overview" ref="A2:G62" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{128A59F9-895D-4C60-8954-4F77FF691FFB}" name="Overview" displayName="Overview" ref="A2:G62" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38">
   <autoFilter ref="A2:G62" xr:uid="{C615D3FE-C5C3-4AC1-8573-2115046F6FC7}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{FDED3D30-FC03-4894-AAAE-7069E3558798}" name="Input"/>
@@ -1695,8 +1733,8 @@
     <tableColumn id="3" xr3:uid="{122DBA8D-3347-48F4-8A76-270615744B5D}" name="Unit"/>
     <tableColumn id="4" xr3:uid="{B4BA3D29-867B-4EF8-A808-EE6581BB8115}" name="Category"/>
     <tableColumn id="5" xr3:uid="{CB74FB27-39F6-4359-BAC6-C5DFAC8E01C0}" name="Used for"/>
-    <tableColumn id="6" xr3:uid="{266927E0-00C5-4D6A-BB41-21164D34B2CE}" name="Necessary input" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{30AC8882-C2A6-43C1-86B7-25C9ED481C62}" name="Remarks" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{266927E0-00C5-4D6A-BB41-21164D34B2CE}" name="Necessary input" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{30AC8882-C2A6-43C1-86B7-25C9ED481C62}" name="Remarks" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1727,58 +1765,59 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6634BB44-66AA-43C5-94C9-21ADB80AD51A}" name="input_requirements" displayName="input_requirements" ref="A1:G6" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6634BB44-66AA-43C5-94C9-21ADB80AD51A}" name="input_requirements" displayName="input_requirements" ref="A1:G6" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="A1:G6" xr:uid="{AC8FC8D0-6474-4C46-AABC-7775C18E706C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{ED5624B9-4A0A-4F41-BA44-D0E02EE32577}" name="Parameter" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{2B068622-98F3-4E2A-BE8E-A97C121E3F4C}" name="Symbol" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{4BC1E5B1-1862-4E8F-8CC1-D2F05F356929}" name="Unit " dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{F431E098-CB44-4ACA-97A5-C64500DD9528}" name="Explanation" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{C6914755-DB47-4220-827C-0984890970A0}" name="ELS" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{D3A99EAE-B2C9-4E74-B3E2-A288F4532A21}" name="SLS" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{9350B3BA-690A-42F3-BB94-29E26F161B54}" name="ULS" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{ED5624B9-4A0A-4F41-BA44-D0E02EE32577}" name="Parameter" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{2B068622-98F3-4E2A-BE8E-A97C121E3F4C}" name="Symbol" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{4BC1E5B1-1862-4E8F-8CC1-D2F05F356929}" name="Unit " dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{F431E098-CB44-4ACA-97A5-C64500DD9528}" name="Explanation" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{C6914755-DB47-4220-827C-0984890970A0}" name="ELS" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{D3A99EAE-B2C9-4E74-B3E2-A288F4532A21}" name="SLS" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{9350B3BA-690A-42F3-BB94-29E26F161B54}" name="ULS" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A63CE4AC-CF5D-406B-B465-B4984FB45555}" name="input_hydrometeo" displayName="input_hydrometeo" ref="A2:K170" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A63CE4AC-CF5D-406B-B465-B4984FB45555}" name="input_hydrometeo" displayName="input_hydrometeo" ref="A2:K170" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A2:K170" xr:uid="{8EC5B0C1-E4CA-4C7B-AA39-695D226630E3}"/>
   <tableColumns count="11">
-    <tableColumn id="6" xr3:uid="{F9A5357A-5DE4-4408-A14A-E6698FD3755F}" name="Calculation_case" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{012C1F4F-AAC2-4FD0-A162-E004B1A207F9}" name="Structure" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{BE45E132-052E-4051-A5CC-2691B8D1D576}" name="Chainage" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{CE4FADC8-9574-4B7C-9E02-F0716073BF79}" name="Offshore bin" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{C0A99159-F33E-4796-BC72-CB4DE68B9FDE}" name="Limit State" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{240593D5-435F-4039-BD0D-5B8B3FDD3128}" name="wl" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{1A72D5A3-EEEE-48D4-B8C7-0BC7A1474131}" name="Hm0" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{937FF273-2A9A-4DA7-AC8F-B2F74F1681D7}" name="dir_wave" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{24ED7C68-4403-4BB0-A849-0C22B2AF55BB}" name="Tp" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{A397DA8E-DE81-4096-A083-356358DACD29}" name="Tm-1,0" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{17652E84-F087-4BBA-B4B9-CD36B5153566}" name="Tm0,2" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{F9A5357A-5DE4-4408-A14A-E6698FD3755F}" name="Calculation_case" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{012C1F4F-AAC2-4FD0-A162-E004B1A207F9}" name="Structure" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{BE45E132-052E-4051-A5CC-2691B8D1D576}" name="Chainage" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{CE4FADC8-9574-4B7C-9E02-F0716073BF79}" name="Offshore bin" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{C0A99159-F33E-4796-BC72-CB4DE68B9FDE}" name="Limit State" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{240593D5-435F-4039-BD0D-5B8B3FDD3128}" name="wl" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{1A72D5A3-EEEE-48D4-B8C7-0BC7A1474131}" name="Hm0" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{937FF273-2A9A-4DA7-AC8F-B2F74F1681D7}" name="dir_wave" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{24ED7C68-4403-4BB0-A849-0C22B2AF55BB}" name="Tp" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{A397DA8E-DE81-4096-A083-356358DACD29}" name="Tm-1,0" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{17652E84-F087-4BBA-B4B9-CD36B5153566}" name="Tm0,2" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5DFFFB11-DDA0-4FF0-A99C-C5B40B22BB0F}" name="input_cross_section" displayName="input_cross_section" ref="A2:M9" totalsRowShown="0" tableBorderDxfId="8">
-  <autoFilter ref="A2:M9" xr:uid="{EDBA852A-A4D9-4055-8891-B74537BE60D1}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{65F89A4D-13BC-480A-9A54-9B5181E61222}" name="Structure" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{DD7D1624-C590-49ED-8883-96E10DDFDC57}" name="Chainage" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{56CAAB95-7C5D-4C77-9690-8C7E28E5E58F}" name="dir_structure" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5DFFFB11-DDA0-4FF0-A99C-C5B40B22BB0F}" name="input_cross_section" displayName="input_cross_section" ref="A2:N9" totalsRowShown="0" tableBorderDxfId="5">
+  <autoFilter ref="A2:N9" xr:uid="{EDBA852A-A4D9-4055-8891-B74537BE60D1}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{65F89A4D-13BC-480A-9A54-9B5181E61222}" name="Structure" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{DD7D1624-C590-49ED-8883-96E10DDFDC57}" name="Chainage" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{56CAAB95-7C5D-4C77-9690-8C7E28E5E58F}" name="dir_structure" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{3211485F-4253-4196-9552-5388E1C18679}" name="z_bed"/>
     <tableColumn id="5" xr3:uid="{12FF2071-DB6F-4635-AAF2-7224DB03F7AF}" name="public"/>
     <tableColumn id="6" xr3:uid="{3C50E8D0-D9A3-4D42-9184-21A91AB97D26}" name="P"/>
-    <tableColumn id="7" xr3:uid="{67557D02-D417-4935-83D4-56C7A3EC4E57}" name="tan_a"/>
+    <tableColumn id="7" xr3:uid="{67557D02-D417-4935-83D4-56C7A3EC4E57}" name="tan_a" dataDxfId="0"/>
     <tableColumn id="9" xr3:uid="{0A204ACD-A807-4615-BEB7-8F6AA353A3CD}" name="Gc"/>
-    <tableColumn id="10" xr3:uid="{0003E8D8-CC23-4555-A626-BC13BBABE9B8}" name="slope_foreshore"/>
+    <tableColumn id="10" xr3:uid="{0003E8D8-CC23-4555-A626-BC13BBABE9B8}" name="slope_foreshore" dataDxfId="3"/>
     <tableColumn id="12" xr3:uid="{74307101-79D4-4197-A798-20BAE3C12767}" name="gamma_f_c"/>
     <tableColumn id="13" xr3:uid="{30E9BE3D-820F-4565-AD86-93CC1E7A860F}" name="cot_a_rear"/>
     <tableColumn id="14" xr3:uid="{A3804960-2456-4577-852A-50CF47F120BD}" name="B"/>
     <tableColumn id="15" xr3:uid="{CDF10425-8C56-4935-8140-3DF50B45D054}" name="roundhead"/>
+    <tableColumn id="8" xr3:uid="{C1C74C48-BB3B-4A8D-A9CB-54DD71D28B09}" name="safety"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3436,7 +3475,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B1 B3:B1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3779,7 +3818,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B16">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3935,7 +3974,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3948,8 +3987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAEB3671-1ED6-422F-86FB-257A56869058}">
   <dimension ref="A2:N170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9921,7 +9960,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9935,8 +9974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7027210-EB2D-4810-B641-E47C920F8A87}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9953,11 +9992,12 @@
     <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C1" s="27" t="s">
-        <v>16</v>
+        <v>253</v>
       </c>
       <c r="D1" s="27" t="s">
         <v>20</v>
@@ -9989,7 +10029,9 @@
       <c r="M1" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="N1" s="7"/>
+      <c r="N1" s="27" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
@@ -10031,6 +10073,9 @@
       <c r="M2" t="s">
         <v>227</v>
       </c>
+      <c r="N2" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
@@ -10039,11 +10084,11 @@
       <c r="B3" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="C3" s="6">
-        <v>85</v>
+      <c r="C3" s="31">
+        <v>353.4</v>
       </c>
       <c r="D3" s="31">
-        <v>-6.6</v>
+        <v>-6.61</v>
       </c>
       <c r="E3" s="31">
         <v>0</v>
@@ -10051,14 +10096,14 @@
       <c r="F3" s="31">
         <v>0.4</v>
       </c>
-      <c r="G3">
-        <v>0.75</v>
+      <c r="G3" s="33">
+        <v>0.66666666666670005</v>
       </c>
       <c r="H3" s="31">
         <v>1.5</v>
       </c>
-      <c r="I3" s="6">
-        <v>0.01</v>
+      <c r="I3" s="31">
+        <v>300</v>
       </c>
       <c r="J3" s="31">
         <v>0.55000000000000004</v>
@@ -10072,6 +10117,9 @@
       <c r="M3" s="31">
         <v>1</v>
       </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
@@ -10080,11 +10128,11 @@
       <c r="B4" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="C4" s="6">
-        <v>85</v>
+      <c r="C4" s="31">
+        <v>353.4</v>
       </c>
       <c r="D4">
-        <v>-5.9</v>
+        <v>-6.52</v>
       </c>
       <c r="E4" s="31">
         <v>0</v>
@@ -10092,14 +10140,14 @@
       <c r="F4" s="31">
         <v>0.4</v>
       </c>
-      <c r="G4">
-        <v>0.67</v>
+      <c r="G4" s="33">
+        <v>0.66666666666670005</v>
       </c>
       <c r="H4" s="31">
         <v>1.5</v>
       </c>
-      <c r="I4" s="6">
-        <v>0.01</v>
+      <c r="I4" s="31">
+        <v>300</v>
       </c>
       <c r="J4" s="31">
         <v>0.55000000000000004</v>
@@ -10113,6 +10161,9 @@
       <c r="M4">
         <v>0</v>
       </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -10121,11 +10172,11 @@
       <c r="B5" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="C5" s="6">
-        <v>85</v>
+      <c r="C5" s="31">
+        <v>353.4</v>
       </c>
       <c r="D5">
-        <v>-4</v>
+        <v>-4.41</v>
       </c>
       <c r="E5" s="31">
         <v>0</v>
@@ -10133,14 +10184,14 @@
       <c r="F5" s="31">
         <v>0.4</v>
       </c>
-      <c r="G5">
-        <v>0.67</v>
+      <c r="G5" s="33">
+        <v>0.66666666666670005</v>
       </c>
       <c r="H5" s="31">
         <v>1.5</v>
       </c>
-      <c r="I5" s="6">
-        <v>0.01</v>
+      <c r="I5" s="31">
+        <v>300</v>
       </c>
       <c r="J5" s="31">
         <v>0.55000000000000004</v>
@@ -10154,6 +10205,9 @@
       <c r="M5">
         <v>0</v>
       </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
@@ -10162,11 +10216,11 @@
       <c r="B6" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="C6" s="6">
-        <v>85</v>
+      <c r="C6" s="31">
+        <v>353.4</v>
       </c>
       <c r="D6">
-        <v>-3.5</v>
+        <v>-3.32</v>
       </c>
       <c r="E6" s="31">
         <v>0</v>
@@ -10174,14 +10228,14 @@
       <c r="F6" s="31">
         <v>0.4</v>
       </c>
-      <c r="G6">
-        <v>0.67</v>
+      <c r="G6" s="33">
+        <v>0.66666666666670005</v>
       </c>
       <c r="H6" s="31">
         <v>1.5</v>
       </c>
-      <c r="I6" s="6">
-        <v>0.01</v>
+      <c r="I6" s="31">
+        <v>300</v>
       </c>
       <c r="J6" s="31">
         <v>0.55000000000000004</v>
@@ -10195,6 +10249,9 @@
       <c r="M6">
         <v>0</v>
       </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
@@ -10203,8 +10260,8 @@
       <c r="B7" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="C7" s="6">
-        <v>85</v>
+      <c r="C7" s="31">
+        <v>353.4</v>
       </c>
       <c r="D7">
         <v>-3</v>
@@ -10215,14 +10272,14 @@
       <c r="F7" s="31">
         <v>0.4</v>
       </c>
-      <c r="G7">
-        <v>0.67</v>
+      <c r="G7" s="33">
+        <v>0.66666666666670005</v>
       </c>
       <c r="H7" s="31">
         <v>1.5</v>
       </c>
-      <c r="I7" s="6">
-        <v>0.01</v>
+      <c r="I7" s="31">
+        <v>300</v>
       </c>
       <c r="J7" s="31">
         <v>0.55000000000000004</v>
@@ -10236,6 +10293,9 @@
       <c r="M7">
         <v>0</v>
       </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
@@ -10244,11 +10304,11 @@
       <c r="B8" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="C8" s="6">
-        <v>85</v>
+      <c r="C8" s="31">
+        <v>353.4</v>
       </c>
       <c r="D8">
-        <v>-2</v>
+        <v>-2.29</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -10256,14 +10316,14 @@
       <c r="F8" s="31">
         <v>0.4</v>
       </c>
-      <c r="G8">
-        <v>0.67</v>
+      <c r="G8" s="33">
+        <v>0.66666666666670005</v>
       </c>
       <c r="H8" s="31">
         <v>1.5</v>
       </c>
-      <c r="I8" s="6">
-        <v>0.01</v>
+      <c r="I8" s="31">
+        <v>300</v>
       </c>
       <c r="J8" s="31">
         <v>0.55000000000000004</v>
@@ -10277,6 +10337,9 @@
       <c r="M8">
         <v>0</v>
       </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
@@ -10285,11 +10348,11 @@
       <c r="B9" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="C9" s="6">
-        <v>85</v>
+      <c r="C9" s="31">
+        <v>353.4</v>
       </c>
       <c r="D9">
-        <v>-1.2</v>
+        <v>-1.21</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -10297,14 +10360,14 @@
       <c r="F9" s="31">
         <v>0.4</v>
       </c>
-      <c r="G9">
-        <v>0.67</v>
+      <c r="G9" s="33">
+        <v>0.66666666666670005</v>
       </c>
       <c r="H9" s="31">
         <v>1.5</v>
       </c>
-      <c r="I9" s="6">
-        <v>0.01</v>
+      <c r="I9" s="31">
+        <v>300</v>
       </c>
       <c r="J9" s="31">
         <v>0.55000000000000004</v>
@@ -10316,6 +10379,9 @@
         <v>6</v>
       </c>
       <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
         <v>0</v>
       </c>
     </row>
@@ -10329,18 +10395,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10573,6 +10639,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A202D3EF-E74A-4B50-BD9D-588EBDA690CE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -10585,14 +10659,6 @@
     <ds:schemaRef ds:uri="fc9abb88-5dc8-4425-a823-e2986ac3f199"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update overtopping for loop creation
</commit_message>
<xml_diff>
--- a/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
+++ b/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JY6\github\breakwater\Notebooks\Constanta Phase III\Input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2206A65-4F63-4948-AB34-616349ED67DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{05F97F8B-FECC-41EA-9AAF-9A10AE16922B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{06ED436A-2CC0-4489-A506-29F94518B839}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
     <sheet name="Input_Project specific" sheetId="4" r:id="rId3"/>
     <sheet name="Input_requirements" sheetId="6" r:id="rId4"/>
-    <sheet name="input_hydrotechnical" sheetId="5" r:id="rId5"/>
-    <sheet name="Input_Cross section" sheetId="8" r:id="rId6"/>
+    <sheet name="Input_Cross section" sheetId="8" r:id="rId5"/>
+    <sheet name="input_hydrotechnical" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="264">
   <si>
     <t>Input</t>
   </si>
@@ -916,13 +916,37 @@
   <si>
     <t>safety</t>
   </si>
+  <si>
+    <t>Plunging coefficient deep</t>
+  </si>
+  <si>
+    <t>Surging coefficient deep</t>
+  </si>
+  <si>
+    <t>Plunging coefficient shallow</t>
+  </si>
+  <si>
+    <t>Surging coefficient shallow</t>
+  </si>
+  <si>
+    <t>Cpl_deep</t>
+  </si>
+  <si>
+    <t>Cpl_shallow</t>
+  </si>
+  <si>
+    <t>Cs_deep</t>
+  </si>
+  <si>
+    <t>Cs_shallow</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1098,7 +1122,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1146,7 +1170,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1154,7 +1181,61 @@
   </cellStyles>
   <dxfs count="42">
     <dxf>
-      <numFmt numFmtId="174" formatCode="0.0000000000000"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000000000000"/>
     </dxf>
     <dxf>
       <font>
@@ -1203,20 +1284,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1371,16 +1438,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -1476,16 +1533,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1623,16 +1670,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1701,16 +1738,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1725,7 +1752,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{128A59F9-895D-4C60-8954-4F77FF691FFB}" name="Overview" displayName="Overview" ref="A2:G62" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{128A59F9-895D-4C60-8954-4F77FF691FFB}" name="Overview" displayName="Overview" ref="A2:G62" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39">
   <autoFilter ref="A2:G62" xr:uid="{C615D3FE-C5C3-4AC1-8573-2115046F6FC7}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{FDED3D30-FC03-4894-AAAE-7069E3558798}" name="Input"/>
@@ -1733,8 +1760,8 @@
     <tableColumn id="3" xr3:uid="{122DBA8D-3347-48F4-8A76-270615744B5D}" name="Unit"/>
     <tableColumn id="4" xr3:uid="{B4BA3D29-867B-4EF8-A808-EE6581BB8115}" name="Category"/>
     <tableColumn id="5" xr3:uid="{CB74FB27-39F6-4359-BAC6-C5DFAC8E01C0}" name="Used for"/>
-    <tableColumn id="6" xr3:uid="{266927E0-00C5-4D6A-BB41-21164D34B2CE}" name="Necessary input" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{30AC8882-C2A6-43C1-86B7-25C9ED481C62}" name="Remarks" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{266927E0-00C5-4D6A-BB41-21164D34B2CE}" name="Necessary input" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{30AC8882-C2A6-43C1-86B7-25C9ED481C62}" name="Remarks" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1751,13 +1778,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{88915663-9067-4DC4-90A4-2D7CD517273B}" name="input_project" displayName="input_project" ref="A1:E16" totalsRowShown="0">
-  <autoFilter ref="A1:E16" xr:uid="{8653FB80-28B1-42DD-ADDB-1F402573EE6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{88915663-9067-4DC4-90A4-2D7CD517273B}" name="input_project" displayName="input_project" ref="A1:E17" totalsRowShown="0">
+  <autoFilter ref="A1:E17" xr:uid="{8653FB80-28B1-42DD-ADDB-1F402573EE6E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{10575A1B-65C2-4D3D-A919-D5D631E15E73}" name="Parameter" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{9F5575C0-7208-43BD-86BC-6A3485FF384C}" name="Symbol" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{1CF28AEF-1CBA-48D2-A66A-EE6DC73C8CC9}" name="Unit " dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{FB5987BB-56D7-412F-8C95-1F5820C3E77A}" name="Explanation" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{10575A1B-65C2-4D3D-A919-D5D631E15E73}" name="Parameter" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{9F5575C0-7208-43BD-86BC-6A3485FF384C}" name="Symbol" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{1CF28AEF-1CBA-48D2-A66A-EE6DC73C8CC9}" name="Unit " dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{FB5987BB-56D7-412F-8C95-1F5820C3E77A}" name="Explanation" dataDxfId="33"/>
     <tableColumn id="4" xr3:uid="{5ABE4DA7-DB09-46BC-AF34-3D5B699627F3}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1765,59 +1792,59 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6634BB44-66AA-43C5-94C9-21ADB80AD51A}" name="input_requirements" displayName="input_requirements" ref="A1:G6" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6634BB44-66AA-43C5-94C9-21ADB80AD51A}" name="input_requirements" displayName="input_requirements" ref="A1:G6" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="A1:G6" xr:uid="{AC8FC8D0-6474-4C46-AABC-7775C18E706C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{ED5624B9-4A0A-4F41-BA44-D0E02EE32577}" name="Parameter" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{2B068622-98F3-4E2A-BE8E-A97C121E3F4C}" name="Symbol" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{4BC1E5B1-1862-4E8F-8CC1-D2F05F356929}" name="Unit " dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{F431E098-CB44-4ACA-97A5-C64500DD9528}" name="Explanation" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{C6914755-DB47-4220-827C-0984890970A0}" name="ELS" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{D3A99EAE-B2C9-4E74-B3E2-A288F4532A21}" name="SLS" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{9350B3BA-690A-42F3-BB94-29E26F161B54}" name="ULS" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{ED5624B9-4A0A-4F41-BA44-D0E02EE32577}" name="Parameter" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{2B068622-98F3-4E2A-BE8E-A97C121E3F4C}" name="Symbol" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{4BC1E5B1-1862-4E8F-8CC1-D2F05F356929}" name="Unit " dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{F431E098-CB44-4ACA-97A5-C64500DD9528}" name="Explanation" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{C6914755-DB47-4220-827C-0984890970A0}" name="ELS" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{D3A99EAE-B2C9-4E74-B3E2-A288F4532A21}" name="SLS" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{9350B3BA-690A-42F3-BB94-29E26F161B54}" name="ULS" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A63CE4AC-CF5D-406B-B465-B4984FB45555}" name="input_hydrometeo" displayName="input_hydrometeo" ref="A2:K170" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A2:K170" xr:uid="{8EC5B0C1-E4CA-4C7B-AA39-695D226630E3}"/>
-  <tableColumns count="11">
-    <tableColumn id="6" xr3:uid="{F9A5357A-5DE4-4408-A14A-E6698FD3755F}" name="Calculation_case" dataDxfId="16"/>
-    <tableColumn id="1" xr3:uid="{012C1F4F-AAC2-4FD0-A162-E004B1A207F9}" name="Structure" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{BE45E132-052E-4051-A5CC-2691B8D1D576}" name="Chainage" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{CE4FADC8-9574-4B7C-9E02-F0716073BF79}" name="Offshore bin" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{C0A99159-F33E-4796-BC72-CB4DE68B9FDE}" name="Limit State" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{240593D5-435F-4039-BD0D-5B8B3FDD3128}" name="wl" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{1A72D5A3-EEEE-48D4-B8C7-0BC7A1474131}" name="Hm0" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{937FF273-2A9A-4DA7-AC8F-B2F74F1681D7}" name="dir_wave" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{24ED7C68-4403-4BB0-A849-0C22B2AF55BB}" name="Tp" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{A397DA8E-DE81-4096-A083-356358DACD29}" name="Tm-1,0" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{17652E84-F087-4BBA-B4B9-CD36B5153566}" name="Tm0,2" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5DFFFB11-DDA0-4FF0-A99C-C5B40B22BB0F}" name="input_cross_section" displayName="input_cross_section" ref="A2:N9" totalsRowShown="0" tableBorderDxfId="9">
+  <autoFilter ref="A2:N9" xr:uid="{EDBA852A-A4D9-4055-8891-B74537BE60D1}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{65F89A4D-13BC-480A-9A54-9B5181E61222}" name="Structure" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{DD7D1624-C590-49ED-8883-96E10DDFDC57}" name="Chainage" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{56CAAB95-7C5D-4C77-9690-8C7E28E5E58F}" name="dir_structure" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{3211485F-4253-4196-9552-5388E1C18679}" name="z_bed"/>
+    <tableColumn id="5" xr3:uid="{12FF2071-DB6F-4635-AAF2-7224DB03F7AF}" name="public"/>
+    <tableColumn id="6" xr3:uid="{3C50E8D0-D9A3-4D42-9184-21A91AB97D26}" name="P"/>
+    <tableColumn id="7" xr3:uid="{67557D02-D417-4935-83D4-56C7A3EC4E57}" name="tan_a" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{0A204ACD-A807-4615-BEB7-8F6AA353A3CD}" name="Gc"/>
+    <tableColumn id="10" xr3:uid="{0003E8D8-CC23-4555-A626-BC13BBABE9B8}" name="slope_foreshore" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{74307101-79D4-4197-A798-20BAE3C12767}" name="gamma_f_c"/>
+    <tableColumn id="13" xr3:uid="{30E9BE3D-820F-4565-AD86-93CC1E7A860F}" name="cot_a_rear"/>
+    <tableColumn id="14" xr3:uid="{A3804960-2456-4577-852A-50CF47F120BD}" name="B"/>
+    <tableColumn id="15" xr3:uid="{CDF10425-8C56-4935-8140-3DF50B45D054}" name="roundhead"/>
+    <tableColumn id="8" xr3:uid="{C1C74C48-BB3B-4A8D-A9CB-54DD71D28B09}" name="safety"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5DFFFB11-DDA0-4FF0-A99C-C5B40B22BB0F}" name="input_cross_section" displayName="input_cross_section" ref="A2:N9" totalsRowShown="0" tableBorderDxfId="5">
-  <autoFilter ref="A2:N9" xr:uid="{EDBA852A-A4D9-4055-8891-B74537BE60D1}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{65F89A4D-13BC-480A-9A54-9B5181E61222}" name="Structure" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{DD7D1624-C590-49ED-8883-96E10DDFDC57}" name="Chainage" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{56CAAB95-7C5D-4C77-9690-8C7E28E5E58F}" name="dir_structure" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{3211485F-4253-4196-9552-5388E1C18679}" name="z_bed"/>
-    <tableColumn id="5" xr3:uid="{12FF2071-DB6F-4635-AAF2-7224DB03F7AF}" name="public"/>
-    <tableColumn id="6" xr3:uid="{3C50E8D0-D9A3-4D42-9184-21A91AB97D26}" name="P"/>
-    <tableColumn id="7" xr3:uid="{67557D02-D417-4935-83D4-56C7A3EC4E57}" name="tan_a" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{0A204ACD-A807-4615-BEB7-8F6AA353A3CD}" name="Gc"/>
-    <tableColumn id="10" xr3:uid="{0003E8D8-CC23-4555-A626-BC13BBABE9B8}" name="slope_foreshore" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{74307101-79D4-4197-A798-20BAE3C12767}" name="gamma_f_c"/>
-    <tableColumn id="13" xr3:uid="{30E9BE3D-820F-4565-AD86-93CC1E7A860F}" name="cot_a_rear"/>
-    <tableColumn id="14" xr3:uid="{A3804960-2456-4577-852A-50CF47F120BD}" name="B"/>
-    <tableColumn id="15" xr3:uid="{CDF10425-8C56-4935-8140-3DF50B45D054}" name="roundhead"/>
-    <tableColumn id="8" xr3:uid="{C1C74C48-BB3B-4A8D-A9CB-54DD71D28B09}" name="safety"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A63CE4AC-CF5D-406B-B465-B4984FB45555}" name="input_hydrometeo" displayName="input_hydrometeo" ref="A2:K170" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A2:K170" xr:uid="{8EC5B0C1-E4CA-4C7B-AA39-695D226630E3}"/>
+  <tableColumns count="11">
+    <tableColumn id="6" xr3:uid="{F9A5357A-5DE4-4408-A14A-E6698FD3755F}" name="Calculation_case" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{012C1F4F-AAC2-4FD0-A162-E004B1A207F9}" name="Structure" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{BE45E132-052E-4051-A5CC-2691B8D1D576}" name="Chainage" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{CE4FADC8-9574-4B7C-9E02-F0716073BF79}" name="Offshore bin" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{C0A99159-F33E-4796-BC72-CB4DE68B9FDE}" name="Limit State" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{240593D5-435F-4039-BD0D-5B8B3FDD3128}" name="wl" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{1A72D5A3-EEEE-48D4-B8C7-0BC7A1474131}" name="Hm0" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{937FF273-2A9A-4DA7-AC8F-B2F74F1681D7}" name="dir_wave" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{24ED7C68-4403-4BB0-A849-0C22B2AF55BB}" name="Tp" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{A397DA8E-DE81-4096-A083-356358DACD29}" name="Tm-1,0" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{17652E84-F087-4BBA-B4B9-CD36B5153566}" name="Tm0,2" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2126,25 +2153,25 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="30.5546875" customWidth="1"/>
-    <col min="6" max="6" width="46.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="60.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="61.5546875" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+    <col min="6" max="6" width="46.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="60.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="61.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B1" s="5"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -2167,7 +2194,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2187,7 +2214,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2207,7 +2234,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>183</v>
       </c>
@@ -2227,7 +2254,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2244,7 +2271,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2267,7 +2294,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2287,7 +2314,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2310,7 +2337,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2330,7 +2357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -2353,7 +2380,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -2373,7 +2400,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -2396,7 +2423,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -2419,7 +2446,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2442,7 +2469,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -2465,7 +2492,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -2485,7 +2512,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -2508,7 +2535,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -2531,7 +2558,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -2554,7 +2581,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>165</v>
       </c>
@@ -2577,7 +2604,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -2600,7 +2627,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>142</v>
       </c>
@@ -2623,7 +2650,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>143</v>
       </c>
@@ -2643,7 +2670,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -2666,7 +2693,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>65</v>
       </c>
@@ -2684,7 +2711,7 @@
       </c>
       <c r="G26" s="28"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -2704,7 +2731,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -2727,7 +2754,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -2751,7 +2778,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -2774,7 +2801,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -2794,7 +2821,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -2814,7 +2841,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -2837,7 +2864,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -2857,7 +2884,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>238</v>
       </c>
@@ -2877,7 +2904,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -2897,7 +2924,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -2917,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -2943,7 +2970,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>228</v>
       </c>
@@ -2963,7 +2990,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>230</v>
       </c>
@@ -2984,7 +3011,7 @@
       </c>
       <c r="G40" s="28"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>107</v>
       </c>
@@ -3004,7 +3031,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -3024,7 +3051,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -3044,7 +3071,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>113</v>
       </c>
@@ -3064,7 +3091,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>116</v>
       </c>
@@ -3087,7 +3114,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>119</v>
       </c>
@@ -3110,7 +3137,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>120</v>
       </c>
@@ -3133,7 +3160,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>124</v>
       </c>
@@ -3156,7 +3183,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>140</v>
       </c>
@@ -3179,7 +3206,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>141</v>
       </c>
@@ -3199,7 +3226,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -3219,7 +3246,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>147</v>
       </c>
@@ -3245,7 +3272,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>147</v>
       </c>
@@ -3271,7 +3298,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>147</v>
       </c>
@@ -3297,7 +3324,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>152</v>
       </c>
@@ -3320,7 +3347,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>159</v>
       </c>
@@ -3343,7 +3370,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>161</v>
       </c>
@@ -3366,7 +3393,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>162</v>
       </c>
@@ -3386,7 +3413,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>167</v>
       </c>
@@ -3406,7 +3433,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>169</v>
       </c>
@@ -3429,7 +3456,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>174</v>
       </c>
@@ -3452,7 +3479,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>177</v>
       </c>
@@ -3475,7 +3502,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B1 B3:B1048576">
-    <cfRule type="duplicateValues" dxfId="41" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3503,47 +3530,47 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>211</v>
       </c>
@@ -3558,21 +3585,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B902128-77A3-4FC4-8358-70CDD0AB45F8}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
     <col min="4" max="5" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>198</v>
       </c>
@@ -3589,7 +3616,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
@@ -3603,7 +3630,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
@@ -3617,7 +3644,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>183</v>
       </c>
@@ -3631,7 +3658,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
@@ -3645,7 +3672,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>245</v>
       </c>
@@ -3659,7 +3686,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>246</v>
       </c>
@@ -3674,7 +3701,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>247</v>
       </c>
@@ -3689,12 +3716,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>95</v>
+        <v>256</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>96</v>
+        <v>260</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>11</v>
@@ -3703,12 +3730,12 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>97</v>
+        <v>257</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>98</v>
+        <v>262</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>11</v>
@@ -3717,108 +3744,124 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="15" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E11">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D11" s="30"/>
+      <c r="E11" s="34">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>147</v>
+        <v>259</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>150</v>
+        <v>263</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
-        <v>204</v>
-      </c>
-      <c r="E12">
-        <v>1.45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="D12" s="30"/>
+      <c r="E12" s="34">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C13" s="15" t="s">
+      <c r="B13" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
         <v>204</v>
       </c>
       <c r="E13">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="C14" s="13" t="s">
+      <c r="B14" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D14" t="s">
         <v>204</v>
       </c>
       <c r="E14">
-        <v>4.4800000000000004</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C15" s="15" t="s">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D15" t="s">
         <v>204</v>
       </c>
       <c r="E15">
+        <v>4.4800000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>204</v>
+      </c>
+      <c r="E16">
         <v>1.76</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B17" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C17" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>248</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E17" s="6">
         <v>0.7</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B16">
-    <cfRule type="duplicateValues" dxfId="35" priority="2"/>
+  <conditionalFormatting sqref="B2:B17">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3833,18 +3876,18 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.44140625" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>198</v>
       </c>
@@ -3867,7 +3910,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>251</v>
       </c>
@@ -3888,7 +3931,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>252</v>
       </c>
@@ -3902,14 +3945,10 @@
       <c r="E3" s="23">
         <v>50</v>
       </c>
-      <c r="F3" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>59</v>
       </c>
@@ -3930,7 +3969,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>62</v>
       </c>
@@ -3951,7 +3990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>165</v>
       </c>
@@ -3974,7 +4013,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="30" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3984,27 +4023,451 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7027210-EB2D-4810-B641-E47C920F8A87}">
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:N3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C1" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L2" t="s">
+        <v>138</v>
+      </c>
+      <c r="M2" t="s">
+        <v>227</v>
+      </c>
+      <c r="N2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="31">
+        <v>353.4</v>
+      </c>
+      <c r="D3" s="31">
+        <v>-6.61</v>
+      </c>
+      <c r="E3" s="31">
+        <v>0</v>
+      </c>
+      <c r="F3" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="33">
+        <v>0.66666666666670005</v>
+      </c>
+      <c r="H3" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="I3" s="31">
+        <v>300</v>
+      </c>
+      <c r="J3" s="31">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K3" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="L3" s="31">
+        <v>6</v>
+      </c>
+      <c r="M3" s="31">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" s="31">
+        <v>353.4</v>
+      </c>
+      <c r="D4">
+        <v>-6.52</v>
+      </c>
+      <c r="E4" s="31">
+        <v>0</v>
+      </c>
+      <c r="F4" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="33">
+        <v>0.66666666666670005</v>
+      </c>
+      <c r="H4" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="I4" s="31">
+        <v>300</v>
+      </c>
+      <c r="J4" s="31">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K4" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="L4" s="31">
+        <v>6</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="C5" s="31">
+        <v>353.4</v>
+      </c>
+      <c r="D5">
+        <v>-4.41</v>
+      </c>
+      <c r="E5" s="31">
+        <v>0</v>
+      </c>
+      <c r="F5" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="33">
+        <v>0.66666666666670005</v>
+      </c>
+      <c r="H5" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="I5" s="31">
+        <v>300</v>
+      </c>
+      <c r="J5" s="31">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K5" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="L5" s="31">
+        <v>6</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C6" s="31">
+        <v>353.4</v>
+      </c>
+      <c r="D6">
+        <v>-3.32</v>
+      </c>
+      <c r="E6" s="31">
+        <v>0</v>
+      </c>
+      <c r="F6" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="33">
+        <v>0.66666666666670005</v>
+      </c>
+      <c r="H6" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="I6" s="31">
+        <v>300</v>
+      </c>
+      <c r="J6" s="31">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K6" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="L6" s="31">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="31">
+        <v>353.4</v>
+      </c>
+      <c r="D7">
+        <v>-3</v>
+      </c>
+      <c r="E7" s="31">
+        <v>0</v>
+      </c>
+      <c r="F7" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="33">
+        <v>0.66666666666670005</v>
+      </c>
+      <c r="H7" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="I7" s="31">
+        <v>300</v>
+      </c>
+      <c r="J7" s="31">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K7" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="L7" s="31">
+        <v>6</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C8" s="31">
+        <v>353.4</v>
+      </c>
+      <c r="D8">
+        <v>-2.29</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="33">
+        <v>0.66666666666670005</v>
+      </c>
+      <c r="H8" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="I8" s="31">
+        <v>300</v>
+      </c>
+      <c r="J8" s="31">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K8" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="L8" s="31">
+        <v>6</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="C9" s="31">
+        <v>353.4</v>
+      </c>
+      <c r="D9">
+        <v>-1.21</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="33">
+        <v>0.66666666666670005</v>
+      </c>
+      <c r="H9" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="I9" s="31">
+        <v>300</v>
+      </c>
+      <c r="J9" s="31">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K9" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="L9" s="31">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAEB3671-1ED6-422F-86FB-257A56869058}">
   <dimension ref="A2:N170"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>250</v>
       </c>
@@ -4039,7 +4502,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="23">
         <v>1</v>
       </c>
@@ -4074,7 +4537,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="23">
         <v>2</v>
       </c>
@@ -4109,7 +4572,7 @@
         <v>4.8499999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="23">
         <v>3</v>
       </c>
@@ -4144,7 +4607,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="23">
         <v>4</v>
       </c>
@@ -4179,7 +4642,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="23">
         <v>5</v>
       </c>
@@ -4214,7 +4677,7 @@
         <v>4.7699999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="23">
         <v>6</v>
       </c>
@@ -4249,7 +4712,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23">
         <v>7</v>
       </c>
@@ -4284,7 +4747,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="23">
         <v>8</v>
       </c>
@@ -4319,7 +4782,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="23">
         <v>9</v>
       </c>
@@ -4354,7 +4817,7 @@
         <v>2.74</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="23">
         <v>10</v>
       </c>
@@ -4389,7 +4852,7 @@
         <v>4.79</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="23">
         <v>11</v>
       </c>
@@ -4424,7 +4887,7 @@
         <v>6.61</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="23">
         <v>12</v>
       </c>
@@ -4459,7 +4922,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="23">
         <v>13</v>
       </c>
@@ -4494,7 +4957,7 @@
         <v>4.8899999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="23">
         <v>14</v>
       </c>
@@ -4529,7 +4992,7 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="23">
         <v>15</v>
       </c>
@@ -4564,7 +5027,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="23">
         <v>16</v>
       </c>
@@ -4599,7 +5062,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="23">
         <v>17</v>
       </c>
@@ -4634,7 +5097,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="23">
         <v>18</v>
       </c>
@@ -4669,7 +5132,7 @@
         <v>4.91</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="23">
         <v>19</v>
       </c>
@@ -4704,7 +5167,7 @@
         <v>6.88</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="23">
         <v>20</v>
       </c>
@@ -4739,7 +5202,7 @@
         <v>6.52</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="23">
         <v>21</v>
       </c>
@@ -4774,7 +5237,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="23">
         <v>22</v>
       </c>
@@ -4809,7 +5272,7 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="23">
         <v>23</v>
       </c>
@@ -4844,7 +5307,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="23">
         <v>24</v>
       </c>
@@ -4879,7 +5342,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="23">
         <v>25</v>
       </c>
@@ -4914,7 +5377,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="23">
         <v>26</v>
       </c>
@@ -4949,7 +5412,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="23">
         <v>27</v>
       </c>
@@ -4984,7 +5447,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="23">
         <v>28</v>
       </c>
@@ -5019,7 +5482,7 @@
         <v>6.87</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="23">
         <v>29</v>
       </c>
@@ -5054,7 +5517,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="23">
         <v>30</v>
       </c>
@@ -5089,7 +5552,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="23">
         <v>31</v>
       </c>
@@ -5124,7 +5587,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="23">
         <v>32</v>
       </c>
@@ -5159,7 +5622,7 @@
         <v>2.76</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="23">
         <v>33</v>
       </c>
@@ -5194,7 +5657,7 @@
         <v>2.77</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="23">
         <v>34</v>
       </c>
@@ -5229,7 +5692,7 @@
         <v>5.77</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="23">
         <v>35</v>
       </c>
@@ -5264,7 +5727,7 @@
         <v>7.46</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="23">
         <v>36</v>
       </c>
@@ -5299,7 +5762,7 @@
         <v>7.11</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="23">
         <v>37</v>
       </c>
@@ -5334,7 +5797,7 @@
         <v>4.97</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="23">
         <v>38</v>
       </c>
@@ -5369,7 +5832,7 @@
         <v>4.08</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="23">
         <v>39</v>
       </c>
@@ -5404,7 +5867,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="23">
         <v>40</v>
       </c>
@@ -5439,7 +5902,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="23">
         <v>41</v>
       </c>
@@ -5474,7 +5937,7 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="23">
         <v>42</v>
       </c>
@@ -5509,7 +5972,7 @@
         <v>5.97</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="23">
         <v>43</v>
       </c>
@@ -5544,7 +6007,7 @@
         <v>7.56</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="23">
         <v>44</v>
       </c>
@@ -5579,7 +6042,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="23">
         <v>45</v>
       </c>
@@ -5614,7 +6077,7 @@
         <v>5.07</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="23">
         <v>46</v>
       </c>
@@ -5649,7 +6112,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="23">
         <v>47</v>
       </c>
@@ -5684,7 +6147,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="23">
         <v>48</v>
       </c>
@@ -5719,7 +6182,7 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="23">
         <v>49</v>
       </c>
@@ -5754,7 +6217,7 @@
         <v>3.37</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="23">
         <v>50</v>
       </c>
@@ -5789,7 +6252,7 @@
         <v>6.43</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="23">
         <v>51</v>
       </c>
@@ -5824,7 +6287,7 @@
         <v>7.83</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="23">
         <v>52</v>
       </c>
@@ -5859,7 +6322,7 @@
         <v>7.59</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="23">
         <v>53</v>
       </c>
@@ -5894,7 +6357,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="23">
         <v>54</v>
       </c>
@@ -5929,7 +6392,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="23">
         <v>55</v>
       </c>
@@ -5964,7 +6427,7 @@
         <v>4.22</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="23">
         <v>56</v>
       </c>
@@ -5999,7 +6462,7 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="23">
         <v>57</v>
       </c>
@@ -6034,7 +6497,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="23">
         <v>58</v>
       </c>
@@ -6069,7 +6532,7 @@
         <v>8.94</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="23">
         <v>59</v>
       </c>
@@ -6104,7 +6567,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="23">
         <v>60</v>
       </c>
@@ -6139,7 +6602,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="23">
         <v>61</v>
       </c>
@@ -6174,7 +6637,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="23">
         <v>62</v>
       </c>
@@ -6209,7 +6672,7 @@
         <v>6.71</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="23">
         <v>63</v>
       </c>
@@ -6244,7 +6707,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="23">
         <v>64</v>
       </c>
@@ -6279,7 +6742,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="23">
         <v>65</v>
       </c>
@@ -6314,7 +6777,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="23">
         <v>66</v>
       </c>
@@ -6349,7 +6812,7 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="23">
         <v>67</v>
       </c>
@@ -6384,7 +6847,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="23">
         <v>68</v>
       </c>
@@ -6419,7 +6882,7 @@
         <v>10.59</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="23">
         <v>69</v>
       </c>
@@ -6454,7 +6917,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="23">
         <v>70</v>
       </c>
@@ -6489,7 +6952,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="23">
         <v>71</v>
       </c>
@@ -6524,7 +6987,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="23">
         <v>72</v>
       </c>
@@ -6559,7 +7022,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="23">
         <v>73</v>
       </c>
@@ -6594,7 +7057,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="23">
         <v>74</v>
       </c>
@@ -6629,7 +7092,7 @@
         <v>9.2100000000000009</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="23">
         <v>75</v>
       </c>
@@ -6667,7 +7130,7 @@
       <c r="M77" s="7"/>
       <c r="N77" s="7"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="23">
         <v>76</v>
       </c>
@@ -6705,7 +7168,7 @@
       <c r="M78" s="7"/>
       <c r="N78" s="7"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="23">
         <v>77</v>
       </c>
@@ -6743,7 +7206,7 @@
       <c r="M79" s="7"/>
       <c r="N79" s="7"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="23">
         <v>78</v>
       </c>
@@ -6781,7 +7244,7 @@
       <c r="M80" s="7"/>
       <c r="N80" s="7"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="23">
         <v>79</v>
       </c>
@@ -6819,7 +7282,7 @@
       <c r="M81" s="7"/>
       <c r="N81" s="7"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="23">
         <v>80</v>
       </c>
@@ -6857,7 +7320,7 @@
       <c r="M82" s="7"/>
       <c r="N82" s="7"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="23">
         <v>81</v>
       </c>
@@ -6895,7 +7358,7 @@
       <c r="M83" s="7"/>
       <c r="N83" s="7"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="23">
         <v>82</v>
       </c>
@@ -6933,7 +7396,7 @@
       <c r="M84" s="7"/>
       <c r="N84" s="7"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="23">
         <v>83</v>
       </c>
@@ -6971,7 +7434,7 @@
       <c r="M85" s="7"/>
       <c r="N85" s="7"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="23">
         <v>84</v>
       </c>
@@ -7009,7 +7472,7 @@
       <c r="M86" s="7"/>
       <c r="N86" s="7"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="23">
         <v>85</v>
       </c>
@@ -7047,7 +7510,7 @@
       <c r="M87" s="7"/>
       <c r="N87" s="7"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="23">
         <v>86</v>
       </c>
@@ -7085,7 +7548,7 @@
       <c r="M88" s="7"/>
       <c r="N88" s="7"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="23">
         <v>87</v>
       </c>
@@ -7123,7 +7586,7 @@
       <c r="M89" s="7"/>
       <c r="N89" s="7"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="23">
         <v>88</v>
       </c>
@@ -7158,7 +7621,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="23">
         <v>89</v>
       </c>
@@ -7193,7 +7656,7 @@
         <v>5.61</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="23">
         <v>90</v>
       </c>
@@ -7228,7 +7691,7 @@
         <v>9.56</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="23">
         <v>91</v>
       </c>
@@ -7263,7 +7726,7 @@
         <v>10.29</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="23">
         <v>92</v>
       </c>
@@ -7298,7 +7761,7 @@
         <v>10.81</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="23">
         <v>93</v>
       </c>
@@ -7333,7 +7796,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="23">
         <v>94</v>
       </c>
@@ -7368,7 +7831,7 @@
         <v>7.44</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="23">
         <v>95</v>
       </c>
@@ -7403,7 +7866,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="23">
         <v>96</v>
       </c>
@@ -7438,7 +7901,7 @@
         <v>2.23</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="23">
         <v>97</v>
       </c>
@@ -7473,7 +7936,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="23">
         <v>98</v>
       </c>
@@ -7508,7 +7971,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="23">
         <v>99</v>
       </c>
@@ -7543,7 +8006,7 @@
         <v>10.32</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="23">
         <v>100</v>
       </c>
@@ -7578,7 +8041,7 @@
         <v>10.84</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="23">
         <v>101</v>
       </c>
@@ -7613,7 +8076,7 @@
         <v>8.51</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="23">
         <v>102</v>
       </c>
@@ -7648,7 +8111,7 @@
         <v>7.57</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="23">
         <v>103</v>
       </c>
@@ -7683,7 +8146,7 @@
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="23">
         <v>104</v>
       </c>
@@ -7718,7 +8181,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="23">
         <v>105</v>
       </c>
@@ -7753,7 +8216,7 @@
         <v>6.23</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="23">
         <v>106</v>
       </c>
@@ -7788,7 +8251,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="23">
         <v>107</v>
       </c>
@@ -7823,7 +8286,7 @@
         <v>10.43</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="23">
         <v>108</v>
       </c>
@@ -7858,7 +8321,7 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="23">
         <v>109</v>
       </c>
@@ -7893,7 +8356,7 @@
         <v>8.7200000000000006</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="23">
         <v>110</v>
       </c>
@@ -7928,7 +8391,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="23">
         <v>111</v>
       </c>
@@ -7963,7 +8426,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="23">
         <v>112</v>
       </c>
@@ -7998,7 +8461,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="23">
         <v>113</v>
       </c>
@@ -8033,7 +8496,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="23">
         <v>114</v>
       </c>
@@ -8068,7 +8531,7 @@
         <v>8.94</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="23">
         <v>115</v>
       </c>
@@ -8103,7 +8566,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="23">
         <v>116</v>
       </c>
@@ -8138,7 +8601,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="23">
         <v>117</v>
       </c>
@@ -8173,7 +8636,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="23">
         <v>118</v>
       </c>
@@ -8208,7 +8671,7 @@
         <v>6.71</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="23">
         <v>119</v>
       </c>
@@ -8243,7 +8706,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="23">
         <v>120</v>
       </c>
@@ -8278,7 +8741,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="23">
         <v>121</v>
       </c>
@@ -8313,7 +8776,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="23">
         <v>122</v>
       </c>
@@ -8348,7 +8811,7 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="23">
         <v>123</v>
       </c>
@@ -8383,7 +8846,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="23">
         <v>124</v>
       </c>
@@ -8418,7 +8881,7 @@
         <v>10.59</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="23">
         <v>125</v>
       </c>
@@ -8453,7 +8916,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="23">
         <v>126</v>
       </c>
@@ -8488,7 +8951,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="23">
         <v>127</v>
       </c>
@@ -8523,7 +8986,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="23">
         <v>128</v>
       </c>
@@ -8558,7 +9021,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="23">
         <v>129</v>
       </c>
@@ -8593,7 +9056,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="23">
         <v>130</v>
       </c>
@@ -8628,7 +9091,7 @@
         <v>9.2100000000000009</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="23">
         <v>131</v>
       </c>
@@ -8663,7 +9126,7 @@
         <v>10.11</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="23">
         <v>132</v>
       </c>
@@ -8698,7 +9161,7 @@
         <v>10.67</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="23">
         <v>133</v>
       </c>
@@ -8733,7 +9196,7 @@
         <v>8.11</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="23">
         <v>134</v>
       </c>
@@ -8768,7 +9231,7 @@
         <v>7.09</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="23">
         <v>135</v>
       </c>
@@ -8803,7 +9266,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="23">
         <v>136</v>
       </c>
@@ -8838,7 +9301,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="23">
         <v>137</v>
       </c>
@@ -8873,7 +9336,7 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="23">
         <v>138</v>
       </c>
@@ -8908,7 +9371,7 @@
         <v>9.4499999999999993</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="23">
         <v>139</v>
       </c>
@@ -8943,7 +9406,7 @@
         <v>10.23</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="23">
         <v>140</v>
       </c>
@@ -8978,7 +9441,7 @@
         <v>10.76</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="23">
         <v>141</v>
       </c>
@@ -9013,7 +9476,7 @@
         <v>8.31</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="23">
         <v>142</v>
       </c>
@@ -9048,7 +9511,7 @@
         <v>7.26</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="23">
         <v>143</v>
       </c>
@@ -9083,7 +9546,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="23">
         <v>144</v>
       </c>
@@ -9118,7 +9581,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="23">
         <v>145</v>
       </c>
@@ -9153,7 +9616,7 @@
         <v>5.61</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="23">
         <v>146</v>
       </c>
@@ -9188,7 +9651,7 @@
         <v>9.56</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="23">
         <v>147</v>
       </c>
@@ -9223,7 +9686,7 @@
         <v>10.29</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="23">
         <v>148</v>
       </c>
@@ -9258,7 +9721,7 @@
         <v>10.81</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="23">
         <v>149</v>
       </c>
@@ -9293,7 +9756,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="23">
         <v>150</v>
       </c>
@@ -9328,7 +9791,7 @@
         <v>7.44</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="23">
         <v>151</v>
       </c>
@@ -9363,7 +9826,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="23">
         <v>152</v>
       </c>
@@ -9398,7 +9861,7 @@
         <v>2.23</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="23">
         <v>153</v>
       </c>
@@ -9433,7 +9896,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="23">
         <v>154</v>
       </c>
@@ -9468,7 +9931,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="23">
         <v>155</v>
       </c>
@@ -9503,7 +9966,7 @@
         <v>10.32</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="23">
         <v>156</v>
       </c>
@@ -9538,7 +10001,7 @@
         <v>10.84</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="23">
         <v>157</v>
       </c>
@@ -9573,7 +10036,7 @@
         <v>8.51</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="23">
         <v>158</v>
       </c>
@@ -9608,7 +10071,7 @@
         <v>7.57</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="23">
         <v>159</v>
       </c>
@@ -9643,7 +10106,7 @@
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="23">
         <v>160</v>
       </c>
@@ -9678,7 +10141,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="23">
         <v>161</v>
       </c>
@@ -9713,7 +10176,7 @@
         <v>6.23</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="23">
         <v>162</v>
       </c>
@@ -9748,7 +10211,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="23">
         <v>163</v>
       </c>
@@ -9783,7 +10246,7 @@
         <v>10.43</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="23">
         <v>164</v>
       </c>
@@ -9818,7 +10281,7 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="23">
         <v>165</v>
       </c>
@@ -9853,7 +10316,7 @@
         <v>8.7200000000000006</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="23">
         <v>166</v>
       </c>
@@ -9888,7 +10351,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="23">
         <v>167</v>
       </c>
@@ -9923,7 +10386,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="23">
         <v>168</v>
       </c>
@@ -9960,7 +10423,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2">
-    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9970,443 +10433,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7027210-EB2D-4810-B641-E47C920F8A87}">
-  <dimension ref="A1:N9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="10.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C1" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="K1" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="M1" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="N1" s="27" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="C2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J2" t="s">
-        <v>135</v>
-      </c>
-      <c r="K2" t="s">
-        <v>137</v>
-      </c>
-      <c r="L2" t="s">
-        <v>138</v>
-      </c>
-      <c r="M2" t="s">
-        <v>227</v>
-      </c>
-      <c r="N2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="C3" s="31">
-        <v>353.4</v>
-      </c>
-      <c r="D3" s="31">
-        <v>-6.61</v>
-      </c>
-      <c r="E3" s="31">
-        <v>0</v>
-      </c>
-      <c r="F3" s="31">
-        <v>0.4</v>
-      </c>
-      <c r="G3" s="33">
-        <v>0.66666666666670005</v>
-      </c>
-      <c r="H3" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="I3" s="31">
-        <v>300</v>
-      </c>
-      <c r="J3" s="31">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="K3" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="L3" s="31">
-        <v>6</v>
-      </c>
-      <c r="M3" s="31">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="C4" s="31">
-        <v>353.4</v>
-      </c>
-      <c r="D4">
-        <v>-6.52</v>
-      </c>
-      <c r="E4" s="31">
-        <v>0</v>
-      </c>
-      <c r="F4" s="31">
-        <v>0.4</v>
-      </c>
-      <c r="G4" s="33">
-        <v>0.66666666666670005</v>
-      </c>
-      <c r="H4" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="I4" s="31">
-        <v>300</v>
-      </c>
-      <c r="J4" s="31">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="K4" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="L4" s="31">
-        <v>6</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="C5" s="31">
-        <v>353.4</v>
-      </c>
-      <c r="D5">
-        <v>-4.41</v>
-      </c>
-      <c r="E5" s="31">
-        <v>0</v>
-      </c>
-      <c r="F5" s="31">
-        <v>0.4</v>
-      </c>
-      <c r="G5" s="33">
-        <v>0.66666666666670005</v>
-      </c>
-      <c r="H5" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="I5" s="31">
-        <v>300</v>
-      </c>
-      <c r="J5" s="31">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="K5" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="L5" s="31">
-        <v>6</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="C6" s="31">
-        <v>353.4</v>
-      </c>
-      <c r="D6">
-        <v>-3.32</v>
-      </c>
-      <c r="E6" s="31">
-        <v>0</v>
-      </c>
-      <c r="F6" s="31">
-        <v>0.4</v>
-      </c>
-      <c r="G6" s="33">
-        <v>0.66666666666670005</v>
-      </c>
-      <c r="H6" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="I6" s="31">
-        <v>300</v>
-      </c>
-      <c r="J6" s="31">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="K6" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="L6" s="31">
-        <v>6</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="C7" s="31">
-        <v>353.4</v>
-      </c>
-      <c r="D7">
-        <v>-3</v>
-      </c>
-      <c r="E7" s="31">
-        <v>0</v>
-      </c>
-      <c r="F7" s="31">
-        <v>0.4</v>
-      </c>
-      <c r="G7" s="33">
-        <v>0.66666666666670005</v>
-      </c>
-      <c r="H7" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="I7" s="31">
-        <v>300</v>
-      </c>
-      <c r="J7" s="31">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="K7" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="L7" s="31">
-        <v>6</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="C8" s="31">
-        <v>353.4</v>
-      </c>
-      <c r="D8">
-        <v>-2.29</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="31">
-        <v>0.4</v>
-      </c>
-      <c r="G8" s="33">
-        <v>0.66666666666670005</v>
-      </c>
-      <c r="H8" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="I8" s="31">
-        <v>300</v>
-      </c>
-      <c r="J8" s="31">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="K8" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="L8" s="31">
-        <v>6</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="C9" s="31">
-        <v>353.4</v>
-      </c>
-      <c r="D9">
-        <v>-1.21</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="31">
-        <v>0.4</v>
-      </c>
-      <c r="G9" s="33">
-        <v>0.66666666666670005</v>
-      </c>
-      <c r="H9" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="I9" s="31">
-        <v>300</v>
-      </c>
-      <c r="J9" s="31">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="K9" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="L9" s="31">
-        <v>6</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10639,14 +10678,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A202D3EF-E74A-4B50-BD9D-588EBDA690CE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -10659,6 +10690,14 @@
     <ds:schemaRef ds:uri="fc9abb88-5dc8-4425-a823-e2986ac3f199"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added functions for determination of rear side stability
</commit_message>
<xml_diff>
--- a/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
+++ b/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JY6\github\breakwater\Notebooks\Constanta Phase III\Input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2920953B-2B0C-465C-B8EE-357A7F1554FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{027E285B-CEFC-45F9-8B7B-6BCC3B932875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{06ED436A-2CC0-4489-A506-29F94518B839}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{06ED436A-2CC0-4489-A506-29F94518B839}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="282">
   <si>
     <t>Input</t>
   </si>
@@ -960,15 +960,9 @@
     <t>No</t>
   </si>
   <si>
-    <t>Maximum wave incidence</t>
-  </si>
-  <si>
     <t>beta_max</t>
   </si>
   <si>
-    <t>Increse factor for rock roundheads</t>
-  </si>
-  <si>
     <t>Damage level</t>
   </si>
   <si>
@@ -988,6 +982,18 @@
   </si>
   <si>
     <t>Hudson design values</t>
+  </si>
+  <si>
+    <t>Dn50 increase factor for rock roundheads</t>
+  </si>
+  <si>
+    <t>Maximum wave incidence for armour stability</t>
+  </si>
+  <si>
+    <t>crest_roughness</t>
+  </si>
+  <si>
+    <t>rough</t>
   </si>
 </sst>
 </file>
@@ -1255,16 +1261,44 @@
   </cellStyles>
   <dxfs count="46">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1372,16 +1406,6 @@
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1592,16 +1616,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1735,14 +1749,16 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -1814,16 +1830,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1838,7 +1844,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{128A59F9-895D-4C60-8954-4F77FF691FFB}" name="Overview" displayName="Overview" ref="A2:G62" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{128A59F9-895D-4C60-8954-4F77FF691FFB}" name="Overview" displayName="Overview" ref="A2:G62" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43">
   <autoFilter ref="A2:G62" xr:uid="{C615D3FE-C5C3-4AC1-8573-2115046F6FC7}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{FDED3D30-FC03-4894-AAAE-7069E3558798}" name="Input"/>
@@ -1846,8 +1852,8 @@
     <tableColumn id="3" xr3:uid="{122DBA8D-3347-48F4-8A76-270615744B5D}" name="Unit"/>
     <tableColumn id="4" xr3:uid="{B4BA3D29-867B-4EF8-A808-EE6581BB8115}" name="Category"/>
     <tableColumn id="5" xr3:uid="{CB74FB27-39F6-4359-BAC6-C5DFAC8E01C0}" name="Used for"/>
-    <tableColumn id="6" xr3:uid="{266927E0-00C5-4D6A-BB41-21164D34B2CE}" name="Necessary input" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{30AC8882-C2A6-43C1-86B7-25C9ED481C62}" name="Remarks" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{266927E0-00C5-4D6A-BB41-21164D34B2CE}" name="Necessary input" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{30AC8882-C2A6-43C1-86B7-25C9ED481C62}" name="Remarks" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1869,23 +1875,23 @@
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{32645932-B206-41E7-B1E9-2A52D9AE0D60}" name="Limit State"/>
     <tableColumn id="1" xr3:uid="{B6826C86-D95D-4464-8196-B4E1CEBC5F0A}" name="Nod"/>
-    <tableColumn id="2" xr3:uid="{12FE237E-CE70-4E63-BE4C-9D0365BAB8AC}" name="Accropode II-trunk" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{3045C02B-DCDC-42A1-B50F-88D0E610E62A}" name="Accropode II-roundhead" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{0280B610-A0B2-48C8-AB40-3AE6F87EDE4A}" name="Xbloc-trunk" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{C26BCBB6-089E-47C5-9394-EA17687F6843}" name="Xbloc-roundhead" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{12FE237E-CE70-4E63-BE4C-9D0365BAB8AC}" name="Accropode II-trunk" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{3045C02B-DCDC-42A1-B50F-88D0E610E62A}" name="Accropode II-roundhead" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{0280B610-A0B2-48C8-AB40-3AE6F87EDE4A}" name="Xbloc-trunk" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{C26BCBB6-089E-47C5-9394-EA17687F6843}" name="Xbloc-roundhead" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{88915663-9067-4DC4-90A4-2D7CD517273B}" name="input_project" displayName="input_project" ref="A1:E20" totalsRowShown="0">
-  <autoFilter ref="A1:E20" xr:uid="{8653FB80-28B1-42DD-ADDB-1F402573EE6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{88915663-9067-4DC4-90A4-2D7CD517273B}" name="input_project" displayName="input_project" ref="A1:E17" totalsRowShown="0">
+  <autoFilter ref="A1:E17" xr:uid="{8653FB80-28B1-42DD-ADDB-1F402573EE6E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{10575A1B-65C2-4D3D-A919-D5D631E15E73}" name="Parameter" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{9F5575C0-7208-43BD-86BC-6A3485FF384C}" name="Symbol" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{1CF28AEF-1CBA-48D2-A66A-EE6DC73C8CC9}" name="Unit " dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{FB5987BB-56D7-412F-8C95-1F5820C3E77A}" name="Explanation" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{10575A1B-65C2-4D3D-A919-D5D631E15E73}" name="Parameter" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{9F5575C0-7208-43BD-86BC-6A3485FF384C}" name="Symbol" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{1CF28AEF-1CBA-48D2-A66A-EE6DC73C8CC9}" name="Unit " dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{FB5987BB-56D7-412F-8C95-1F5820C3E77A}" name="Explanation" dataDxfId="33"/>
     <tableColumn id="4" xr3:uid="{5ABE4DA7-DB09-46BC-AF34-3D5B699627F3}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1893,35 +1899,35 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6634BB44-66AA-43C5-94C9-21ADB80AD51A}" name="input_requirements" displayName="input_requirements" ref="A1:G6" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6634BB44-66AA-43C5-94C9-21ADB80AD51A}" name="input_requirements" displayName="input_requirements" ref="A1:G6" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="A1:G6" xr:uid="{AC8FC8D0-6474-4C46-AABC-7775C18E706C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{ED5624B9-4A0A-4F41-BA44-D0E02EE32577}" name="Parameter" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{2B068622-98F3-4E2A-BE8E-A97C121E3F4C}" name="Symbol" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{4BC1E5B1-1862-4E8F-8CC1-D2F05F356929}" name="Unit " dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{F431E098-CB44-4ACA-97A5-C64500DD9528}" name="Explanation" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{C6914755-DB47-4220-827C-0984890970A0}" name="ELS" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{D3A99EAE-B2C9-4E74-B3E2-A288F4532A21}" name="SLS" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{9350B3BA-690A-42F3-BB94-29E26F161B54}" name="ULS" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{ED5624B9-4A0A-4F41-BA44-D0E02EE32577}" name="Parameter" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{2B068622-98F3-4E2A-BE8E-A97C121E3F4C}" name="Symbol" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{4BC1E5B1-1862-4E8F-8CC1-D2F05F356929}" name="Unit " dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{F431E098-CB44-4ACA-97A5-C64500DD9528}" name="Explanation" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{C6914755-DB47-4220-827C-0984890970A0}" name="ELS" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{D3A99EAE-B2C9-4E74-B3E2-A288F4532A21}" name="SLS" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{9350B3BA-690A-42F3-BB94-29E26F161B54}" name="ULS" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5DFFFB11-DDA0-4FF0-A99C-C5B40B22BB0F}" name="input_cross_section" displayName="input_cross_section" ref="A2:N9" totalsRowShown="0" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5DFFFB11-DDA0-4FF0-A99C-C5B40B22BB0F}" name="input_cross_section" displayName="input_cross_section" ref="A2:N9" totalsRowShown="0" tableBorderDxfId="22">
   <autoFilter ref="A2:N9" xr:uid="{EDBA852A-A4D9-4055-8891-B74537BE60D1}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{65F89A4D-13BC-480A-9A54-9B5181E61222}" name="Structure" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{DD7D1624-C590-49ED-8883-96E10DDFDC57}" name="Chainage" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{56CAAB95-7C5D-4C77-9690-8C7E28E5E58F}" name="dir_structure" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{65F89A4D-13BC-480A-9A54-9B5181E61222}" name="Structure" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{DD7D1624-C590-49ED-8883-96E10DDFDC57}" name="Chainage" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{56CAAB95-7C5D-4C77-9690-8C7E28E5E58F}" name="dir_structure" dataDxfId="19"/>
     <tableColumn id="4" xr3:uid="{3211485F-4253-4196-9552-5388E1C18679}" name="z_bed"/>
     <tableColumn id="5" xr3:uid="{12FF2071-DB6F-4635-AAF2-7224DB03F7AF}" name="public"/>
     <tableColumn id="6" xr3:uid="{3C50E8D0-D9A3-4D42-9184-21A91AB97D26}" name="P"/>
-    <tableColumn id="7" xr3:uid="{67557D02-D417-4935-83D4-56C7A3EC4E57}" name="tan_a" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{67557D02-D417-4935-83D4-56C7A3EC4E57}" name="tan_a" dataDxfId="18"/>
     <tableColumn id="9" xr3:uid="{0A204ACD-A807-4615-BEB7-8F6AA353A3CD}" name="Gc"/>
-    <tableColumn id="10" xr3:uid="{0003E8D8-CC23-4555-A626-BC13BBABE9B8}" name="slope_foreshore" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{74307101-79D4-4197-A798-20BAE3C12767}" name="gamma_f_c"/>
+    <tableColumn id="10" xr3:uid="{0003E8D8-CC23-4555-A626-BC13BBABE9B8}" name="slope_foreshore" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{74307101-79D4-4197-A798-20BAE3C12767}" name="crest_roughness"/>
     <tableColumn id="13" xr3:uid="{30E9BE3D-820F-4565-AD86-93CC1E7A860F}" name="cot_a_rear"/>
     <tableColumn id="14" xr3:uid="{A3804960-2456-4577-852A-50CF47F120BD}" name="B"/>
     <tableColumn id="15" xr3:uid="{CDF10425-8C56-4935-8140-3DF50B45D054}" name="roundhead"/>
@@ -2254,25 +2260,25 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
-    <col min="6" max="6" width="46.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="60.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="61.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" customWidth="1"/>
+    <col min="6" max="6" width="46.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="60.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="61.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B1" s="5"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -2295,7 +2301,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2315,7 +2321,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2335,7 +2341,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>183</v>
       </c>
@@ -2355,7 +2361,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2372,7 +2378,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2395,7 +2401,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2415,7 +2421,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2438,7 +2444,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2458,7 +2464,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -2481,7 +2487,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -2501,7 +2507,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -2524,7 +2530,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -2547,7 +2553,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2570,7 +2576,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -2593,7 +2599,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -2613,7 +2619,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -2636,7 +2642,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -2659,7 +2665,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -2682,7 +2688,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>165</v>
       </c>
@@ -2705,7 +2711,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -2728,7 +2734,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>142</v>
       </c>
@@ -2751,7 +2757,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>143</v>
       </c>
@@ -2771,7 +2777,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -2794,7 +2800,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>65</v>
       </c>
@@ -2812,7 +2818,7 @@
       </c>
       <c r="G26" s="28"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -2832,7 +2838,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -2855,7 +2861,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -2879,7 +2885,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -2902,7 +2908,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -2922,7 +2928,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -2942,7 +2948,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -2965,7 +2971,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -2985,7 +2991,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>238</v>
       </c>
@@ -3005,7 +3011,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -3025,7 +3031,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -3045,7 +3051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -3071,7 +3077,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>228</v>
       </c>
@@ -3091,7 +3097,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>230</v>
       </c>
@@ -3112,7 +3118,7 @@
       </c>
       <c r="G40" s="28"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>107</v>
       </c>
@@ -3132,7 +3138,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -3152,7 +3158,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -3172,7 +3178,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>113</v>
       </c>
@@ -3192,7 +3198,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>116</v>
       </c>
@@ -3215,7 +3221,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>119</v>
       </c>
@@ -3238,7 +3244,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>120</v>
       </c>
@@ -3261,7 +3267,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>124</v>
       </c>
@@ -3284,7 +3290,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>140</v>
       </c>
@@ -3307,7 +3313,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>141</v>
       </c>
@@ -3327,7 +3333,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -3347,7 +3353,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>147</v>
       </c>
@@ -3373,7 +3379,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>147</v>
       </c>
@@ -3399,7 +3405,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>147</v>
       </c>
@@ -3425,7 +3431,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>152</v>
       </c>
@@ -3448,7 +3454,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>159</v>
       </c>
@@ -3471,7 +3477,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>161</v>
       </c>
@@ -3494,7 +3500,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>162</v>
       </c>
@@ -3514,7 +3520,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>167</v>
       </c>
@@ -3534,7 +3540,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>169</v>
       </c>
@@ -3557,7 +3563,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>174</v>
       </c>
@@ -3580,7 +3586,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>177</v>
       </c>
@@ -3603,7 +3609,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B1 B3:B1048576">
-    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3631,47 +3637,47 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>211</v>
       </c>
@@ -3688,49 +3694,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2A734E-EE5D-4E22-9A61-D491991AFF7E}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>51</v>
       </c>
       <c r="B2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D2" t="s">
         <v>274</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>275</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>276</v>
       </c>
-      <c r="E2" t="s">
-        <v>277</v>
-      </c>
-      <c r="F2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>209</v>
       </c>
@@ -3750,7 +3756,7 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>210</v>
       </c>
@@ -3780,21 +3786,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B902128-77A3-4FC4-8358-70CDD0AB45F8}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="A13" sqref="A13:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="1" max="1" width="39.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" customWidth="1"/>
     <col min="4" max="5" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>198</v>
       </c>
@@ -3811,7 +3817,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
@@ -3825,7 +3831,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
@@ -3839,7 +3845,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>183</v>
       </c>
@@ -3853,7 +3859,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
@@ -3867,7 +3873,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>245</v>
       </c>
@@ -3881,7 +3887,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>246</v>
       </c>
@@ -3895,7 +3901,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>247</v>
       </c>
@@ -3909,7 +3915,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>256</v>
       </c>
@@ -3923,7 +3929,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>257</v>
       </c>
@@ -3937,7 +3943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>258</v>
       </c>
@@ -3951,7 +3957,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>259</v>
       </c>
@@ -3966,145 +3972,94 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="C13" s="13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
         <v>204</v>
       </c>
       <c r="E13">
-        <v>1.45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C14" s="15" t="s">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>248</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="C15" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
-        <v>204</v>
-      </c>
-      <c r="E14">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="C15" s="13" t="s">
+      <c r="D15" s="37" t="s">
+        <v>266</v>
+      </c>
+      <c r="E15" s="26">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="C16" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="s">
-        <v>204</v>
-      </c>
-      <c r="E15">
-        <v>4.4800000000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C16" s="15" t="s">
+      <c r="D16" s="37" t="s">
+        <v>268</v>
+      </c>
+      <c r="E16" s="26">
+        <v>1.077</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="35" t="s">
+        <v>279</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="C17" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D16" t="s">
-        <v>204</v>
-      </c>
-      <c r="E16">
-        <v>1.76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" t="s">
-        <v>248</v>
-      </c>
-      <c r="E17" s="6">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
-        <v>265</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>264</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="37" t="s">
-        <v>266</v>
-      </c>
-      <c r="E18" s="26">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
-        <v>272</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>267</v>
-      </c>
-      <c r="C19" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="37" t="s">
+      <c r="D17" s="37" t="s">
         <v>268</v>
       </c>
-      <c r="E19" s="26">
-        <v>1.077</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
-        <v>270</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>271</v>
-      </c>
-      <c r="C20" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="37" t="s">
-        <v>268</v>
-      </c>
-      <c r="E20" s="26">
+      <c r="E17" s="26">
         <v>90</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B20">
-    <cfRule type="duplicateValues" dxfId="39" priority="3"/>
+  <conditionalFormatting sqref="B2:B17">
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4122,15 +4077,15 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
     <col min="5" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>198</v>
       </c>
@@ -4153,7 +4108,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>251</v>
       </c>
@@ -4174,7 +4129,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>252</v>
       </c>
@@ -4191,7 +4146,7 @@
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>59</v>
       </c>
@@ -4212,7 +4167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>62</v>
       </c>
@@ -4233,7 +4188,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>165</v>
       </c>
@@ -4256,7 +4211,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4269,28 +4224,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7027210-EB2D-4810-B641-E47C920F8A87}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.7109375" customWidth="1"/>
+    <col min="1" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C1" s="27" t="s">
         <v>253</v>
       </c>
@@ -4328,7 +4283,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>205</v>
       </c>
@@ -4357,7 +4312,7 @@
         <v>85</v>
       </c>
       <c r="J2" t="s">
-        <v>135</v>
+        <v>280</v>
       </c>
       <c r="K2" t="s">
         <v>137</v>
@@ -4372,7 +4327,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>212</v>
       </c>
@@ -4400,8 +4355,8 @@
       <c r="I3" s="31">
         <v>300</v>
       </c>
-      <c r="J3" s="31">
-        <v>0.55000000000000004</v>
+      <c r="J3" s="31" t="s">
+        <v>281</v>
       </c>
       <c r="K3" s="31">
         <v>1.5</v>
@@ -4416,7 +4371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>212</v>
       </c>
@@ -4444,8 +4399,8 @@
       <c r="I4" s="31">
         <v>300</v>
       </c>
-      <c r="J4" s="31">
-        <v>0.55000000000000004</v>
+      <c r="J4" s="31" t="s">
+        <v>281</v>
       </c>
       <c r="K4" s="31">
         <v>1.5</v>
@@ -4460,7 +4415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>212</v>
       </c>
@@ -4488,8 +4443,8 @@
       <c r="I5" s="31">
         <v>300</v>
       </c>
-      <c r="J5" s="31">
-        <v>0.55000000000000004</v>
+      <c r="J5" s="31" t="s">
+        <v>281</v>
       </c>
       <c r="K5" s="31">
         <v>1.5</v>
@@ -4504,7 +4459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>212</v>
       </c>
@@ -4532,8 +4487,8 @@
       <c r="I6" s="31">
         <v>300</v>
       </c>
-      <c r="J6" s="31">
-        <v>0.55000000000000004</v>
+      <c r="J6" s="31" t="s">
+        <v>281</v>
       </c>
       <c r="K6" s="31">
         <v>1.5</v>
@@ -4548,7 +4503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>212</v>
       </c>
@@ -4576,8 +4531,8 @@
       <c r="I7" s="31">
         <v>300</v>
       </c>
-      <c r="J7" s="31">
-        <v>0.55000000000000004</v>
+      <c r="J7" s="31" t="s">
+        <v>281</v>
       </c>
       <c r="K7" s="31">
         <v>1.5</v>
@@ -4592,7 +4547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>212</v>
       </c>
@@ -4620,8 +4575,8 @@
       <c r="I8" s="31">
         <v>300</v>
       </c>
-      <c r="J8" s="31">
-        <v>0.55000000000000004</v>
+      <c r="J8" s="31" t="s">
+        <v>281</v>
       </c>
       <c r="K8" s="31">
         <v>1.5</v>
@@ -4636,7 +4591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>212</v>
       </c>
@@ -4664,8 +4619,8 @@
       <c r="I9" s="31">
         <v>300</v>
       </c>
-      <c r="J9" s="31">
-        <v>0.55000000000000004</v>
+      <c r="J9" s="31" t="s">
+        <v>281</v>
       </c>
       <c r="K9" s="31">
         <v>1.5</v>
@@ -4693,24 +4648,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAEB3671-1ED6-422F-86FB-257A56869058}">
   <dimension ref="A2:N170"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>250</v>
       </c>
@@ -4745,7 +4700,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="23">
         <v>1</v>
       </c>
@@ -4780,7 +4735,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="23">
         <v>2</v>
       </c>
@@ -4815,7 +4770,7 @@
         <v>4.8499999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="23">
         <v>3</v>
       </c>
@@ -4850,7 +4805,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="23">
         <v>4</v>
       </c>
@@ -4885,7 +4840,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="23">
         <v>5</v>
       </c>
@@ -4920,7 +4875,7 @@
         <v>4.7699999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="23">
         <v>6</v>
       </c>
@@ -4955,7 +4910,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23">
         <v>7</v>
       </c>
@@ -4990,7 +4945,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="23">
         <v>8</v>
       </c>
@@ -5025,7 +4980,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="23">
         <v>9</v>
       </c>
@@ -5060,7 +5015,7 @@
         <v>2.74</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
         <v>10</v>
       </c>
@@ -5095,7 +5050,7 @@
         <v>4.79</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="23">
         <v>11</v>
       </c>
@@ -5130,7 +5085,7 @@
         <v>6.61</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="23">
         <v>12</v>
       </c>
@@ -5165,7 +5120,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="23">
         <v>13</v>
       </c>
@@ -5200,7 +5155,7 @@
         <v>4.8899999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="23">
         <v>14</v>
       </c>
@@ -5235,7 +5190,7 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
         <v>15</v>
       </c>
@@ -5270,7 +5225,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>16</v>
       </c>
@@ -5305,7 +5260,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="23">
         <v>17</v>
       </c>
@@ -5340,7 +5295,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="23">
         <v>18</v>
       </c>
@@ -5375,7 +5330,7 @@
         <v>4.91</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="23">
         <v>19</v>
       </c>
@@ -5410,7 +5365,7 @@
         <v>6.88</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="23">
         <v>20</v>
       </c>
@@ -5445,7 +5400,7 @@
         <v>6.52</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="23">
         <v>21</v>
       </c>
@@ -5480,7 +5435,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="23">
         <v>22</v>
       </c>
@@ -5515,7 +5470,7 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="23">
         <v>23</v>
       </c>
@@ -5550,7 +5505,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="23">
         <v>24</v>
       </c>
@@ -5585,7 +5540,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="23">
         <v>25</v>
       </c>
@@ -5620,7 +5575,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="23">
         <v>26</v>
       </c>
@@ -5655,7 +5610,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="23">
         <v>27</v>
       </c>
@@ -5690,7 +5645,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="23">
         <v>28</v>
       </c>
@@ -5725,7 +5680,7 @@
         <v>6.87</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="23">
         <v>29</v>
       </c>
@@ -5760,7 +5715,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="23">
         <v>30</v>
       </c>
@@ -5795,7 +5750,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="23">
         <v>31</v>
       </c>
@@ -5830,7 +5785,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="23">
         <v>32</v>
       </c>
@@ -5865,7 +5820,7 @@
         <v>2.76</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="23">
         <v>33</v>
       </c>
@@ -5900,7 +5855,7 @@
         <v>2.77</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="23">
         <v>34</v>
       </c>
@@ -5935,7 +5890,7 @@
         <v>5.77</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="23">
         <v>35</v>
       </c>
@@ -5970,7 +5925,7 @@
         <v>7.46</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="23">
         <v>36</v>
       </c>
@@ -6005,7 +5960,7 @@
         <v>7.11</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="23">
         <v>37</v>
       </c>
@@ -6040,7 +5995,7 @@
         <v>4.97</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="23">
         <v>38</v>
       </c>
@@ -6075,7 +6030,7 @@
         <v>4.08</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="23">
         <v>39</v>
       </c>
@@ -6110,7 +6065,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="23">
         <v>40</v>
       </c>
@@ -6145,7 +6100,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="23">
         <v>41</v>
       </c>
@@ -6180,7 +6135,7 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="23">
         <v>42</v>
       </c>
@@ -6215,7 +6170,7 @@
         <v>5.97</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="23">
         <v>43</v>
       </c>
@@ -6250,7 +6205,7 @@
         <v>7.56</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="23">
         <v>44</v>
       </c>
@@ -6285,7 +6240,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="23">
         <v>45</v>
       </c>
@@ -6320,7 +6275,7 @@
         <v>5.07</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="23">
         <v>46</v>
       </c>
@@ -6355,7 +6310,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="23">
         <v>47</v>
       </c>
@@ -6390,7 +6345,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="23">
         <v>48</v>
       </c>
@@ -6425,7 +6380,7 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="23">
         <v>49</v>
       </c>
@@ -6460,7 +6415,7 @@
         <v>3.37</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="23">
         <v>50</v>
       </c>
@@ -6495,7 +6450,7 @@
         <v>6.43</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="23">
         <v>51</v>
       </c>
@@ -6530,7 +6485,7 @@
         <v>7.83</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="23">
         <v>52</v>
       </c>
@@ -6565,7 +6520,7 @@
         <v>7.59</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="23">
         <v>53</v>
       </c>
@@ -6600,7 +6555,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="23">
         <v>54</v>
       </c>
@@ -6635,7 +6590,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="23">
         <v>55</v>
       </c>
@@ -6670,7 +6625,7 @@
         <v>4.22</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="23">
         <v>56</v>
       </c>
@@ -6705,7 +6660,7 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="23">
         <v>57</v>
       </c>
@@ -6740,7 +6695,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="23">
         <v>58</v>
       </c>
@@ -6775,7 +6730,7 @@
         <v>8.94</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="23">
         <v>59</v>
       </c>
@@ -6810,7 +6765,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="23">
         <v>60</v>
       </c>
@@ -6845,7 +6800,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="23">
         <v>61</v>
       </c>
@@ -6880,7 +6835,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="23">
         <v>62</v>
       </c>
@@ -6915,7 +6870,7 @@
         <v>6.71</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="23">
         <v>63</v>
       </c>
@@ -6950,7 +6905,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="23">
         <v>64</v>
       </c>
@@ -6985,7 +6940,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="23">
         <v>65</v>
       </c>
@@ -7020,7 +6975,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="23">
         <v>66</v>
       </c>
@@ -7055,7 +7010,7 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="23">
         <v>67</v>
       </c>
@@ -7090,7 +7045,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="23">
         <v>68</v>
       </c>
@@ -7125,7 +7080,7 @@
         <v>10.59</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="23">
         <v>69</v>
       </c>
@@ -7160,7 +7115,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="23">
         <v>70</v>
       </c>
@@ -7195,7 +7150,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="23">
         <v>71</v>
       </c>
@@ -7230,7 +7185,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" s="23">
         <v>72</v>
       </c>
@@ -7265,7 +7220,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="23">
         <v>73</v>
       </c>
@@ -7300,7 +7255,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="23">
         <v>74</v>
       </c>
@@ -7335,7 +7290,7 @@
         <v>9.2100000000000009</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="23">
         <v>75</v>
       </c>
@@ -7373,7 +7328,7 @@
       <c r="M77" s="7"/>
       <c r="N77" s="7"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="23">
         <v>76</v>
       </c>
@@ -7411,7 +7366,7 @@
       <c r="M78" s="7"/>
       <c r="N78" s="7"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" s="23">
         <v>77</v>
       </c>
@@ -7449,7 +7404,7 @@
       <c r="M79" s="7"/>
       <c r="N79" s="7"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" s="23">
         <v>78</v>
       </c>
@@ -7487,7 +7442,7 @@
       <c r="M80" s="7"/>
       <c r="N80" s="7"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="23">
         <v>79</v>
       </c>
@@ -7525,7 +7480,7 @@
       <c r="M81" s="7"/>
       <c r="N81" s="7"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="23">
         <v>80</v>
       </c>
@@ -7563,7 +7518,7 @@
       <c r="M82" s="7"/>
       <c r="N82" s="7"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="23">
         <v>81</v>
       </c>
@@ -7601,7 +7556,7 @@
       <c r="M83" s="7"/>
       <c r="N83" s="7"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="23">
         <v>82</v>
       </c>
@@ -7639,7 +7594,7 @@
       <c r="M84" s="7"/>
       <c r="N84" s="7"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" s="23">
         <v>83</v>
       </c>
@@ -7677,7 +7632,7 @@
       <c r="M85" s="7"/>
       <c r="N85" s="7"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" s="23">
         <v>84</v>
       </c>
@@ -7715,7 +7670,7 @@
       <c r="M86" s="7"/>
       <c r="N86" s="7"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" s="23">
         <v>85</v>
       </c>
@@ -7753,7 +7708,7 @@
       <c r="M87" s="7"/>
       <c r="N87" s="7"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" s="23">
         <v>86</v>
       </c>
@@ -7791,7 +7746,7 @@
       <c r="M88" s="7"/>
       <c r="N88" s="7"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" s="23">
         <v>87</v>
       </c>
@@ -7829,7 +7784,7 @@
       <c r="M89" s="7"/>
       <c r="N89" s="7"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" s="23">
         <v>88</v>
       </c>
@@ -7864,7 +7819,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" s="23">
         <v>89</v>
       </c>
@@ -7899,7 +7854,7 @@
         <v>5.61</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" s="23">
         <v>90</v>
       </c>
@@ -7934,7 +7889,7 @@
         <v>9.56</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" s="23">
         <v>91</v>
       </c>
@@ -7969,7 +7924,7 @@
         <v>10.29</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" s="23">
         <v>92</v>
       </c>
@@ -8004,7 +7959,7 @@
         <v>10.81</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" s="23">
         <v>93</v>
       </c>
@@ -8039,7 +7994,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" s="23">
         <v>94</v>
       </c>
@@ -8074,7 +8029,7 @@
         <v>7.44</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="23">
         <v>95</v>
       </c>
@@ -8109,7 +8064,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="23">
         <v>96</v>
       </c>
@@ -8144,7 +8099,7 @@
         <v>2.23</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="23">
         <v>97</v>
       </c>
@@ -8179,7 +8134,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="23">
         <v>98</v>
       </c>
@@ -8214,7 +8169,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="23">
         <v>99</v>
       </c>
@@ -8249,7 +8204,7 @@
         <v>10.32</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="23">
         <v>100</v>
       </c>
@@ -8284,7 +8239,7 @@
         <v>10.84</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="23">
         <v>101</v>
       </c>
@@ -8319,7 +8274,7 @@
         <v>8.51</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="23">
         <v>102</v>
       </c>
@@ -8354,7 +8309,7 @@
         <v>7.57</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="23">
         <v>103</v>
       </c>
@@ -8389,7 +8344,7 @@
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="23">
         <v>104</v>
       </c>
@@ -8424,7 +8379,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="23">
         <v>105</v>
       </c>
@@ -8459,7 +8414,7 @@
         <v>6.23</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="23">
         <v>106</v>
       </c>
@@ -8494,7 +8449,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="23">
         <v>107</v>
       </c>
@@ -8529,7 +8484,7 @@
         <v>10.43</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="23">
         <v>108</v>
       </c>
@@ -8564,7 +8519,7 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="23">
         <v>109</v>
       </c>
@@ -8599,7 +8554,7 @@
         <v>8.7200000000000006</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="23">
         <v>110</v>
       </c>
@@ -8634,7 +8589,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="23">
         <v>111</v>
       </c>
@@ -8669,7 +8624,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="23">
         <v>112</v>
       </c>
@@ -8704,7 +8659,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="23">
         <v>113</v>
       </c>
@@ -8739,7 +8694,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="23">
         <v>114</v>
       </c>
@@ -8774,7 +8729,7 @@
         <v>8.94</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="23">
         <v>115</v>
       </c>
@@ -8809,7 +8764,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="23">
         <v>116</v>
       </c>
@@ -8844,7 +8799,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="23">
         <v>117</v>
       </c>
@@ -8879,7 +8834,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="23">
         <v>118</v>
       </c>
@@ -8914,7 +8869,7 @@
         <v>6.71</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="23">
         <v>119</v>
       </c>
@@ -8949,7 +8904,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="23">
         <v>120</v>
       </c>
@@ -8984,7 +8939,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="23">
         <v>121</v>
       </c>
@@ -9019,7 +8974,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="23">
         <v>122</v>
       </c>
@@ -9054,7 +9009,7 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="23">
         <v>123</v>
       </c>
@@ -9089,7 +9044,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="23">
         <v>124</v>
       </c>
@@ -9124,7 +9079,7 @@
         <v>10.59</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="23">
         <v>125</v>
       </c>
@@ -9159,7 +9114,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="23">
         <v>126</v>
       </c>
@@ -9194,7 +9149,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="23">
         <v>127</v>
       </c>
@@ -9229,7 +9184,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="23">
         <v>128</v>
       </c>
@@ -9264,7 +9219,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="23">
         <v>129</v>
       </c>
@@ -9299,7 +9254,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" s="23">
         <v>130</v>
       </c>
@@ -9334,7 +9289,7 @@
         <v>9.2100000000000009</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" s="23">
         <v>131</v>
       </c>
@@ -9369,7 +9324,7 @@
         <v>10.11</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" s="23">
         <v>132</v>
       </c>
@@ -9404,7 +9359,7 @@
         <v>10.67</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" s="23">
         <v>133</v>
       </c>
@@ -9439,7 +9394,7 @@
         <v>8.11</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" s="23">
         <v>134</v>
       </c>
@@ -9474,7 +9429,7 @@
         <v>7.09</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137" s="23">
         <v>135</v>
       </c>
@@ -9509,7 +9464,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" s="23">
         <v>136</v>
       </c>
@@ -9544,7 +9499,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" s="23">
         <v>137</v>
       </c>
@@ -9579,7 +9534,7 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140" s="23">
         <v>138</v>
       </c>
@@ -9614,7 +9569,7 @@
         <v>9.4499999999999993</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141" s="23">
         <v>139</v>
       </c>
@@ -9649,7 +9604,7 @@
         <v>10.23</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142" s="23">
         <v>140</v>
       </c>
@@ -9684,7 +9639,7 @@
         <v>10.76</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" s="23">
         <v>141</v>
       </c>
@@ -9719,7 +9674,7 @@
         <v>8.31</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" s="23">
         <v>142</v>
       </c>
@@ -9754,7 +9709,7 @@
         <v>7.26</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" s="23">
         <v>143</v>
       </c>
@@ -9789,7 +9744,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" s="23">
         <v>144</v>
       </c>
@@ -9824,7 +9779,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" s="23">
         <v>145</v>
       </c>
@@ -9859,7 +9814,7 @@
         <v>5.61</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" s="23">
         <v>146</v>
       </c>
@@ -9894,7 +9849,7 @@
         <v>9.56</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149" s="23">
         <v>147</v>
       </c>
@@ -9929,7 +9884,7 @@
         <v>10.29</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150" s="23">
         <v>148</v>
       </c>
@@ -9964,7 +9919,7 @@
         <v>10.81</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151" s="23">
         <v>149</v>
       </c>
@@ -9999,7 +9954,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" s="23">
         <v>150</v>
       </c>
@@ -10034,7 +9989,7 @@
         <v>7.44</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" s="23">
         <v>151</v>
       </c>
@@ -10069,7 +10024,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154" s="23">
         <v>152</v>
       </c>
@@ -10104,7 +10059,7 @@
         <v>2.23</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" s="23">
         <v>153</v>
       </c>
@@ -10139,7 +10094,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" s="23">
         <v>154</v>
       </c>
@@ -10174,7 +10129,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157" s="23">
         <v>155</v>
       </c>
@@ -10209,7 +10164,7 @@
         <v>10.32</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" s="23">
         <v>156</v>
       </c>
@@ -10244,7 +10199,7 @@
         <v>10.84</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" s="23">
         <v>157</v>
       </c>
@@ -10279,7 +10234,7 @@
         <v>8.51</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" s="23">
         <v>158</v>
       </c>
@@ -10314,7 +10269,7 @@
         <v>7.57</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161" s="23">
         <v>159</v>
       </c>
@@ -10349,7 +10304,7 @@
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162" s="23">
         <v>160</v>
       </c>
@@ -10384,7 +10339,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163" s="23">
         <v>161</v>
       </c>
@@ -10419,7 +10374,7 @@
         <v>6.23</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164" s="23">
         <v>162</v>
       </c>
@@ -10454,7 +10409,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165" s="23">
         <v>163</v>
       </c>
@@ -10489,7 +10444,7 @@
         <v>10.43</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166" s="23">
         <v>164</v>
       </c>
@@ -10524,7 +10479,7 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167" s="23">
         <v>165</v>
       </c>
@@ -10559,7 +10514,7 @@
         <v>8.7200000000000006</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168" s="23">
         <v>166</v>
       </c>
@@ -10594,7 +10549,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169" s="23">
         <v>167</v>
       </c>
@@ -10629,7 +10584,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170" s="23">
         <v>168</v>
       </c>
@@ -10666,7 +10621,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2">
-    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10677,6 +10632,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008ABF17219AE49A4BA0BDD81D071BF678" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27f34586c84b8c90a2cb002f0f0fc035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fc9abb88-5dc8-4425-a823-e2986ac3f199" xmlns:ns4="13eb6276-85db-4ef3-a671-167ab07ac255" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ec505085f4519de6c764bdf3897c86a" ns3:_="" ns4:_="">
     <xsd:import namespace="fc9abb88-5dc8-4425-a823-e2986ac3f199"/>
@@ -10905,15 +10869,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -10921,6 +10876,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60595BF4-BDC7-43A9-9318-C73E99FECE97}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10935,14 +10898,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Addition of rear-side armour stability, start of toe stability
</commit_message>
<xml_diff>
--- a/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
+++ b/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JY6\github\breakwater\Notebooks\Constanta Phase III\Input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{027E285B-CEFC-45F9-8B7B-6BCC3B932875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7B95A51-FD88-41D1-B2AB-4B090A5E8482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{06ED436A-2CC0-4489-A506-29F94518B839}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{06ED436A-2CC0-4489-A506-29F94518B839}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="285">
   <si>
     <t>Input</t>
   </si>
@@ -994,6 +994,15 @@
   </si>
   <si>
     <t>rough</t>
+  </si>
+  <si>
+    <t>Slope roughness indication for rear side stability</t>
+  </si>
+  <si>
+    <t>slope_roughness</t>
+  </si>
+  <si>
+    <t>Based on Rock Manual</t>
   </si>
 </sst>
 </file>
@@ -1261,46 +1270,6 @@
   </cellStyles>
   <dxfs count="46">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -1406,6 +1375,16 @@
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1616,6 +1595,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1749,6 +1738,16 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -1830,6 +1829,16 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1844,7 +1853,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{128A59F9-895D-4C60-8954-4F77FF691FFB}" name="Overview" displayName="Overview" ref="A2:G62" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{128A59F9-895D-4C60-8954-4F77FF691FFB}" name="Overview" displayName="Overview" ref="A2:G62" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42">
   <autoFilter ref="A2:G62" xr:uid="{C615D3FE-C5C3-4AC1-8573-2115046F6FC7}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{FDED3D30-FC03-4894-AAAE-7069E3558798}" name="Input"/>
@@ -1852,8 +1861,8 @@
     <tableColumn id="3" xr3:uid="{122DBA8D-3347-48F4-8A76-270615744B5D}" name="Unit"/>
     <tableColumn id="4" xr3:uid="{B4BA3D29-867B-4EF8-A808-EE6581BB8115}" name="Category"/>
     <tableColumn id="5" xr3:uid="{CB74FB27-39F6-4359-BAC6-C5DFAC8E01C0}" name="Used for"/>
-    <tableColumn id="6" xr3:uid="{266927E0-00C5-4D6A-BB41-21164D34B2CE}" name="Necessary input" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{30AC8882-C2A6-43C1-86B7-25C9ED481C62}" name="Remarks" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{266927E0-00C5-4D6A-BB41-21164D34B2CE}" name="Necessary input" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{30AC8882-C2A6-43C1-86B7-25C9ED481C62}" name="Remarks" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1875,23 +1884,23 @@
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{32645932-B206-41E7-B1E9-2A52D9AE0D60}" name="Limit State"/>
     <tableColumn id="1" xr3:uid="{B6826C86-D95D-4464-8196-B4E1CEBC5F0A}" name="Nod"/>
-    <tableColumn id="2" xr3:uid="{12FE237E-CE70-4E63-BE4C-9D0365BAB8AC}" name="Accropode II-trunk" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{3045C02B-DCDC-42A1-B50F-88D0E610E62A}" name="Accropode II-roundhead" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{0280B610-A0B2-48C8-AB40-3AE6F87EDE4A}" name="Xbloc-trunk" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{C26BCBB6-089E-47C5-9394-EA17687F6843}" name="Xbloc-roundhead" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{12FE237E-CE70-4E63-BE4C-9D0365BAB8AC}" name="Accropode II-trunk" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{3045C02B-DCDC-42A1-B50F-88D0E610E62A}" name="Accropode II-roundhead" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{0280B610-A0B2-48C8-AB40-3AE6F87EDE4A}" name="Xbloc-trunk" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{C26BCBB6-089E-47C5-9394-EA17687F6843}" name="Xbloc-roundhead" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{88915663-9067-4DC4-90A4-2D7CD517273B}" name="input_project" displayName="input_project" ref="A1:E17" totalsRowShown="0">
-  <autoFilter ref="A1:E17" xr:uid="{8653FB80-28B1-42DD-ADDB-1F402573EE6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{88915663-9067-4DC4-90A4-2D7CD517273B}" name="input_project" displayName="input_project" ref="A1:E18" totalsRowShown="0">
+  <autoFilter ref="A1:E18" xr:uid="{8653FB80-28B1-42DD-ADDB-1F402573EE6E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{10575A1B-65C2-4D3D-A919-D5D631E15E73}" name="Parameter" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{9F5575C0-7208-43BD-86BC-6A3485FF384C}" name="Symbol" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{1CF28AEF-1CBA-48D2-A66A-EE6DC73C8CC9}" name="Unit " dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{FB5987BB-56D7-412F-8C95-1F5820C3E77A}" name="Explanation" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{10575A1B-65C2-4D3D-A919-D5D631E15E73}" name="Parameter" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{9F5575C0-7208-43BD-86BC-6A3485FF384C}" name="Symbol" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{1CF28AEF-1CBA-48D2-A66A-EE6DC73C8CC9}" name="Unit " dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{FB5987BB-56D7-412F-8C95-1F5820C3E77A}" name="Explanation" dataDxfId="31"/>
     <tableColumn id="4" xr3:uid="{5ABE4DA7-DB09-46BC-AF34-3D5B699627F3}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1899,34 +1908,34 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6634BB44-66AA-43C5-94C9-21ADB80AD51A}" name="input_requirements" displayName="input_requirements" ref="A1:G6" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6634BB44-66AA-43C5-94C9-21ADB80AD51A}" name="input_requirements" displayName="input_requirements" ref="A1:G6" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="A1:G6" xr:uid="{AC8FC8D0-6474-4C46-AABC-7775C18E706C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{ED5624B9-4A0A-4F41-BA44-D0E02EE32577}" name="Parameter" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{2B068622-98F3-4E2A-BE8E-A97C121E3F4C}" name="Symbol" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{4BC1E5B1-1862-4E8F-8CC1-D2F05F356929}" name="Unit " dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{F431E098-CB44-4ACA-97A5-C64500DD9528}" name="Explanation" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{C6914755-DB47-4220-827C-0984890970A0}" name="ELS" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{D3A99EAE-B2C9-4E74-B3E2-A288F4532A21}" name="SLS" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{9350B3BA-690A-42F3-BB94-29E26F161B54}" name="ULS" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{ED5624B9-4A0A-4F41-BA44-D0E02EE32577}" name="Parameter" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{2B068622-98F3-4E2A-BE8E-A97C121E3F4C}" name="Symbol" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{4BC1E5B1-1862-4E8F-8CC1-D2F05F356929}" name="Unit " dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{F431E098-CB44-4ACA-97A5-C64500DD9528}" name="Explanation" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{C6914755-DB47-4220-827C-0984890970A0}" name="ELS" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{D3A99EAE-B2C9-4E74-B3E2-A288F4532A21}" name="SLS" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{9350B3BA-690A-42F3-BB94-29E26F161B54}" name="ULS" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5DFFFB11-DDA0-4FF0-A99C-C5B40B22BB0F}" name="input_cross_section" displayName="input_cross_section" ref="A2:N9" totalsRowShown="0" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5DFFFB11-DDA0-4FF0-A99C-C5B40B22BB0F}" name="input_cross_section" displayName="input_cross_section" ref="A2:N9" totalsRowShown="0" tableBorderDxfId="19">
   <autoFilter ref="A2:N9" xr:uid="{EDBA852A-A4D9-4055-8891-B74537BE60D1}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{65F89A4D-13BC-480A-9A54-9B5181E61222}" name="Structure" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{DD7D1624-C590-49ED-8883-96E10DDFDC57}" name="Chainage" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{56CAAB95-7C5D-4C77-9690-8C7E28E5E58F}" name="dir_structure" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{65F89A4D-13BC-480A-9A54-9B5181E61222}" name="Structure" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{DD7D1624-C590-49ED-8883-96E10DDFDC57}" name="Chainage" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{56CAAB95-7C5D-4C77-9690-8C7E28E5E58F}" name="dir_structure" dataDxfId="16"/>
     <tableColumn id="4" xr3:uid="{3211485F-4253-4196-9552-5388E1C18679}" name="z_bed"/>
     <tableColumn id="5" xr3:uid="{12FF2071-DB6F-4635-AAF2-7224DB03F7AF}" name="public"/>
     <tableColumn id="6" xr3:uid="{3C50E8D0-D9A3-4D42-9184-21A91AB97D26}" name="P"/>
-    <tableColumn id="7" xr3:uid="{67557D02-D417-4935-83D4-56C7A3EC4E57}" name="tan_a" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{67557D02-D417-4935-83D4-56C7A3EC4E57}" name="tan_a" dataDxfId="15"/>
     <tableColumn id="9" xr3:uid="{0A204ACD-A807-4615-BEB7-8F6AA353A3CD}" name="Gc"/>
-    <tableColumn id="10" xr3:uid="{0003E8D8-CC23-4555-A626-BC13BBABE9B8}" name="slope_foreshore" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{0003E8D8-CC23-4555-A626-BC13BBABE9B8}" name="slope_foreshore" dataDxfId="14"/>
     <tableColumn id="12" xr3:uid="{74307101-79D4-4197-A798-20BAE3C12767}" name="crest_roughness"/>
     <tableColumn id="13" xr3:uid="{30E9BE3D-820F-4565-AD86-93CC1E7A860F}" name="cot_a_rear"/>
     <tableColumn id="14" xr3:uid="{A3804960-2456-4577-852A-50CF47F120BD}" name="B"/>
@@ -1938,20 +1947,20 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A63CE4AC-CF5D-406B-B465-B4984FB45555}" name="input_hydrometeo" displayName="input_hydrometeo" ref="A2:K170" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A63CE4AC-CF5D-406B-B465-B4984FB45555}" name="input_hydrometeo" displayName="input_hydrometeo" ref="A2:K170" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A2:K170" xr:uid="{8EC5B0C1-E4CA-4C7B-AA39-695D226630E3}"/>
   <tableColumns count="11">
-    <tableColumn id="6" xr3:uid="{F9A5357A-5DE4-4408-A14A-E6698FD3755F}" name="Calculation_case" dataDxfId="14"/>
-    <tableColumn id="1" xr3:uid="{012C1F4F-AAC2-4FD0-A162-E004B1A207F9}" name="Structure" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{BE45E132-052E-4051-A5CC-2691B8D1D576}" name="Chainage" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{CE4FADC8-9574-4B7C-9E02-F0716073BF79}" name="Offshore bin" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{C0A99159-F33E-4796-BC72-CB4DE68B9FDE}" name="Limit State" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{240593D5-435F-4039-BD0D-5B8B3FDD3128}" name="wl" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{1A72D5A3-EEEE-48D4-B8C7-0BC7A1474131}" name="Hm0" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{937FF273-2A9A-4DA7-AC8F-B2F74F1681D7}" name="dir_wave" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{24ED7C68-4403-4BB0-A849-0C22B2AF55BB}" name="Tp" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{A397DA8E-DE81-4096-A083-356358DACD29}" name="Tm-1,0" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{17652E84-F087-4BBA-B4B9-CD36B5153566}" name="Tm0,2" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{F9A5357A-5DE4-4408-A14A-E6698FD3755F}" name="Calculation_case" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{012C1F4F-AAC2-4FD0-A162-E004B1A207F9}" name="Structure" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{BE45E132-052E-4051-A5CC-2691B8D1D576}" name="Chainage" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{CE4FADC8-9574-4B7C-9E02-F0716073BF79}" name="Offshore bin" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{C0A99159-F33E-4796-BC72-CB4DE68B9FDE}" name="Limit State" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{240593D5-435F-4039-BD0D-5B8B3FDD3128}" name="wl" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{1A72D5A3-EEEE-48D4-B8C7-0BC7A1474131}" name="Hm0" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{937FF273-2A9A-4DA7-AC8F-B2F74F1681D7}" name="dir_wave" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{24ED7C68-4403-4BB0-A849-0C22B2AF55BB}" name="Tp" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{A397DA8E-DE81-4096-A083-356358DACD29}" name="Tm-1,0" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{17652E84-F087-4BBA-B4B9-CD36B5153566}" name="Tm0,2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2260,25 +2269,25 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="30.5546875" customWidth="1"/>
-    <col min="6" max="6" width="46.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="60.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="61.5546875" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+    <col min="6" max="6" width="46.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="60.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="61.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B1" s="5"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -2301,7 +2310,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2321,7 +2330,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2341,7 +2350,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>183</v>
       </c>
@@ -2361,7 +2370,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2378,7 +2387,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2401,7 +2410,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2421,7 +2430,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2444,7 +2453,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2464,7 +2473,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -2487,7 +2496,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -2507,7 +2516,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -2530,7 +2539,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -2553,7 +2562,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2576,7 +2585,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -2599,7 +2608,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -2619,7 +2628,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -2642,7 +2651,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -2665,7 +2674,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -2688,7 +2697,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>165</v>
       </c>
@@ -2711,7 +2720,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -2734,7 +2743,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>142</v>
       </c>
@@ -2757,7 +2766,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>143</v>
       </c>
@@ -2777,7 +2786,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -2800,7 +2809,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>65</v>
       </c>
@@ -2818,7 +2827,7 @@
       </c>
       <c r="G26" s="28"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -2838,7 +2847,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -2861,7 +2870,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -2885,7 +2894,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -2908,7 +2917,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -2928,7 +2937,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -2948,7 +2957,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -2971,7 +2980,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -2991,7 +3000,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>238</v>
       </c>
@@ -3011,7 +3020,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -3031,7 +3040,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -3051,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -3077,7 +3086,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>228</v>
       </c>
@@ -3097,7 +3106,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>230</v>
       </c>
@@ -3118,7 +3127,7 @@
       </c>
       <c r="G40" s="28"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>107</v>
       </c>
@@ -3138,7 +3147,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -3158,7 +3167,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -3178,7 +3187,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>113</v>
       </c>
@@ -3198,7 +3207,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>116</v>
       </c>
@@ -3221,7 +3230,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>119</v>
       </c>
@@ -3244,7 +3253,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>120</v>
       </c>
@@ -3267,7 +3276,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>124</v>
       </c>
@@ -3290,7 +3299,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>140</v>
       </c>
@@ -3313,7 +3322,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>141</v>
       </c>
@@ -3333,7 +3342,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -3353,7 +3362,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>147</v>
       </c>
@@ -3379,7 +3388,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>147</v>
       </c>
@@ -3405,7 +3414,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>147</v>
       </c>
@@ -3431,7 +3440,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>152</v>
       </c>
@@ -3454,7 +3463,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>159</v>
       </c>
@@ -3477,7 +3486,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>161</v>
       </c>
@@ -3500,7 +3509,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>162</v>
       </c>
@@ -3520,7 +3529,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>167</v>
       </c>
@@ -3540,7 +3549,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>169</v>
       </c>
@@ -3563,7 +3572,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>174</v>
       </c>
@@ -3586,7 +3595,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>177</v>
       </c>
@@ -3609,7 +3618,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B1 B3:B1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3637,47 +3646,47 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>211</v>
       </c>
@@ -3698,17 +3707,17 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>271</v>
       </c>
@@ -3716,7 +3725,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -3736,7 +3745,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>209</v>
       </c>
@@ -3756,7 +3765,7 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>210</v>
       </c>
@@ -3786,21 +3795,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B902128-77A3-4FC4-8358-70CDD0AB45F8}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
     <col min="4" max="5" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>198</v>
       </c>
@@ -3817,7 +3826,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
@@ -3831,7 +3840,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
@@ -3845,7 +3854,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>183</v>
       </c>
@@ -3859,7 +3868,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
@@ -3873,7 +3882,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>245</v>
       </c>
@@ -3887,7 +3896,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>246</v>
       </c>
@@ -3901,7 +3910,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>247</v>
       </c>
@@ -3915,7 +3924,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>256</v>
       </c>
@@ -3929,7 +3938,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>257</v>
       </c>
@@ -3943,7 +3952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>258</v>
       </c>
@@ -3957,7 +3966,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>259</v>
       </c>
@@ -3972,7 +3981,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>152</v>
       </c>
@@ -3989,7 +3998,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>174</v>
       </c>
@@ -4006,7 +4015,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
         <v>265</v>
       </c>
@@ -4023,7 +4032,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>278</v>
       </c>
@@ -4040,7 +4049,7 @@
         <v>1.077</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>279</v>
       </c>
@@ -4057,9 +4066,26 @@
         <v>90</v>
       </c>
     </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>283</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>284</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>281</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B17">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  <conditionalFormatting sqref="B2:B18">
+    <cfRule type="duplicateValues" dxfId="35" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4077,15 +4103,15 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.44140625" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>198</v>
       </c>
@@ -4108,7 +4134,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>251</v>
       </c>
@@ -4129,7 +4155,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>252</v>
       </c>
@@ -4146,7 +4172,7 @@
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>59</v>
       </c>
@@ -4167,7 +4193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>62</v>
       </c>
@@ -4188,7 +4214,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>165</v>
       </c>
@@ -4211,7 +4237,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4224,28 +4250,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7027210-EB2D-4810-B641-E47C920F8A87}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" customWidth="1"/>
+    <col min="1" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C1" s="27" t="s">
         <v>253</v>
       </c>
@@ -4283,7 +4309,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>205</v>
       </c>
@@ -4327,7 +4353,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>212</v>
       </c>
@@ -4371,7 +4397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>212</v>
       </c>
@@ -4415,7 +4441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>212</v>
       </c>
@@ -4459,7 +4485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>212</v>
       </c>
@@ -4503,7 +4529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>212</v>
       </c>
@@ -4547,7 +4573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>212</v>
       </c>
@@ -4591,7 +4617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>212</v>
       </c>
@@ -4652,20 +4678,20 @@
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>250</v>
       </c>
@@ -4700,7 +4726,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="23">
         <v>1</v>
       </c>
@@ -4735,7 +4761,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="23">
         <v>2</v>
       </c>
@@ -4770,7 +4796,7 @@
         <v>4.8499999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="23">
         <v>3</v>
       </c>
@@ -4805,7 +4831,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="23">
         <v>4</v>
       </c>
@@ -4840,7 +4866,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="23">
         <v>5</v>
       </c>
@@ -4875,7 +4901,7 @@
         <v>4.7699999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="23">
         <v>6</v>
       </c>
@@ -4910,7 +4936,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23">
         <v>7</v>
       </c>
@@ -4945,7 +4971,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="23">
         <v>8</v>
       </c>
@@ -4980,7 +5006,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="23">
         <v>9</v>
       </c>
@@ -5015,7 +5041,7 @@
         <v>2.74</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="23">
         <v>10</v>
       </c>
@@ -5050,7 +5076,7 @@
         <v>4.79</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="23">
         <v>11</v>
       </c>
@@ -5085,7 +5111,7 @@
         <v>6.61</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="23">
         <v>12</v>
       </c>
@@ -5120,7 +5146,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="23">
         <v>13</v>
       </c>
@@ -5155,7 +5181,7 @@
         <v>4.8899999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="23">
         <v>14</v>
       </c>
@@ -5190,7 +5216,7 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="23">
         <v>15</v>
       </c>
@@ -5225,7 +5251,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="23">
         <v>16</v>
       </c>
@@ -5260,7 +5286,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="23">
         <v>17</v>
       </c>
@@ -5295,7 +5321,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="23">
         <v>18</v>
       </c>
@@ -5330,7 +5356,7 @@
         <v>4.91</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="23">
         <v>19</v>
       </c>
@@ -5365,7 +5391,7 @@
         <v>6.88</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="23">
         <v>20</v>
       </c>
@@ -5400,7 +5426,7 @@
         <v>6.52</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="23">
         <v>21</v>
       </c>
@@ -5435,7 +5461,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="23">
         <v>22</v>
       </c>
@@ -5470,7 +5496,7 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="23">
         <v>23</v>
       </c>
@@ -5505,7 +5531,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="23">
         <v>24</v>
       </c>
@@ -5540,7 +5566,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="23">
         <v>25</v>
       </c>
@@ -5575,7 +5601,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="23">
         <v>26</v>
       </c>
@@ -5610,7 +5636,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="23">
         <v>27</v>
       </c>
@@ -5645,7 +5671,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="23">
         <v>28</v>
       </c>
@@ -5680,7 +5706,7 @@
         <v>6.87</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="23">
         <v>29</v>
       </c>
@@ -5715,7 +5741,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="23">
         <v>30</v>
       </c>
@@ -5750,7 +5776,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="23">
         <v>31</v>
       </c>
@@ -5785,7 +5811,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="23">
         <v>32</v>
       </c>
@@ -5820,7 +5846,7 @@
         <v>2.76</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="23">
         <v>33</v>
       </c>
@@ -5855,7 +5881,7 @@
         <v>2.77</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="23">
         <v>34</v>
       </c>
@@ -5890,7 +5916,7 @@
         <v>5.77</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="23">
         <v>35</v>
       </c>
@@ -5925,7 +5951,7 @@
         <v>7.46</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="23">
         <v>36</v>
       </c>
@@ -5960,7 +5986,7 @@
         <v>7.11</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="23">
         <v>37</v>
       </c>
@@ -5995,7 +6021,7 @@
         <v>4.97</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="23">
         <v>38</v>
       </c>
@@ -6030,7 +6056,7 @@
         <v>4.08</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="23">
         <v>39</v>
       </c>
@@ -6065,7 +6091,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="23">
         <v>40</v>
       </c>
@@ -6100,7 +6126,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="23">
         <v>41</v>
       </c>
@@ -6135,7 +6161,7 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="23">
         <v>42</v>
       </c>
@@ -6170,7 +6196,7 @@
         <v>5.97</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="23">
         <v>43</v>
       </c>
@@ -6205,7 +6231,7 @@
         <v>7.56</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="23">
         <v>44</v>
       </c>
@@ -6240,7 +6266,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="23">
         <v>45</v>
       </c>
@@ -6275,7 +6301,7 @@
         <v>5.07</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="23">
         <v>46</v>
       </c>
@@ -6310,7 +6336,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="23">
         <v>47</v>
       </c>
@@ -6345,7 +6371,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="23">
         <v>48</v>
       </c>
@@ -6380,7 +6406,7 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="23">
         <v>49</v>
       </c>
@@ -6415,7 +6441,7 @@
         <v>3.37</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="23">
         <v>50</v>
       </c>
@@ -6450,7 +6476,7 @@
         <v>6.43</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="23">
         <v>51</v>
       </c>
@@ -6485,7 +6511,7 @@
         <v>7.83</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="23">
         <v>52</v>
       </c>
@@ -6520,7 +6546,7 @@
         <v>7.59</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="23">
         <v>53</v>
       </c>
@@ -6555,7 +6581,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="23">
         <v>54</v>
       </c>
@@ -6590,7 +6616,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="23">
         <v>55</v>
       </c>
@@ -6625,7 +6651,7 @@
         <v>4.22</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="23">
         <v>56</v>
       </c>
@@ -6660,7 +6686,7 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="23">
         <v>57</v>
       </c>
@@ -6695,7 +6721,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="23">
         <v>58</v>
       </c>
@@ -6730,7 +6756,7 @@
         <v>8.94</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="23">
         <v>59</v>
       </c>
@@ -6765,7 +6791,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="23">
         <v>60</v>
       </c>
@@ -6800,7 +6826,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="23">
         <v>61</v>
       </c>
@@ -6835,7 +6861,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="23">
         <v>62</v>
       </c>
@@ -6870,7 +6896,7 @@
         <v>6.71</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="23">
         <v>63</v>
       </c>
@@ -6905,7 +6931,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="23">
         <v>64</v>
       </c>
@@ -6940,7 +6966,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="23">
         <v>65</v>
       </c>
@@ -6975,7 +7001,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="23">
         <v>66</v>
       </c>
@@ -7010,7 +7036,7 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="23">
         <v>67</v>
       </c>
@@ -7045,7 +7071,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="23">
         <v>68</v>
       </c>
@@ -7080,7 +7106,7 @@
         <v>10.59</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="23">
         <v>69</v>
       </c>
@@ -7115,7 +7141,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="23">
         <v>70</v>
       </c>
@@ -7150,7 +7176,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="23">
         <v>71</v>
       </c>
@@ -7185,7 +7211,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="23">
         <v>72</v>
       </c>
@@ -7220,7 +7246,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="23">
         <v>73</v>
       </c>
@@ -7255,7 +7281,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="23">
         <v>74</v>
       </c>
@@ -7290,7 +7316,7 @@
         <v>9.2100000000000009</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="23">
         <v>75</v>
       </c>
@@ -7328,7 +7354,7 @@
       <c r="M77" s="7"/>
       <c r="N77" s="7"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="23">
         <v>76</v>
       </c>
@@ -7366,7 +7392,7 @@
       <c r="M78" s="7"/>
       <c r="N78" s="7"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="23">
         <v>77</v>
       </c>
@@ -7404,7 +7430,7 @@
       <c r="M79" s="7"/>
       <c r="N79" s="7"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="23">
         <v>78</v>
       </c>
@@ -7442,7 +7468,7 @@
       <c r="M80" s="7"/>
       <c r="N80" s="7"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="23">
         <v>79</v>
       </c>
@@ -7480,7 +7506,7 @@
       <c r="M81" s="7"/>
       <c r="N81" s="7"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="23">
         <v>80</v>
       </c>
@@ -7518,7 +7544,7 @@
       <c r="M82" s="7"/>
       <c r="N82" s="7"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="23">
         <v>81</v>
       </c>
@@ -7556,7 +7582,7 @@
       <c r="M83" s="7"/>
       <c r="N83" s="7"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="23">
         <v>82</v>
       </c>
@@ -7594,7 +7620,7 @@
       <c r="M84" s="7"/>
       <c r="N84" s="7"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="23">
         <v>83</v>
       </c>
@@ -7632,7 +7658,7 @@
       <c r="M85" s="7"/>
       <c r="N85" s="7"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="23">
         <v>84</v>
       </c>
@@ -7670,7 +7696,7 @@
       <c r="M86" s="7"/>
       <c r="N86" s="7"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="23">
         <v>85</v>
       </c>
@@ -7708,7 +7734,7 @@
       <c r="M87" s="7"/>
       <c r="N87" s="7"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="23">
         <v>86</v>
       </c>
@@ -7746,7 +7772,7 @@
       <c r="M88" s="7"/>
       <c r="N88" s="7"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="23">
         <v>87</v>
       </c>
@@ -7784,7 +7810,7 @@
       <c r="M89" s="7"/>
       <c r="N89" s="7"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="23">
         <v>88</v>
       </c>
@@ -7819,7 +7845,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="23">
         <v>89</v>
       </c>
@@ -7854,7 +7880,7 @@
         <v>5.61</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="23">
         <v>90</v>
       </c>
@@ -7889,7 +7915,7 @@
         <v>9.56</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="23">
         <v>91</v>
       </c>
@@ -7924,7 +7950,7 @@
         <v>10.29</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="23">
         <v>92</v>
       </c>
@@ -7959,7 +7985,7 @@
         <v>10.81</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="23">
         <v>93</v>
       </c>
@@ -7994,7 +8020,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="23">
         <v>94</v>
       </c>
@@ -8029,7 +8055,7 @@
         <v>7.44</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="23">
         <v>95</v>
       </c>
@@ -8064,7 +8090,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="23">
         <v>96</v>
       </c>
@@ -8099,7 +8125,7 @@
         <v>2.23</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="23">
         <v>97</v>
       </c>
@@ -8134,7 +8160,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="23">
         <v>98</v>
       </c>
@@ -8169,7 +8195,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="23">
         <v>99</v>
       </c>
@@ -8204,7 +8230,7 @@
         <v>10.32</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="23">
         <v>100</v>
       </c>
@@ -8239,7 +8265,7 @@
         <v>10.84</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="23">
         <v>101</v>
       </c>
@@ -8274,7 +8300,7 @@
         <v>8.51</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="23">
         <v>102</v>
       </c>
@@ -8309,7 +8335,7 @@
         <v>7.57</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="23">
         <v>103</v>
       </c>
@@ -8344,7 +8370,7 @@
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="23">
         <v>104</v>
       </c>
@@ -8379,7 +8405,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="23">
         <v>105</v>
       </c>
@@ -8414,7 +8440,7 @@
         <v>6.23</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="23">
         <v>106</v>
       </c>
@@ -8449,7 +8475,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="23">
         <v>107</v>
       </c>
@@ -8484,7 +8510,7 @@
         <v>10.43</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="23">
         <v>108</v>
       </c>
@@ -8519,7 +8545,7 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="23">
         <v>109</v>
       </c>
@@ -8554,7 +8580,7 @@
         <v>8.7200000000000006</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="23">
         <v>110</v>
       </c>
@@ -8589,7 +8615,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="23">
         <v>111</v>
       </c>
@@ -8624,7 +8650,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="23">
         <v>112</v>
       </c>
@@ -8659,7 +8685,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="23">
         <v>113</v>
       </c>
@@ -8694,7 +8720,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="23">
         <v>114</v>
       </c>
@@ -8729,7 +8755,7 @@
         <v>8.94</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="23">
         <v>115</v>
       </c>
@@ -8764,7 +8790,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="23">
         <v>116</v>
       </c>
@@ -8799,7 +8825,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="23">
         <v>117</v>
       </c>
@@ -8834,7 +8860,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="23">
         <v>118</v>
       </c>
@@ -8869,7 +8895,7 @@
         <v>6.71</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="23">
         <v>119</v>
       </c>
@@ -8904,7 +8930,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="23">
         <v>120</v>
       </c>
@@ -8939,7 +8965,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="23">
         <v>121</v>
       </c>
@@ -8974,7 +9000,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="23">
         <v>122</v>
       </c>
@@ -9009,7 +9035,7 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="23">
         <v>123</v>
       </c>
@@ -9044,7 +9070,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="23">
         <v>124</v>
       </c>
@@ -9079,7 +9105,7 @@
         <v>10.59</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="23">
         <v>125</v>
       </c>
@@ -9114,7 +9140,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="23">
         <v>126</v>
       </c>
@@ -9149,7 +9175,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="23">
         <v>127</v>
       </c>
@@ -9184,7 +9210,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="23">
         <v>128</v>
       </c>
@@ -9219,7 +9245,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="23">
         <v>129</v>
       </c>
@@ -9254,7 +9280,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="23">
         <v>130</v>
       </c>
@@ -9289,7 +9315,7 @@
         <v>9.2100000000000009</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="23">
         <v>131</v>
       </c>
@@ -9324,7 +9350,7 @@
         <v>10.11</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="23">
         <v>132</v>
       </c>
@@ -9359,7 +9385,7 @@
         <v>10.67</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="23">
         <v>133</v>
       </c>
@@ -9394,7 +9420,7 @@
         <v>8.11</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="23">
         <v>134</v>
       </c>
@@ -9429,7 +9455,7 @@
         <v>7.09</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="23">
         <v>135</v>
       </c>
@@ -9464,7 +9490,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="23">
         <v>136</v>
       </c>
@@ -9499,7 +9525,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="23">
         <v>137</v>
       </c>
@@ -9534,7 +9560,7 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="23">
         <v>138</v>
       </c>
@@ -9569,7 +9595,7 @@
         <v>9.4499999999999993</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="23">
         <v>139</v>
       </c>
@@ -9604,7 +9630,7 @@
         <v>10.23</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="23">
         <v>140</v>
       </c>
@@ -9639,7 +9665,7 @@
         <v>10.76</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="23">
         <v>141</v>
       </c>
@@ -9674,7 +9700,7 @@
         <v>8.31</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="23">
         <v>142</v>
       </c>
@@ -9709,7 +9735,7 @@
         <v>7.26</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="23">
         <v>143</v>
       </c>
@@ -9744,7 +9770,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="23">
         <v>144</v>
       </c>
@@ -9779,7 +9805,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="23">
         <v>145</v>
       </c>
@@ -9814,7 +9840,7 @@
         <v>5.61</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="23">
         <v>146</v>
       </c>
@@ -9849,7 +9875,7 @@
         <v>9.56</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="23">
         <v>147</v>
       </c>
@@ -9884,7 +9910,7 @@
         <v>10.29</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="23">
         <v>148</v>
       </c>
@@ -9919,7 +9945,7 @@
         <v>10.81</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="23">
         <v>149</v>
       </c>
@@ -9954,7 +9980,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="23">
         <v>150</v>
       </c>
@@ -9989,7 +10015,7 @@
         <v>7.44</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="23">
         <v>151</v>
       </c>
@@ -10024,7 +10050,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="23">
         <v>152</v>
       </c>
@@ -10059,7 +10085,7 @@
         <v>2.23</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="23">
         <v>153</v>
       </c>
@@ -10094,7 +10120,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="23">
         <v>154</v>
       </c>
@@ -10129,7 +10155,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="23">
         <v>155</v>
       </c>
@@ -10164,7 +10190,7 @@
         <v>10.32</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="23">
         <v>156</v>
       </c>
@@ -10199,7 +10225,7 @@
         <v>10.84</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="23">
         <v>157</v>
       </c>
@@ -10234,7 +10260,7 @@
         <v>8.51</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="23">
         <v>158</v>
       </c>
@@ -10269,7 +10295,7 @@
         <v>7.57</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="23">
         <v>159</v>
       </c>
@@ -10304,7 +10330,7 @@
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="23">
         <v>160</v>
       </c>
@@ -10339,7 +10365,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="23">
         <v>161</v>
       </c>
@@ -10374,7 +10400,7 @@
         <v>6.23</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="23">
         <v>162</v>
       </c>
@@ -10409,7 +10435,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="23">
         <v>163</v>
       </c>
@@ -10444,7 +10470,7 @@
         <v>10.43</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="23">
         <v>164</v>
       </c>
@@ -10479,7 +10505,7 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="23">
         <v>165</v>
       </c>
@@ -10514,7 +10540,7 @@
         <v>8.7200000000000006</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="23">
         <v>166</v>
       </c>
@@ -10549,7 +10575,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="23">
         <v>167</v>
       </c>
@@ -10584,7 +10610,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="23">
         <v>168</v>
       </c>
@@ -10621,7 +10647,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10632,12 +10658,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10870,15 +10893,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A202D3EF-E74A-4B50-BD9D-588EBDA690CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="13eb6276-85db-4ef3-a671-167ab07ac255"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fc9abb88-5dc8-4425-a823-e2986ac3f199"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10903,18 +10938,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A202D3EF-E74A-4B50-BD9D-588EBDA690CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="13eb6276-85db-4ef3-a671-167ab07ac255"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fc9abb88-5dc8-4425-a823-e2986ac3f199"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added validation of overtopping, armour stability and rear side armour stability
</commit_message>
<xml_diff>
--- a/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
+++ b/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JY6\github\breakwater\Notebooks\Constanta Phase III\Input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFEAA79C-A6EA-48B8-98B0-0CBB1E86BAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD1D6321-167E-4B47-B495-15ED9B8147B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="709" firstSheet="1" activeTab="7" xr2:uid="{06ED436A-2CC0-4489-A506-29F94518B839}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="709" firstSheet="1" activeTab="8" xr2:uid="{06ED436A-2CC0-4489-A506-29F94518B839}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Input_Cross section" sheetId="8" r:id="rId6"/>
     <sheet name="input_hydrotechnical" sheetId="5" r:id="rId7"/>
     <sheet name="input_rock_gradings" sheetId="10" r:id="rId8"/>
+    <sheet name="input_cross_section_validation" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="Lt">'Input_Project specific'!$E$20</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="384">
   <si>
     <t>Input</t>
   </si>
@@ -1098,9 +1099,6 @@
     <t>130</t>
   </si>
   <si>
-    <t>0.3-1 ton</t>
-  </si>
-  <si>
     <t>540</t>
   </si>
   <si>
@@ -1264,6 +1262,51 @@
   </si>
   <si>
     <t>Based on Phase II, underlayer to sea bed</t>
+  </si>
+  <si>
+    <t>Armour_class</t>
+  </si>
+  <si>
+    <t>Armour grading</t>
+  </si>
+  <si>
+    <t>Crest height</t>
+  </si>
+  <si>
+    <t>Concrete</t>
+  </si>
+  <si>
+    <t>Rock</t>
+  </si>
+  <si>
+    <t>Unit_volume</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>rear_armour_class</t>
+  </si>
+  <si>
+    <t>toe_armour_class</t>
+  </si>
+  <si>
+    <t>access_type</t>
+  </si>
+  <si>
+    <t>restricted</t>
+  </si>
+  <si>
+    <t>300-1000 kg</t>
+  </si>
+  <si>
+    <t>Underlayer concrete units</t>
+  </si>
+  <si>
+    <t>c_underlayer</t>
+  </si>
+  <si>
+    <t>Armour_type</t>
   </si>
 </sst>
 </file>
@@ -1601,46 +1644,6 @@
   </cellStyles>
   <dxfs count="48">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -1746,6 +1749,16 @@
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1955,6 +1968,16 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2099,6 +2122,16 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -2180,6 +2213,16 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2194,7 +2237,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{128A59F9-895D-4C60-8954-4F77FF691FFB}" name="Overview" displayName="Overview" ref="A2:G62" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{128A59F9-895D-4C60-8954-4F77FF691FFB}" name="Overview" displayName="Overview" ref="A2:G62" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44">
   <autoFilter ref="A2:G62" xr:uid="{C615D3FE-C5C3-4AC1-8573-2115046F6FC7}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{FDED3D30-FC03-4894-AAAE-7069E3558798}" name="Input"/>
@@ -2202,8 +2245,26 @@
     <tableColumn id="3" xr3:uid="{122DBA8D-3347-48F4-8A76-270615744B5D}" name="Unit"/>
     <tableColumn id="4" xr3:uid="{B4BA3D29-867B-4EF8-A808-EE6581BB8115}" name="Category"/>
     <tableColumn id="5" xr3:uid="{CB74FB27-39F6-4359-BAC6-C5DFAC8E01C0}" name="Used for"/>
-    <tableColumn id="6" xr3:uid="{266927E0-00C5-4D6A-BB41-21164D34B2CE}" name="Necessary input" dataDxfId="44"/>
-    <tableColumn id="7" xr3:uid="{30AC8882-C2A6-43C1-86B7-25C9ED481C62}" name="Remarks" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{266927E0-00C5-4D6A-BB41-21164D34B2CE}" name="Necessary input" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{30AC8882-C2A6-43C1-86B7-25C9ED481C62}" name="Remarks" dataDxfId="42"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{F3910581-BF80-43BD-BC4E-E63C5EA06E87}" name="Table10" displayName="Table10" ref="A2:I9" totalsRowShown="0">
+  <autoFilter ref="A2:I9" xr:uid="{F3910581-BF80-43BD-BC4E-E63C5EA06E87}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{F23F178C-7758-4DAE-80A2-5DE494BECEC6}" name="Structure"/>
+    <tableColumn id="2" xr3:uid="{F1B52775-943A-47C9-818E-44C8CEDAB9EA}" name="Chainage"/>
+    <tableColumn id="10" xr3:uid="{EEEED623-18C7-41E9-ADA5-7120BA5F693C}" name="access_type"/>
+    <tableColumn id="6" xr3:uid="{82DECA7D-96F5-4F14-BD62-3B902EC9B6E6}" name="z_crest"/>
+    <tableColumn id="3" xr3:uid="{EF4761C1-3047-4246-B73D-E95BD77B923A}" name="Armour_type"/>
+    <tableColumn id="4" xr3:uid="{D5E84631-6F04-40E5-A257-6B0867875D8E}" name="Armour_class"/>
+    <tableColumn id="5" xr3:uid="{E811378E-84D4-42C7-A78F-4D6C5F6A9648}" name="Unit_volume"/>
+    <tableColumn id="7" xr3:uid="{10E7DC6E-2831-41C8-8AAA-AE8315234826}" name="rear_armour_class"/>
+    <tableColumn id="8" xr3:uid="{C035176E-2F9A-4343-9611-95E8A88A393E}" name="toe_armour_class"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2245,58 +2306,58 @@
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{32645932-B206-41E7-B1E9-2A52D9AE0D60}" name="Limit State"/>
     <tableColumn id="1" xr3:uid="{B6826C86-D95D-4464-8196-B4E1CEBC5F0A}" name="Nod"/>
-    <tableColumn id="2" xr3:uid="{12FE237E-CE70-4E63-BE4C-9D0365BAB8AC}" name="Accropode II-trunk" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{3045C02B-DCDC-42A1-B50F-88D0E610E62A}" name="Accropode II-roundhead" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{0280B610-A0B2-48C8-AB40-3AE6F87EDE4A}" name="Xbloc-trunk" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{C26BCBB6-089E-47C5-9394-EA17687F6843}" name="Xbloc-roundhead" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{12FE237E-CE70-4E63-BE4C-9D0365BAB8AC}" name="Accropode II-trunk" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{3045C02B-DCDC-42A1-B50F-88D0E610E62A}" name="Accropode II-roundhead" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{0280B610-A0B2-48C8-AB40-3AE6F87EDE4A}" name="Xbloc-trunk" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{C26BCBB6-089E-47C5-9394-EA17687F6843}" name="Xbloc-roundhead" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{88915663-9067-4DC4-90A4-2D7CD517273B}" name="input_project" displayName="input_project" ref="A1:E28" totalsRowShown="0" dataDxfId="38">
-  <autoFilter ref="A1:E28" xr:uid="{8653FB80-28B1-42DD-ADDB-1F402573EE6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{88915663-9067-4DC4-90A4-2D7CD517273B}" name="input_project" displayName="input_project" ref="A1:E29" totalsRowShown="0" dataDxfId="36">
+  <autoFilter ref="A1:E29" xr:uid="{8653FB80-28B1-42DD-ADDB-1F402573EE6E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{10575A1B-65C2-4D3D-A919-D5D631E15E73}" name="Parameter" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{9F5575C0-7208-43BD-86BC-6A3485FF384C}" name="Symbol" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{1CF28AEF-1CBA-48D2-A66A-EE6DC73C8CC9}" name="Unit " dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{FB5987BB-56D7-412F-8C95-1F5820C3E77A}" name="Explanation" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{5ABE4DA7-DB09-46BC-AF34-3D5B699627F3}" name="Value" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{10575A1B-65C2-4D3D-A919-D5D631E15E73}" name="Parameter" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{9F5575C0-7208-43BD-86BC-6A3485FF384C}" name="Symbol" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{1CF28AEF-1CBA-48D2-A66A-EE6DC73C8CC9}" name="Unit " dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{FB5987BB-56D7-412F-8C95-1F5820C3E77A}" name="Explanation" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{5ABE4DA7-DB09-46BC-AF34-3D5B699627F3}" name="Value" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6634BB44-66AA-43C5-94C9-21ADB80AD51A}" name="input_requirements" displayName="input_requirements" ref="A1:G6" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6634BB44-66AA-43C5-94C9-21ADB80AD51A}" name="input_requirements" displayName="input_requirements" ref="A1:G6" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="A1:G6" xr:uid="{AC8FC8D0-6474-4C46-AABC-7775C18E706C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{ED5624B9-4A0A-4F41-BA44-D0E02EE32577}" name="Parameter" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{2B068622-98F3-4E2A-BE8E-A97C121E3F4C}" name="Symbol" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{4BC1E5B1-1862-4E8F-8CC1-D2F05F356929}" name="Unit " dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{F431E098-CB44-4ACA-97A5-C64500DD9528}" name="Explanation" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{C6914755-DB47-4220-827C-0984890970A0}" name="ELS" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{D3A99EAE-B2C9-4E74-B3E2-A288F4532A21}" name="SLS" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{9350B3BA-690A-42F3-BB94-29E26F161B54}" name="ULS" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{ED5624B9-4A0A-4F41-BA44-D0E02EE32577}" name="Parameter" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{2B068622-98F3-4E2A-BE8E-A97C121E3F4C}" name="Symbol" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{4BC1E5B1-1862-4E8F-8CC1-D2F05F356929}" name="Unit " dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{F431E098-CB44-4ACA-97A5-C64500DD9528}" name="Explanation" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{C6914755-DB47-4220-827C-0984890970A0}" name="ELS" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{D3A99EAE-B2C9-4E74-B3E2-A288F4532A21}" name="SLS" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{9350B3BA-690A-42F3-BB94-29E26F161B54}" name="ULS" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5DFFFB11-DDA0-4FF0-A99C-C5B40B22BB0F}" name="input_cross_section" displayName="input_cross_section" ref="A2:N9" totalsRowShown="0" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5DFFFB11-DDA0-4FF0-A99C-C5B40B22BB0F}" name="input_cross_section" displayName="input_cross_section" ref="A2:N9" totalsRowShown="0" tableBorderDxfId="19">
   <autoFilter ref="A2:N9" xr:uid="{EDBA852A-A4D9-4055-8891-B74537BE60D1}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{65F89A4D-13BC-480A-9A54-9B5181E61222}" name="Structure" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{DD7D1624-C590-49ED-8883-96E10DDFDC57}" name="Chainage" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{56CAAB95-7C5D-4C77-9690-8C7E28E5E58F}" name="dir_structure" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{65F89A4D-13BC-480A-9A54-9B5181E61222}" name="Structure" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{DD7D1624-C590-49ED-8883-96E10DDFDC57}" name="Chainage" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{56CAAB95-7C5D-4C77-9690-8C7E28E5E58F}" name="dir_structure" dataDxfId="16"/>
     <tableColumn id="4" xr3:uid="{3211485F-4253-4196-9552-5388E1C18679}" name="z_bed"/>
     <tableColumn id="5" xr3:uid="{12FF2071-DB6F-4635-AAF2-7224DB03F7AF}" name="public"/>
     <tableColumn id="6" xr3:uid="{3C50E8D0-D9A3-4D42-9184-21A91AB97D26}" name="P"/>
-    <tableColumn id="7" xr3:uid="{67557D02-D417-4935-83D4-56C7A3EC4E57}" name="tan_a" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{67557D02-D417-4935-83D4-56C7A3EC4E57}" name="tan_a" dataDxfId="15"/>
     <tableColumn id="9" xr3:uid="{0A204ACD-A807-4615-BEB7-8F6AA353A3CD}" name="Gc"/>
-    <tableColumn id="10" xr3:uid="{0003E8D8-CC23-4555-A626-BC13BBABE9B8}" name="slope_foreshore" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{0003E8D8-CC23-4555-A626-BC13BBABE9B8}" name="slope_foreshore" dataDxfId="14"/>
     <tableColumn id="12" xr3:uid="{74307101-79D4-4197-A798-20BAE3C12767}" name="crest_roughness"/>
     <tableColumn id="13" xr3:uid="{30E9BE3D-820F-4565-AD86-93CC1E7A860F}" name="cot_a_rear"/>
     <tableColumn id="14" xr3:uid="{A3804960-2456-4577-852A-50CF47F120BD}" name="B"/>
@@ -2308,20 +2369,20 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A63CE4AC-CF5D-406B-B465-B4984FB45555}" name="input_hydrometeo" displayName="input_hydrometeo" ref="A2:K170" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A63CE4AC-CF5D-406B-B465-B4984FB45555}" name="input_hydrometeo" displayName="input_hydrometeo" ref="A2:K170" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A2:K170" xr:uid="{8EC5B0C1-E4CA-4C7B-AA39-695D226630E3}"/>
   <tableColumns count="11">
-    <tableColumn id="6" xr3:uid="{F9A5357A-5DE4-4408-A14A-E6698FD3755F}" name="Calculation_case" dataDxfId="14"/>
-    <tableColumn id="1" xr3:uid="{012C1F4F-AAC2-4FD0-A162-E004B1A207F9}" name="Structure" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{BE45E132-052E-4051-A5CC-2691B8D1D576}" name="Chainage" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{CE4FADC8-9574-4B7C-9E02-F0716073BF79}" name="Offshore bin" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{C0A99159-F33E-4796-BC72-CB4DE68B9FDE}" name="Limit State" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{240593D5-435F-4039-BD0D-5B8B3FDD3128}" name="wl" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{1A72D5A3-EEEE-48D4-B8C7-0BC7A1474131}" name="Hm0" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{937FF273-2A9A-4DA7-AC8F-B2F74F1681D7}" name="dir_wave" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{24ED7C68-4403-4BB0-A849-0C22B2AF55BB}" name="Tp" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{A397DA8E-DE81-4096-A083-356358DACD29}" name="Tm-1,0" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{17652E84-F087-4BBA-B4B9-CD36B5153566}" name="Tm0,2" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{F9A5357A-5DE4-4408-A14A-E6698FD3755F}" name="Calculation_case" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{012C1F4F-AAC2-4FD0-A162-E004B1A207F9}" name="Structure" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{BE45E132-052E-4051-A5CC-2691B8D1D576}" name="Chainage" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{CE4FADC8-9574-4B7C-9E02-F0716073BF79}" name="Offshore bin" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{C0A99159-F33E-4796-BC72-CB4DE68B9FDE}" name="Limit State" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{240593D5-435F-4039-BD0D-5B8B3FDD3128}" name="wl" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{1A72D5A3-EEEE-48D4-B8C7-0BC7A1474131}" name="Hm0" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{937FF273-2A9A-4DA7-AC8F-B2F74F1681D7}" name="dir_wave" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{24ED7C68-4403-4BB0-A849-0C22B2AF55BB}" name="Tp" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{A397DA8E-DE81-4096-A083-356358DACD29}" name="Tm-1,0" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{17652E84-F087-4BBA-B4B9-CD36B5153566}" name="Tm0,2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2630,25 +2691,25 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="30.5546875" customWidth="1"/>
-    <col min="6" max="6" width="46.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="60.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="61.5546875" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+    <col min="6" max="6" width="46.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="60.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="61.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B1" s="5"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -2671,7 +2732,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2691,7 +2752,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2711,7 +2772,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>183</v>
       </c>
@@ -2731,7 +2792,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2748,7 +2809,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2771,7 +2832,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2791,7 +2852,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2814,7 +2875,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2834,7 +2895,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -2857,7 +2918,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -2877,7 +2938,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -2900,7 +2961,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -2923,7 +2984,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2946,7 +3007,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -2969,7 +3030,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -2989,7 +3050,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -3012,7 +3073,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -3035,7 +3096,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -3058,7 +3119,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>165</v>
       </c>
@@ -3081,7 +3142,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -3104,7 +3165,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>142</v>
       </c>
@@ -3127,7 +3188,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>143</v>
       </c>
@@ -3147,7 +3208,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -3170,7 +3231,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>65</v>
       </c>
@@ -3188,7 +3249,7 @@
       </c>
       <c r="G26" s="22"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -3208,7 +3269,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -3231,7 +3292,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -3255,7 +3316,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -3278,7 +3339,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -3298,7 +3359,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -3318,7 +3379,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -3341,7 +3402,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -3361,7 +3422,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>238</v>
       </c>
@@ -3381,7 +3442,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -3401,7 +3462,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -3421,7 +3482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -3447,7 +3508,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>228</v>
       </c>
@@ -3467,7 +3528,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>230</v>
       </c>
@@ -3488,7 +3549,7 @@
       </c>
       <c r="G40" s="22"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>107</v>
       </c>
@@ -3508,7 +3569,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -3528,7 +3589,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -3548,7 +3609,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>113</v>
       </c>
@@ -3568,7 +3629,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>116</v>
       </c>
@@ -3591,7 +3652,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>119</v>
       </c>
@@ -3614,7 +3675,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>120</v>
       </c>
@@ -3637,7 +3698,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>124</v>
       </c>
@@ -3660,7 +3721,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>140</v>
       </c>
@@ -3683,7 +3744,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>141</v>
       </c>
@@ -3703,7 +3764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -3723,7 +3784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>147</v>
       </c>
@@ -3749,7 +3810,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>147</v>
       </c>
@@ -3775,7 +3836,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>147</v>
       </c>
@@ -3801,7 +3862,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>152</v>
       </c>
@@ -3824,7 +3885,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>159</v>
       </c>
@@ -3847,7 +3908,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>161</v>
       </c>
@@ -3870,7 +3931,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>162</v>
       </c>
@@ -3890,7 +3951,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>167</v>
       </c>
@@ -3910,7 +3971,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>169</v>
       </c>
@@ -3933,7 +3994,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>174</v>
       </c>
@@ -3956,7 +4017,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>177</v>
       </c>
@@ -3979,7 +4040,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B1 B3:B1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4009,79 +4070,79 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>348</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -4102,17 +4163,17 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>270</v>
       </c>
@@ -4120,7 +4181,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -4140,7 +4201,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>209</v>
       </c>
@@ -4160,7 +4221,7 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>210</v>
       </c>
@@ -4190,22 +4251,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B902128-77A3-4FC4-8358-70CDD0AB45F8}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" customWidth="1"/>
-    <col min="4" max="4" width="53.6640625" customWidth="1"/>
+    <col min="1" max="1" width="46.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="4" max="4" width="53.7109375" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>198</v>
       </c>
@@ -4222,7 +4283,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>6</v>
       </c>
@@ -4237,7 +4298,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>10</v>
       </c>
@@ -4252,7 +4313,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>183</v>
       </c>
@@ -4267,7 +4328,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>13</v>
       </c>
@@ -4282,7 +4343,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>245</v>
       </c>
@@ -4297,7 +4358,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
         <v>246</v>
       </c>
@@ -4312,7 +4373,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
         <v>247</v>
       </c>
@@ -4327,7 +4388,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>255</v>
       </c>
@@ -4342,7 +4403,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>256</v>
       </c>
@@ -4357,7 +4418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
         <v>257</v>
       </c>
@@ -4372,7 +4433,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
         <v>258</v>
       </c>
@@ -4387,7 +4448,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
         <v>152</v>
       </c>
@@ -4404,24 +4465,24 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="47" t="s">
+        <v>338</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>339</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>340</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E14" s="23">
         <v>0.7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
         <v>264</v>
       </c>
@@ -4438,7 +4499,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="53" t="s">
         <v>277</v>
       </c>
@@ -4455,7 +4516,7 @@
         <v>1.077</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
         <v>278</v>
       </c>
@@ -4472,7 +4533,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="53" t="s">
         <v>281</v>
       </c>
@@ -4489,46 +4550,46 @@
         <v>280</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="53" t="s">
+        <v>328</v>
+      </c>
+      <c r="B19" s="54" t="s">
         <v>329</v>
-      </c>
-      <c r="B19" s="54" t="s">
-        <v>330</v>
       </c>
       <c r="C19" s="54" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="53" t="s">
         <v>332</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="53" t="s">
+      <c r="B20" s="54" t="s">
         <v>333</v>
-      </c>
-      <c r="B20" s="54" t="s">
-        <v>334</v>
       </c>
       <c r="C20" s="54" t="s">
         <v>61</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E20" s="7">
         <v>1.82</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="53" t="s">
+        <v>340</v>
+      </c>
+      <c r="B21" s="54" t="s">
         <v>341</v>
-      </c>
-      <c r="B21" s="54" t="s">
-        <v>342</v>
       </c>
       <c r="C21" s="54" t="s">
         <v>23</v>
@@ -4540,63 +4601,63 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="53" t="s">
+        <v>342</v>
+      </c>
+      <c r="B22" s="54" t="s">
         <v>343</v>
-      </c>
-      <c r="B22" s="54" t="s">
-        <v>344</v>
       </c>
       <c r="C22" s="54" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E22" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="53" t="s">
+        <v>344</v>
+      </c>
+      <c r="B23" s="54" t="s">
         <v>345</v>
-      </c>
-      <c r="B23" s="54" t="s">
-        <v>346</v>
       </c>
       <c r="C23" s="54" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="53" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B24" s="54" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C24" s="54" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E24" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="47" t="s">
+        <v>359</v>
+      </c>
+      <c r="B25" s="18" t="s">
         <v>360</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>361</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>11</v>
@@ -4606,46 +4667,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="53" t="s">
+        <v>353</v>
+      </c>
+      <c r="B26" s="54" t="s">
         <v>354</v>
-      </c>
-      <c r="B26" s="54" t="s">
-        <v>355</v>
       </c>
       <c r="C26" s="54" t="s">
         <v>61</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E26" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="53" t="s">
+        <v>356</v>
+      </c>
+      <c r="B27" s="54" t="s">
         <v>357</v>
-      </c>
-      <c r="B27" s="54" t="s">
-        <v>358</v>
       </c>
       <c r="C27" s="54" t="s">
         <v>61</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E27" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="B28" s="54" t="s">
         <v>362</v>
-      </c>
-      <c r="B28" s="54" t="s">
-        <v>363</v>
       </c>
       <c r="C28" s="54" t="s">
         <v>11</v>
@@ -4655,9 +4716,24 @@
         <v>3</v>
       </c>
     </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="53" t="s">
+        <v>381</v>
+      </c>
+      <c r="B29" s="54" t="s">
+        <v>382</v>
+      </c>
+      <c r="C29" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="21"/>
+      <c r="E29" s="7" t="s">
+        <v>380</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B28">
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+  <conditionalFormatting sqref="B2:B29">
+    <cfRule type="duplicateValues" dxfId="37" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4690,18 +4766,18 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.44140625" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>198</v>
       </c>
@@ -4724,7 +4800,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>250</v>
       </c>
@@ -4745,7 +4821,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>251</v>
       </c>
@@ -4762,7 +4838,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>59</v>
       </c>
@@ -4781,7 +4857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>62</v>
       </c>
@@ -4800,7 +4876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>165</v>
       </c>
@@ -4821,7 +4897,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4835,27 +4911,27 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" customWidth="1"/>
+    <col min="1" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C1" s="21" t="s">
         <v>252</v>
       </c>
@@ -4893,7 +4969,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>205</v>
       </c>
@@ -4937,7 +5013,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>212</v>
       </c>
@@ -4981,7 +5057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>212</v>
       </c>
@@ -5025,7 +5101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>212</v>
       </c>
@@ -5069,7 +5145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>212</v>
       </c>
@@ -5113,7 +5189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>212</v>
       </c>
@@ -5157,7 +5233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>212</v>
       </c>
@@ -5201,7 +5277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>212</v>
       </c>
@@ -5258,24 +5334,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAEB3671-1ED6-422F-86FB-257A56869058}">
   <dimension ref="A2:N170"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>249</v>
       </c>
@@ -5310,7 +5386,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>1</v>
       </c>
@@ -5345,7 +5421,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>2</v>
       </c>
@@ -5380,7 +5456,7 @@
         <v>4.8499999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>3</v>
       </c>
@@ -5415,7 +5491,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>4</v>
       </c>
@@ -5450,7 +5526,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>5</v>
       </c>
@@ -5485,7 +5561,7 @@
         <v>4.7699999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>6</v>
       </c>
@@ -5520,7 +5596,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>7</v>
       </c>
@@ -5555,7 +5631,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>8</v>
       </c>
@@ -5590,7 +5666,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>9</v>
       </c>
@@ -5625,7 +5701,7 @@
         <v>2.74</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>10</v>
       </c>
@@ -5660,7 +5736,7 @@
         <v>4.79</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>11</v>
       </c>
@@ -5695,7 +5771,7 @@
         <v>6.61</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>12</v>
       </c>
@@ -5730,7 +5806,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>13</v>
       </c>
@@ -5765,7 +5841,7 @@
         <v>4.8899999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>14</v>
       </c>
@@ -5800,7 +5876,7 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
         <v>15</v>
       </c>
@@ -5835,7 +5911,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>16</v>
       </c>
@@ -5870,7 +5946,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>17</v>
       </c>
@@ -5905,7 +5981,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>18</v>
       </c>
@@ -5940,7 +6016,7 @@
         <v>4.91</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>19</v>
       </c>
@@ -5975,7 +6051,7 @@
         <v>6.88</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>20</v>
       </c>
@@ -6010,7 +6086,7 @@
         <v>6.52</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>21</v>
       </c>
@@ -6045,7 +6121,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <v>22</v>
       </c>
@@ -6080,7 +6156,7 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <v>23</v>
       </c>
@@ -6115,7 +6191,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>24</v>
       </c>
@@ -6150,7 +6226,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>25</v>
       </c>
@@ -6185,7 +6261,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>26</v>
       </c>
@@ -6220,7 +6296,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>27</v>
       </c>
@@ -6255,7 +6331,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>28</v>
       </c>
@@ -6290,7 +6366,7 @@
         <v>6.87</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
         <v>29</v>
       </c>
@@ -6325,7 +6401,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <v>30</v>
       </c>
@@ -6360,7 +6436,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>31</v>
       </c>
@@ -6395,7 +6471,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>32</v>
       </c>
@@ -6430,7 +6506,7 @@
         <v>2.76</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>33</v>
       </c>
@@ -6465,7 +6541,7 @@
         <v>2.77</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>34</v>
       </c>
@@ -6500,7 +6576,7 @@
         <v>5.77</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>35</v>
       </c>
@@ -6535,7 +6611,7 @@
         <v>7.46</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>36</v>
       </c>
@@ -6570,7 +6646,7 @@
         <v>7.11</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>37</v>
       </c>
@@ -6605,7 +6681,7 @@
         <v>4.97</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <v>38</v>
       </c>
@@ -6640,7 +6716,7 @@
         <v>4.08</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
         <v>39</v>
       </c>
@@ -6675,7 +6751,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>40</v>
       </c>
@@ -6710,7 +6786,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
         <v>41</v>
       </c>
@@ -6745,7 +6821,7 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>42</v>
       </c>
@@ -6780,7 +6856,7 @@
         <v>5.97</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <v>43</v>
       </c>
@@ -6815,7 +6891,7 @@
         <v>7.56</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="17">
         <v>44</v>
       </c>
@@ -6850,7 +6926,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <v>45</v>
       </c>
@@ -6885,7 +6961,7 @@
         <v>5.07</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>46</v>
       </c>
@@ -6920,7 +6996,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
         <v>47</v>
       </c>
@@ -6955,7 +7031,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
         <v>48</v>
       </c>
@@ -6990,7 +7066,7 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>49</v>
       </c>
@@ -7025,7 +7101,7 @@
         <v>3.37</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="17">
         <v>50</v>
       </c>
@@ -7060,7 +7136,7 @@
         <v>6.43</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="17">
         <v>51</v>
       </c>
@@ -7095,7 +7171,7 @@
         <v>7.83</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
         <v>52</v>
       </c>
@@ -7130,7 +7206,7 @@
         <v>7.59</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="17">
         <v>53</v>
       </c>
@@ -7165,7 +7241,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
         <v>54</v>
       </c>
@@ -7200,7 +7276,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
         <v>55</v>
       </c>
@@ -7235,7 +7311,7 @@
         <v>4.22</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="17">
         <v>56</v>
       </c>
@@ -7270,7 +7346,7 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="17">
         <v>57</v>
       </c>
@@ -7305,7 +7381,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="17">
         <v>58</v>
       </c>
@@ -7340,7 +7416,7 @@
         <v>8.94</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="17">
         <v>59</v>
       </c>
@@ -7375,7 +7451,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="17">
         <v>60</v>
       </c>
@@ -7410,7 +7486,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="17">
         <v>61</v>
       </c>
@@ -7445,7 +7521,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
         <v>62</v>
       </c>
@@ -7480,7 +7556,7 @@
         <v>6.71</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="17">
         <v>63</v>
       </c>
@@ -7515,7 +7591,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="17">
         <v>64</v>
       </c>
@@ -7550,7 +7626,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="17">
         <v>65</v>
       </c>
@@ -7585,7 +7661,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="17">
         <v>66</v>
       </c>
@@ -7620,7 +7696,7 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
         <v>67</v>
       </c>
@@ -7655,7 +7731,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="17">
         <v>68</v>
       </c>
@@ -7690,7 +7766,7 @@
         <v>10.59</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="17">
         <v>69</v>
       </c>
@@ -7725,7 +7801,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="17">
         <v>70</v>
       </c>
@@ -7760,7 +7836,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="17">
         <v>71</v>
       </c>
@@ -7795,7 +7871,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="17">
         <v>72</v>
       </c>
@@ -7830,7 +7906,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="17">
         <v>73</v>
       </c>
@@ -7865,7 +7941,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="17">
         <v>74</v>
       </c>
@@ -7900,7 +7976,7 @@
         <v>9.2100000000000009</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="17">
         <v>75</v>
       </c>
@@ -7938,7 +8014,7 @@
       <c r="M77" s="7"/>
       <c r="N77" s="7"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="17">
         <v>76</v>
       </c>
@@ -7976,7 +8052,7 @@
       <c r="M78" s="7"/>
       <c r="N78" s="7"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="17">
         <v>77</v>
       </c>
@@ -8014,7 +8090,7 @@
       <c r="M79" s="7"/>
       <c r="N79" s="7"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="17">
         <v>78</v>
       </c>
@@ -8052,7 +8128,7 @@
       <c r="M80" s="7"/>
       <c r="N80" s="7"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="17">
         <v>79</v>
       </c>
@@ -8090,7 +8166,7 @@
       <c r="M81" s="7"/>
       <c r="N81" s="7"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="17">
         <v>80</v>
       </c>
@@ -8128,7 +8204,7 @@
       <c r="M82" s="7"/>
       <c r="N82" s="7"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="17">
         <v>81</v>
       </c>
@@ -8166,7 +8242,7 @@
       <c r="M83" s="7"/>
       <c r="N83" s="7"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="17">
         <v>82</v>
       </c>
@@ -8204,7 +8280,7 @@
       <c r="M84" s="7"/>
       <c r="N84" s="7"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="17">
         <v>83</v>
       </c>
@@ -8242,7 +8318,7 @@
       <c r="M85" s="7"/>
       <c r="N85" s="7"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="17">
         <v>84</v>
       </c>
@@ -8280,7 +8356,7 @@
       <c r="M86" s="7"/>
       <c r="N86" s="7"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="17">
         <v>85</v>
       </c>
@@ -8318,7 +8394,7 @@
       <c r="M87" s="7"/>
       <c r="N87" s="7"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="17">
         <v>86</v>
       </c>
@@ -8356,7 +8432,7 @@
       <c r="M88" s="7"/>
       <c r="N88" s="7"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="17">
         <v>87</v>
       </c>
@@ -8394,7 +8470,7 @@
       <c r="M89" s="7"/>
       <c r="N89" s="7"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="17">
         <v>88</v>
       </c>
@@ -8429,7 +8505,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="17">
         <v>89</v>
       </c>
@@ -8464,7 +8540,7 @@
         <v>5.61</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="17">
         <v>90</v>
       </c>
@@ -8499,7 +8575,7 @@
         <v>9.56</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="17">
         <v>91</v>
       </c>
@@ -8534,7 +8610,7 @@
         <v>10.29</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="17">
         <v>92</v>
       </c>
@@ -8569,7 +8645,7 @@
         <v>10.81</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="17">
         <v>93</v>
       </c>
@@ -8604,7 +8680,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="17">
         <v>94</v>
       </c>
@@ -8639,7 +8715,7 @@
         <v>7.44</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="17">
         <v>95</v>
       </c>
@@ -8674,7 +8750,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="17">
         <v>96</v>
       </c>
@@ -8709,7 +8785,7 @@
         <v>2.23</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="17">
         <v>97</v>
       </c>
@@ -8744,7 +8820,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="17">
         <v>98</v>
       </c>
@@ -8779,7 +8855,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="17">
         <v>99</v>
       </c>
@@ -8814,7 +8890,7 @@
         <v>10.32</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="17">
         <v>100</v>
       </c>
@@ -8849,7 +8925,7 @@
         <v>10.84</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="17">
         <v>101</v>
       </c>
@@ -8884,7 +8960,7 @@
         <v>8.51</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="17">
         <v>102</v>
       </c>
@@ -8919,7 +8995,7 @@
         <v>7.57</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="17">
         <v>103</v>
       </c>
@@ -8954,7 +9030,7 @@
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="17">
         <v>104</v>
       </c>
@@ -8989,7 +9065,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="17">
         <v>105</v>
       </c>
@@ -9024,7 +9100,7 @@
         <v>6.23</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="17">
         <v>106</v>
       </c>
@@ -9059,7 +9135,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="17">
         <v>107</v>
       </c>
@@ -9094,7 +9170,7 @@
         <v>10.43</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="17">
         <v>108</v>
       </c>
@@ -9129,7 +9205,7 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="17">
         <v>109</v>
       </c>
@@ -9164,7 +9240,7 @@
         <v>8.7200000000000006</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="17">
         <v>110</v>
       </c>
@@ -9199,7 +9275,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="17">
         <v>111</v>
       </c>
@@ -9234,7 +9310,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="17">
         <v>112</v>
       </c>
@@ -9269,7 +9345,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="17">
         <v>113</v>
       </c>
@@ -9304,7 +9380,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="17">
         <v>114</v>
       </c>
@@ -9339,7 +9415,7 @@
         <v>8.94</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="17">
         <v>115</v>
       </c>
@@ -9374,7 +9450,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="17">
         <v>116</v>
       </c>
@@ -9409,7 +9485,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="17">
         <v>117</v>
       </c>
@@ -9444,7 +9520,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="17">
         <v>118</v>
       </c>
@@ -9479,7 +9555,7 @@
         <v>6.71</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="17">
         <v>119</v>
       </c>
@@ -9514,7 +9590,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="17">
         <v>120</v>
       </c>
@@ -9549,7 +9625,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="17">
         <v>121</v>
       </c>
@@ -9584,7 +9660,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="17">
         <v>122</v>
       </c>
@@ -9619,7 +9695,7 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="17">
         <v>123</v>
       </c>
@@ -9654,7 +9730,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="17">
         <v>124</v>
       </c>
@@ -9689,7 +9765,7 @@
         <v>10.59</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="17">
         <v>125</v>
       </c>
@@ -9724,7 +9800,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="17">
         <v>126</v>
       </c>
@@ -9759,7 +9835,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="17">
         <v>127</v>
       </c>
@@ -9794,7 +9870,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="17">
         <v>128</v>
       </c>
@@ -9829,7 +9905,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="17">
         <v>129</v>
       </c>
@@ -9864,7 +9940,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="17">
         <v>130</v>
       </c>
@@ -9899,7 +9975,7 @@
         <v>9.2100000000000009</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="17">
         <v>131</v>
       </c>
@@ -9934,7 +10010,7 @@
         <v>10.11</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="17">
         <v>132</v>
       </c>
@@ -9969,7 +10045,7 @@
         <v>10.67</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="17">
         <v>133</v>
       </c>
@@ -10004,7 +10080,7 @@
         <v>8.11</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="17">
         <v>134</v>
       </c>
@@ -10039,7 +10115,7 @@
         <v>7.09</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="17">
         <v>135</v>
       </c>
@@ -10074,7 +10150,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="17">
         <v>136</v>
       </c>
@@ -10109,7 +10185,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="17">
         <v>137</v>
       </c>
@@ -10144,7 +10220,7 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="17">
         <v>138</v>
       </c>
@@ -10179,7 +10255,7 @@
         <v>9.4499999999999993</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="17">
         <v>139</v>
       </c>
@@ -10214,7 +10290,7 @@
         <v>10.23</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="17">
         <v>140</v>
       </c>
@@ -10249,7 +10325,7 @@
         <v>10.76</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="17">
         <v>141</v>
       </c>
@@ -10284,7 +10360,7 @@
         <v>8.31</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="17">
         <v>142</v>
       </c>
@@ -10319,7 +10395,7 @@
         <v>7.26</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="17">
         <v>143</v>
       </c>
@@ -10354,7 +10430,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="17">
         <v>144</v>
       </c>
@@ -10389,7 +10465,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="17">
         <v>145</v>
       </c>
@@ -10424,7 +10500,7 @@
         <v>5.61</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="17">
         <v>146</v>
       </c>
@@ -10459,7 +10535,7 @@
         <v>9.56</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="17">
         <v>147</v>
       </c>
@@ -10494,7 +10570,7 @@
         <v>10.29</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="17">
         <v>148</v>
       </c>
@@ -10529,7 +10605,7 @@
         <v>10.81</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="17">
         <v>149</v>
       </c>
@@ -10564,7 +10640,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="17">
         <v>150</v>
       </c>
@@ -10599,7 +10675,7 @@
         <v>7.44</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="17">
         <v>151</v>
       </c>
@@ -10634,7 +10710,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="17">
         <v>152</v>
       </c>
@@ -10669,7 +10745,7 @@
         <v>2.23</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="17">
         <v>153</v>
       </c>
@@ -10704,7 +10780,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="17">
         <v>154</v>
       </c>
@@ -10739,7 +10815,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="17">
         <v>155</v>
       </c>
@@ -10774,7 +10850,7 @@
         <v>10.32</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="17">
         <v>156</v>
       </c>
@@ -10809,7 +10885,7 @@
         <v>10.84</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="17">
         <v>157</v>
       </c>
@@ -10844,7 +10920,7 @@
         <v>8.51</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="17">
         <v>158</v>
       </c>
@@ -10879,7 +10955,7 @@
         <v>7.57</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="17">
         <v>159</v>
       </c>
@@ -10914,7 +10990,7 @@
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="17">
         <v>160</v>
       </c>
@@ -10949,7 +11025,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="17">
         <v>161</v>
       </c>
@@ -10984,7 +11060,7 @@
         <v>6.23</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="17">
         <v>162</v>
       </c>
@@ -11019,7 +11095,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="17">
         <v>163</v>
       </c>
@@ -11054,7 +11130,7 @@
         <v>10.43</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="17">
         <v>164</v>
       </c>
@@ -11089,7 +11165,7 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="17">
         <v>165</v>
       </c>
@@ -11124,7 +11200,7 @@
         <v>8.7200000000000006</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="17">
         <v>166</v>
       </c>
@@ -11159,7 +11235,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="17">
         <v>167</v>
       </c>
@@ -11194,7 +11270,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="17">
         <v>168</v>
       </c>
@@ -11231,7 +11307,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11245,18 +11321,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{747D2C16-55D6-4EA7-A7D7-F3FDFC546D7E}">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="9.109375" customWidth="1"/>
-    <col min="20" max="20" width="19.88671875" customWidth="1"/>
-    <col min="21" max="21" width="14.5546875" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="20" max="20" width="19.85546875" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>284</v>
       </c>
@@ -11279,30 +11355,30 @@
       <c r="R1" s="30"/>
       <c r="S1" s="30"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>301</v>
       </c>
       <c r="B2" s="39" t="s">
+        <v>323</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>324</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="D2" s="39" t="s">
         <v>325</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="E2" s="39" t="s">
         <v>326</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="F2" s="40" t="s">
         <v>327</v>
       </c>
-      <c r="F2" s="40" t="s">
-        <v>328</v>
-      </c>
       <c r="G2" s="40" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H2" s="40" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I2" s="31"/>
       <c r="J2" s="31"/>
@@ -11335,13 +11411,13 @@
         <v>304</v>
       </c>
       <c r="T2" s="56" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="U2" s="57" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
       <c r="B3" s="32" t="s">
         <v>285</v>
@@ -11390,19 +11466,19 @@
         <v>299</v>
       </c>
       <c r="R3" s="38" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="S3" s="36" t="s">
         <v>300</v>
       </c>
       <c r="T3" s="57" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="U3" s="57" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>306</v>
       </c>
@@ -11469,13 +11545,13 @@
         <v>0.17468808908511205</v>
       </c>
       <c r="T4" s="58" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="U4" s="59" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>308</v>
       </c>
@@ -11542,13 +11618,13 @@
         <v>0.21827857661222116</v>
       </c>
       <c r="T5" s="58" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="U5" s="59" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>310</v>
       </c>
@@ -11615,13 +11691,13 @@
         <v>0.33925486716397496</v>
       </c>
       <c r="T6" s="58" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="U6" s="59" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>312</v>
       </c>
@@ -11688,15 +11764,15 @@
         <v>0.38567931065615685</v>
       </c>
       <c r="T7" s="58" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="U7" s="59" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>314</v>
+        <v>380</v>
       </c>
       <c r="B8" s="31">
         <v>200</v>
@@ -11739,7 +11815,7 @@
         <v>802.47</v>
       </c>
       <c r="N8" s="44" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O8" s="45">
         <v>690</v>
@@ -11761,15 +11837,15 @@
         <v>0.62277816214005777</v>
       </c>
       <c r="T8" s="58" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="U8" s="59" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B9" s="34">
         <v>700</v>
@@ -11812,7 +11888,7 @@
         <v>2307.9</v>
       </c>
       <c r="N9" s="44" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O9" s="45">
         <v>2100</v>
@@ -11834,15 +11910,15 @@
         <v>0.89569006135575246</v>
       </c>
       <c r="T9" s="58" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="U9" s="55" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B10" s="31">
         <v>2000</v>
@@ -11885,7 +11961,7 @@
         <v>5059.2</v>
       </c>
       <c r="N10" s="44" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="O10" s="45">
         <v>4800</v>
@@ -11913,9 +11989,9 @@
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B11" s="31">
         <v>4000</v>
@@ -11958,7 +12034,7 @@
         <v>8704</v>
       </c>
       <c r="N11" s="44" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="O11" s="45">
         <v>8500</v>
@@ -11982,9 +12058,9 @@
       <c r="T11" s="58"/>
       <c r="U11" s="59"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B12" s="31">
         <v>6500</v>
@@ -12027,7 +12103,7 @@
         <v>13026</v>
       </c>
       <c r="N12" s="44" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="O12" s="45">
         <v>13000</v>
@@ -12057,16 +12133,279 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BADE3C9-F1E8-4518-8FC3-9DDBC15FFDFD}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>371</v>
+      </c>
+      <c r="F1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E2" t="s">
+        <v>383</v>
+      </c>
+      <c r="F2" t="s">
+        <v>369</v>
+      </c>
+      <c r="G2" t="s">
+        <v>374</v>
+      </c>
+      <c r="H2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" t="s">
+        <v>379</v>
+      </c>
+      <c r="D3">
+        <v>1.99</v>
+      </c>
+      <c r="E3" t="s">
+        <v>372</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>321</v>
+      </c>
+      <c r="I3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" t="s">
+        <v>379</v>
+      </c>
+      <c r="D4">
+        <v>1.99</v>
+      </c>
+      <c r="E4" t="s">
+        <v>373</v>
+      </c>
+      <c r="F4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H4" t="s">
+        <v>380</v>
+      </c>
+      <c r="I4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C5" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5">
+        <v>1.99</v>
+      </c>
+      <c r="E5" t="s">
+        <v>373</v>
+      </c>
+      <c r="F5" t="s">
+        <v>380</v>
+      </c>
+      <c r="H5" t="s">
+        <v>380</v>
+      </c>
+      <c r="I5" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C6" t="s">
+        <v>379</v>
+      </c>
+      <c r="D6">
+        <v>1.8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>373</v>
+      </c>
+      <c r="F6" t="s">
+        <v>310</v>
+      </c>
+      <c r="H6" t="s">
+        <v>380</v>
+      </c>
+      <c r="I6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7">
+        <v>2.35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>373</v>
+      </c>
+      <c r="F7" t="s">
+        <v>310</v>
+      </c>
+      <c r="H7" t="s">
+        <v>310</v>
+      </c>
+      <c r="I7" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8">
+        <v>2.35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>373</v>
+      </c>
+      <c r="F8" t="s">
+        <v>310</v>
+      </c>
+      <c r="H8" t="s">
+        <v>310</v>
+      </c>
+      <c r="I8" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>2.35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>373</v>
+      </c>
+      <c r="F9" t="s">
+        <v>310</v>
+      </c>
+      <c r="H9" t="s">
+        <v>310</v>
+      </c>
+      <c r="I9" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{13C27F1A-C23E-4325-AD3F-BF27B7EFCF13}">
+          <x14:formula1>
+            <xm:f>input_rock_gradings!$A$4:$A$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3:F9 H3:I9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008ABF17219AE49A4BA0BDD81D071BF678" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27f34586c84b8c90a2cb002f0f0fc035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fc9abb88-5dc8-4425-a823-e2986ac3f199" xmlns:ns4="13eb6276-85db-4ef3-a671-167ab07ac255" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ec505085f4519de6c764bdf3897c86a" ns3:_="" ns4:_="">
     <xsd:import namespace="fc9abb88-5dc8-4425-a823-e2986ac3f199"/>
@@ -12295,6 +12634,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -12302,14 +12650,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60595BF4-BDC7-43A9-9318-C73E99FECE97}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12324,6 +12664,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Completed validation functions by adding toe armour stability validation
</commit_message>
<xml_diff>
--- a/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
+++ b/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JY6\github\breakwater\Notebooks\Constanta Phase III\Input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD1D6321-167E-4B47-B495-15ED9B8147B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B49F237-E56C-4AAE-A627-9B36B4D8112B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="709" firstSheet="1" activeTab="8" xr2:uid="{06ED436A-2CC0-4489-A506-29F94518B839}"/>
   </bookViews>
@@ -5334,8 +5334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAEB3671-1ED6-422F-86FB-257A56869058}">
   <dimension ref="A2:N170"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11322,7 +11322,7 @@
   <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12138,7 +12138,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Results first run Phase III test data
</commit_message>
<xml_diff>
--- a/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
+++ b/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JY6\github\breakwater\Notebooks\Constanta Phase III\Input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B49F237-E56C-4AAE-A627-9B36B4D8112B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A15E3745-4F4A-4777-84DF-4313DEC07554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="709" firstSheet="1" activeTab="8" xr2:uid="{06ED436A-2CC0-4489-A506-29F94518B839}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="709" firstSheet="1" activeTab="5" xr2:uid="{06ED436A-2CC0-4489-A506-29F94518B839}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="388">
   <si>
     <t>Input</t>
   </si>
@@ -1308,13 +1308,25 @@
   <si>
     <t>Armour_type</t>
   </si>
+  <si>
+    <t>Structure slope rock armour</t>
+  </si>
+  <si>
+    <t>Structure slope concrete armour</t>
+  </si>
+  <si>
+    <t>tan_a_rock</t>
+  </si>
+  <si>
+    <t>tan_a_concrete</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="174" formatCode="0.000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1588,7 +1600,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1636,13 +1647,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FADF3455-3E5D-4FF3-B5C3-EF436E5E06DA}"/>
     <cellStyle name="Percent 2" xfId="2" xr:uid="{25A54706-C93D-426F-AE2B-7B22D5D53704}"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="49">
+    <dxf>
+      <numFmt numFmtId="174" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="174" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1754,16 +1812,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1775,9 +1823,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000000000000"/>
     </dxf>
     <dxf>
       <font>
@@ -1968,16 +2013,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2122,16 +2157,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -2213,16 +2238,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2237,7 +2252,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{128A59F9-895D-4C60-8954-4F77FF691FFB}" name="Overview" displayName="Overview" ref="A2:G62" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{128A59F9-895D-4C60-8954-4F77FF691FFB}" name="Overview" displayName="Overview" ref="A2:G62" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46">
   <autoFilter ref="A2:G62" xr:uid="{C615D3FE-C5C3-4AC1-8573-2115046F6FC7}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{FDED3D30-FC03-4894-AAAE-7069E3558798}" name="Input"/>
@@ -2245,8 +2260,8 @@
     <tableColumn id="3" xr3:uid="{122DBA8D-3347-48F4-8A76-270615744B5D}" name="Unit"/>
     <tableColumn id="4" xr3:uid="{B4BA3D29-867B-4EF8-A808-EE6581BB8115}" name="Category"/>
     <tableColumn id="5" xr3:uid="{CB74FB27-39F6-4359-BAC6-C5DFAC8E01C0}" name="Used for"/>
-    <tableColumn id="6" xr3:uid="{266927E0-00C5-4D6A-BB41-21164D34B2CE}" name="Necessary input" dataDxfId="43"/>
-    <tableColumn id="7" xr3:uid="{30AC8882-C2A6-43C1-86B7-25C9ED481C62}" name="Remarks" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{266927E0-00C5-4D6A-BB41-21164D34B2CE}" name="Necessary input" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{30AC8882-C2A6-43C1-86B7-25C9ED481C62}" name="Remarks" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2306,58 +2321,59 @@
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{32645932-B206-41E7-B1E9-2A52D9AE0D60}" name="Limit State"/>
     <tableColumn id="1" xr3:uid="{B6826C86-D95D-4464-8196-B4E1CEBC5F0A}" name="Nod"/>
-    <tableColumn id="2" xr3:uid="{12FE237E-CE70-4E63-BE4C-9D0365BAB8AC}" name="Accropode II-trunk" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{3045C02B-DCDC-42A1-B50F-88D0E610E62A}" name="Accropode II-roundhead" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{0280B610-A0B2-48C8-AB40-3AE6F87EDE4A}" name="Xbloc-trunk" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{C26BCBB6-089E-47C5-9394-EA17687F6843}" name="Xbloc-roundhead" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{12FE237E-CE70-4E63-BE4C-9D0365BAB8AC}" name="Accropode II-trunk" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{3045C02B-DCDC-42A1-B50F-88D0E610E62A}" name="Accropode II-roundhead" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{0280B610-A0B2-48C8-AB40-3AE6F87EDE4A}" name="Xbloc-trunk" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{C26BCBB6-089E-47C5-9394-EA17687F6843}" name="Xbloc-roundhead" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{88915663-9067-4DC4-90A4-2D7CD517273B}" name="input_project" displayName="input_project" ref="A1:E29" totalsRowShown="0" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{88915663-9067-4DC4-90A4-2D7CD517273B}" name="input_project" displayName="input_project" ref="A1:E29" totalsRowShown="0" dataDxfId="39">
   <autoFilter ref="A1:E29" xr:uid="{8653FB80-28B1-42DD-ADDB-1F402573EE6E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{10575A1B-65C2-4D3D-A919-D5D631E15E73}" name="Parameter" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{9F5575C0-7208-43BD-86BC-6A3485FF384C}" name="Symbol" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{1CF28AEF-1CBA-48D2-A66A-EE6DC73C8CC9}" name="Unit " dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{FB5987BB-56D7-412F-8C95-1F5820C3E77A}" name="Explanation" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{5ABE4DA7-DB09-46BC-AF34-3D5B699627F3}" name="Value" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{10575A1B-65C2-4D3D-A919-D5D631E15E73}" name="Parameter" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{9F5575C0-7208-43BD-86BC-6A3485FF384C}" name="Symbol" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{1CF28AEF-1CBA-48D2-A66A-EE6DC73C8CC9}" name="Unit " dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{FB5987BB-56D7-412F-8C95-1F5820C3E77A}" name="Explanation" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{5ABE4DA7-DB09-46BC-AF34-3D5B699627F3}" name="Value" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6634BB44-66AA-43C5-94C9-21ADB80AD51A}" name="input_requirements" displayName="input_requirements" ref="A1:G6" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6634BB44-66AA-43C5-94C9-21ADB80AD51A}" name="input_requirements" displayName="input_requirements" ref="A1:G6" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
   <autoFilter ref="A1:G6" xr:uid="{AC8FC8D0-6474-4C46-AABC-7775C18E706C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{ED5624B9-4A0A-4F41-BA44-D0E02EE32577}" name="Parameter" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{2B068622-98F3-4E2A-BE8E-A97C121E3F4C}" name="Symbol" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{4BC1E5B1-1862-4E8F-8CC1-D2F05F356929}" name="Unit " dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{F431E098-CB44-4ACA-97A5-C64500DD9528}" name="Explanation" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{C6914755-DB47-4220-827C-0984890970A0}" name="ELS" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{D3A99EAE-B2C9-4E74-B3E2-A288F4532A21}" name="SLS" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{9350B3BA-690A-42F3-BB94-29E26F161B54}" name="ULS" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{ED5624B9-4A0A-4F41-BA44-D0E02EE32577}" name="Parameter" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{2B068622-98F3-4E2A-BE8E-A97C121E3F4C}" name="Symbol" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{4BC1E5B1-1862-4E8F-8CC1-D2F05F356929}" name="Unit " dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{F431E098-CB44-4ACA-97A5-C64500DD9528}" name="Explanation" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{C6914755-DB47-4220-827C-0984890970A0}" name="ELS" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{D3A99EAE-B2C9-4E74-B3E2-A288F4532A21}" name="SLS" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{9350B3BA-690A-42F3-BB94-29E26F161B54}" name="ULS" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5DFFFB11-DDA0-4FF0-A99C-C5B40B22BB0F}" name="input_cross_section" displayName="input_cross_section" ref="A2:N9" totalsRowShown="0" tableBorderDxfId="19">
-  <autoFilter ref="A2:N9" xr:uid="{EDBA852A-A4D9-4055-8891-B74537BE60D1}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{65F89A4D-13BC-480A-9A54-9B5181E61222}" name="Structure" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{DD7D1624-C590-49ED-8883-96E10DDFDC57}" name="Chainage" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{56CAAB95-7C5D-4C77-9690-8C7E28E5E58F}" name="dir_structure" dataDxfId="16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5DFFFB11-DDA0-4FF0-A99C-C5B40B22BB0F}" name="input_cross_section" displayName="input_cross_section" ref="A2:O9" totalsRowShown="0" tableBorderDxfId="23">
+  <autoFilter ref="A2:O9" xr:uid="{EDBA852A-A4D9-4055-8891-B74537BE60D1}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{65F89A4D-13BC-480A-9A54-9B5181E61222}" name="Structure" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{DD7D1624-C590-49ED-8883-96E10DDFDC57}" name="Chainage" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{56CAAB95-7C5D-4C77-9690-8C7E28E5E58F}" name="dir_structure" dataDxfId="20"/>
     <tableColumn id="4" xr3:uid="{3211485F-4253-4196-9552-5388E1C18679}" name="z_bed"/>
     <tableColumn id="5" xr3:uid="{12FF2071-DB6F-4635-AAF2-7224DB03F7AF}" name="public"/>
     <tableColumn id="6" xr3:uid="{3C50E8D0-D9A3-4D42-9184-21A91AB97D26}" name="P"/>
-    <tableColumn id="7" xr3:uid="{67557D02-D417-4935-83D4-56C7A3EC4E57}" name="tan_a" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{67557D02-D417-4935-83D4-56C7A3EC4E57}" name="tan_a_rock" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{9B5FF299-F64E-435F-BA43-2A7ACF5DBC47}" name="tan_a_concrete" dataDxfId="0"/>
     <tableColumn id="9" xr3:uid="{0A204ACD-A807-4615-BEB7-8F6AA353A3CD}" name="Gc"/>
-    <tableColumn id="10" xr3:uid="{0003E8D8-CC23-4555-A626-BC13BBABE9B8}" name="slope_foreshore" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{0003E8D8-CC23-4555-A626-BC13BBABE9B8}" name="slope_foreshore" dataDxfId="19"/>
     <tableColumn id="12" xr3:uid="{74307101-79D4-4197-A798-20BAE3C12767}" name="crest_roughness"/>
     <tableColumn id="13" xr3:uid="{30E9BE3D-820F-4565-AD86-93CC1E7A860F}" name="cot_a_rear"/>
     <tableColumn id="14" xr3:uid="{A3804960-2456-4577-852A-50CF47F120BD}" name="B"/>
@@ -2369,20 +2385,20 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A63CE4AC-CF5D-406B-B465-B4984FB45555}" name="input_hydrometeo" displayName="input_hydrometeo" ref="A2:K170" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A63CE4AC-CF5D-406B-B465-B4984FB45555}" name="input_hydrometeo" displayName="input_hydrometeo" ref="A2:K170" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A2:K170" xr:uid="{8EC5B0C1-E4CA-4C7B-AA39-695D226630E3}"/>
   <tableColumns count="11">
-    <tableColumn id="6" xr3:uid="{F9A5357A-5DE4-4408-A14A-E6698FD3755F}" name="Calculation_case" dataDxfId="10"/>
-    <tableColumn id="1" xr3:uid="{012C1F4F-AAC2-4FD0-A162-E004B1A207F9}" name="Structure" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{BE45E132-052E-4051-A5CC-2691B8D1D576}" name="Chainage" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{CE4FADC8-9574-4B7C-9E02-F0716073BF79}" name="Offshore bin" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{C0A99159-F33E-4796-BC72-CB4DE68B9FDE}" name="Limit State" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{240593D5-435F-4039-BD0D-5B8B3FDD3128}" name="wl" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{1A72D5A3-EEEE-48D4-B8C7-0BC7A1474131}" name="Hm0" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{937FF273-2A9A-4DA7-AC8F-B2F74F1681D7}" name="dir_wave" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{24ED7C68-4403-4BB0-A849-0C22B2AF55BB}" name="Tp" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{A397DA8E-DE81-4096-A083-356358DACD29}" name="Tm-1,0" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{17652E84-F087-4BBA-B4B9-CD36B5153566}" name="Tm0,2" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{F9A5357A-5DE4-4408-A14A-E6698FD3755F}" name="Calculation_case" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{012C1F4F-AAC2-4FD0-A162-E004B1A207F9}" name="Structure" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{BE45E132-052E-4051-A5CC-2691B8D1D576}" name="Chainage" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{CE4FADC8-9574-4B7C-9E02-F0716073BF79}" name="Offshore bin" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{C0A99159-F33E-4796-BC72-CB4DE68B9FDE}" name="Limit State" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{240593D5-435F-4039-BD0D-5B8B3FDD3128}" name="wl" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{1A72D5A3-EEEE-48D4-B8C7-0BC7A1474131}" name="Hm0" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{937FF273-2A9A-4DA7-AC8F-B2F74F1681D7}" name="dir_wave" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{24ED7C68-4403-4BB0-A849-0C22B2AF55BB}" name="Tp" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{A397DA8E-DE81-4096-A083-356358DACD29}" name="Tm-1,0" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{17652E84-F087-4BBA-B4B9-CD36B5153566}" name="Tm0,2" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4040,7 +4056,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B1 B3:B1048576">
-    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4208,16 +4224,16 @@
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="26">
         <v>2.8</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="26">
         <v>2.5</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="27">
         <v>2.77</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="27">
         <v>2.57</v>
       </c>
     </row>
@@ -4228,16 +4244,16 @@
       <c r="B4">
         <v>0.5</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="26">
         <v>3.1</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="26">
         <v>2.8</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="26">
         <v>3.1</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="26">
         <v>2.9</v>
       </c>
     </row>
@@ -4254,7 +4270,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="D22" sqref="D22:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4284,7 +4300,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="46" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="18" t="s">
@@ -4299,7 +4315,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="46" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="18" t="s">
@@ -4314,13 +4330,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="48" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="17"/>
@@ -4329,7 +4345,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="46" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="18" t="s">
@@ -4344,7 +4360,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="46" t="s">
         <v>245</v>
       </c>
       <c r="B6" s="18" t="s">
@@ -4359,7 +4375,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="46" t="s">
         <v>246</v>
       </c>
       <c r="B7" s="18" t="s">
@@ -4374,7 +4390,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="46" t="s">
         <v>247</v>
       </c>
       <c r="B8" s="18" t="s">
@@ -4389,7 +4405,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="46" t="s">
         <v>255</v>
       </c>
       <c r="B9" s="18" t="s">
@@ -4399,12 +4415,12 @@
         <v>11</v>
       </c>
       <c r="D9" s="17"/>
-      <c r="E9" s="50">
+      <c r="E9" s="49">
         <v>6.2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="46" t="s">
         <v>256</v>
       </c>
       <c r="B10" s="18" t="s">
@@ -4414,12 +4430,12 @@
         <v>11</v>
       </c>
       <c r="D10" s="17"/>
-      <c r="E10" s="51">
+      <c r="E10" s="50">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="46" t="s">
         <v>257</v>
       </c>
       <c r="B11" s="18" t="s">
@@ -4429,12 +4445,12 @@
         <v>11</v>
       </c>
       <c r="D11" s="17"/>
-      <c r="E11" s="52">
+      <c r="E11" s="51">
         <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="46" t="s">
         <v>258</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -4444,12 +4460,12 @@
         <v>11</v>
       </c>
       <c r="D12" s="25"/>
-      <c r="E12" s="52">
+      <c r="E12" s="51">
         <v>1.4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="46" t="s">
         <v>152</v>
       </c>
       <c r="B13" s="18" t="s">
@@ -4466,7 +4482,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="46" t="s">
         <v>338</v>
       </c>
       <c r="B14" s="18" t="s">
@@ -4483,13 +4499,13 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="52" t="s">
         <v>264</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="53" t="s">
         <v>263</v>
       </c>
-      <c r="C15" s="54" t="s">
+      <c r="C15" s="53" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="21" t="s">
@@ -4500,13 +4516,13 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="53" t="s">
         <v>266</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="53" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="21" t="s">
@@ -4517,13 +4533,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="52" t="s">
         <v>278</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="53" t="s">
         <v>269</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="53" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="21" t="s">
@@ -4534,13 +4550,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="52" t="s">
         <v>281</v>
       </c>
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="53" t="s">
         <v>282</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="53" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="21" t="s">
@@ -4551,13 +4567,13 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="52" t="s">
         <v>328</v>
       </c>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="53" t="s">
         <v>329</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C19" s="53" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="21" t="s">
@@ -4568,13 +4584,13 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="52" t="s">
         <v>332</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="53" t="s">
         <v>333</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="53" t="s">
         <v>61</v>
       </c>
       <c r="D20" s="21" t="s">
@@ -4585,13 +4601,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="52" t="s">
         <v>340</v>
       </c>
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="53" t="s">
         <v>341</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="53" t="s">
         <v>23</v>
       </c>
       <c r="D21" s="21" t="s">
@@ -4602,13 +4618,13 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="52" t="s">
         <v>342</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="53" t="s">
         <v>343</v>
       </c>
-      <c r="C22" s="54" t="s">
+      <c r="C22" s="53" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="21" t="s">
@@ -4619,13 +4635,13 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="52" t="s">
         <v>344</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="53" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="21" t="s">
@@ -4636,13 +4652,13 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="53" t="s">
+      <c r="A24" s="52" t="s">
         <v>349</v>
       </c>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="53" t="s">
         <v>352</v>
       </c>
-      <c r="C24" s="54" t="s">
+      <c r="C24" s="53" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="21" t="s">
@@ -4653,7 +4669,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="47" t="s">
+      <c r="A25" s="46" t="s">
         <v>359</v>
       </c>
       <c r="B25" s="18" t="s">
@@ -4668,13 +4684,13 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="53" t="s">
+      <c r="A26" s="52" t="s">
         <v>353</v>
       </c>
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="53" t="s">
         <v>354</v>
       </c>
-      <c r="C26" s="54" t="s">
+      <c r="C26" s="53" t="s">
         <v>61</v>
       </c>
       <c r="D26" s="21" t="s">
@@ -4685,13 +4701,13 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
+      <c r="A27" s="52" t="s">
         <v>356</v>
       </c>
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="53" t="s">
         <v>357</v>
       </c>
-      <c r="C27" s="54" t="s">
+      <c r="C27" s="53" t="s">
         <v>61</v>
       </c>
       <c r="D27" s="21" t="s">
@@ -4702,13 +4718,13 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="53" t="s">
+      <c r="A28" s="52" t="s">
         <v>361</v>
       </c>
-      <c r="B28" s="54" t="s">
+      <c r="B28" s="53" t="s">
         <v>362</v>
       </c>
-      <c r="C28" s="54" t="s">
+      <c r="C28" s="53" t="s">
         <v>11</v>
       </c>
       <c r="D28" s="21"/>
@@ -4717,13 +4733,13 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="52" t="s">
         <v>381</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="53" t="s">
         <v>382</v>
       </c>
-      <c r="C29" s="54" t="s">
+      <c r="C29" s="53" t="s">
         <v>11</v>
       </c>
       <c r="D29" s="21"/>
@@ -4733,7 +4749,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B29">
-    <cfRule type="duplicateValues" dxfId="37" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4897,7 +4913,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="30" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4908,10 +4924,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7027210-EB2D-4810-B641-E47C920F8A87}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4921,17 +4937,17 @@
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.7109375" customWidth="1"/>
+    <col min="7" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C1" s="21" t="s">
         <v>252</v>
       </c>
@@ -4945,31 +4961,34 @@
         <v>31</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>92</v>
+        <v>384</v>
       </c>
       <c r="H1" s="21" t="s">
+        <v>385</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>205</v>
       </c>
@@ -4989,31 +5008,34 @@
         <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>386</v>
       </c>
       <c r="H2" t="s">
+        <v>387</v>
+      </c>
+      <c r="I2" t="s">
         <v>77</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>85</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>279</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>137</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>138</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>227</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>212</v>
       </c>
@@ -5032,32 +5054,35 @@
       <c r="F3" s="24">
         <v>0.5</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="59">
         <v>0.66666666666670005</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="59">
+        <v>0.75</v>
+      </c>
+      <c r="I3" s="24">
         <v>1.5</v>
       </c>
-      <c r="I3" s="24">
+      <c r="J3" s="24">
         <v>300</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="K3" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="K3" s="24">
+      <c r="L3" s="24">
         <v>1.5</v>
       </c>
-      <c r="L3" s="24">
+      <c r="M3" s="24">
         <v>6</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="N3" s="24" t="s">
         <v>268</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>212</v>
       </c>
@@ -5076,32 +5101,35 @@
       <c r="F4" s="24">
         <v>0.5</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="59">
         <v>0.66666666666670005</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="59">
+        <v>0.75</v>
+      </c>
+      <c r="I4" s="24">
         <v>1.5</v>
       </c>
-      <c r="I4" s="24">
+      <c r="J4" s="24">
         <v>300</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="K4" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="K4" s="24">
+      <c r="L4" s="24">
         <v>1.5</v>
       </c>
-      <c r="L4" s="24">
+      <c r="M4" s="24">
         <v>6</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>268</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>212</v>
       </c>
@@ -5120,32 +5148,35 @@
       <c r="F5" s="24">
         <v>0.5</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="59">
         <v>0.66666666666670005</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="59">
+        <v>0.75</v>
+      </c>
+      <c r="I5" s="24">
         <v>1.5</v>
       </c>
-      <c r="I5" s="24">
+      <c r="J5" s="24">
         <v>300</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="K5" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="K5" s="24">
+      <c r="L5" s="24">
         <v>1.5</v>
       </c>
-      <c r="L5" s="24">
+      <c r="M5" s="24">
         <v>6</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>268</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>212</v>
       </c>
@@ -5164,32 +5195,35 @@
       <c r="F6" s="24">
         <v>0.5</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="59">
         <v>0.66666666666670005</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="59">
+        <v>0.75</v>
+      </c>
+      <c r="I6" s="24">
         <v>1.5</v>
       </c>
-      <c r="I6" s="24">
+      <c r="J6" s="24">
         <v>300</v>
       </c>
-      <c r="J6" s="24" t="s">
+      <c r="K6" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="K6" s="24">
+      <c r="L6" s="24">
         <v>1.5</v>
       </c>
-      <c r="L6" s="24">
+      <c r="M6" s="24">
         <v>6</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>268</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>212</v>
       </c>
@@ -5208,32 +5242,35 @@
       <c r="F7" s="24">
         <v>0.5</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="59">
         <v>0.66666666666670005</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="59">
+        <v>0.75</v>
+      </c>
+      <c r="I7" s="24">
         <v>1.5</v>
       </c>
-      <c r="I7" s="24">
+      <c r="J7" s="24">
         <v>300</v>
       </c>
-      <c r="J7" s="24" t="s">
+      <c r="K7" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="K7" s="24">
+      <c r="L7" s="24">
         <v>1.5</v>
       </c>
-      <c r="L7" s="24">
+      <c r="M7" s="24">
         <v>6</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>268</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>212</v>
       </c>
@@ -5252,32 +5289,35 @@
       <c r="F8" s="24">
         <v>0.5</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="59">
         <v>0.66666666666670005</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="59">
+        <v>0.75</v>
+      </c>
+      <c r="I8" s="24">
         <v>1.5</v>
       </c>
-      <c r="I8" s="24">
+      <c r="J8" s="24">
         <v>300</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="K8" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="K8" s="24">
+      <c r="L8" s="24">
         <v>1.5</v>
       </c>
-      <c r="L8" s="24">
+      <c r="M8" s="24">
         <v>6</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>268</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>212</v>
       </c>
@@ -5296,28 +5336,31 @@
       <c r="F9" s="24">
         <v>0.5</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="59">
         <v>0.66666666666670005</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="59">
+        <v>0.75</v>
+      </c>
+      <c r="I9" s="24">
         <v>1.5</v>
       </c>
-      <c r="I9" s="24">
+      <c r="J9" s="24">
         <v>300</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="K9" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="K9" s="24">
+      <c r="L9" s="24">
         <v>1.5</v>
       </c>
-      <c r="L9" s="24">
+      <c r="M9" s="24">
         <v>6</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>268</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>0</v>
       </c>
     </row>
@@ -11307,7 +11350,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11333,799 +11376,799 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>301</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="38" t="s">
         <v>323</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="38" t="s">
         <v>324</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="38" t="s">
         <v>325</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="38" t="s">
         <v>326</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="39" t="s">
         <v>327</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="39" t="s">
         <v>327</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="39" t="s">
         <v>327</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31" t="s">
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30" t="s">
         <v>305</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="L2" s="30" t="s">
         <v>305</v>
       </c>
-      <c r="M2" s="41" t="s">
+      <c r="M2" s="40" t="s">
         <v>305</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="N2" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="O2" s="34" t="s">
         <v>303</v>
       </c>
-      <c r="P2" s="36" t="s">
+      <c r="P2" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="Q2" s="36" t="s">
+      <c r="Q2" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="R2" s="32" t="str">
+      <c r="R2" s="31" t="str">
         <f>_xlfn.CONCAT("[kg], ",'Input_Project specific'!E19)</f>
         <v>[kg], Minimal</v>
       </c>
-      <c r="S2" s="36" t="s">
+      <c r="S2" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="T2" s="56" t="s">
+      <c r="T2" s="55" t="s">
         <v>366</v>
       </c>
-      <c r="U2" s="57" t="s">
+      <c r="U2" s="56" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="32" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="31" t="s">
         <v>285</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>286</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>287</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="31" t="s">
         <v>288</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="31" t="s">
         <v>289</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="31" t="s">
         <v>291</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="31" t="s">
         <v>292</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="31" t="s">
         <v>293</v>
       </c>
-      <c r="K3" s="32" t="s">
+      <c r="K3" s="31" t="s">
         <v>294</v>
       </c>
-      <c r="L3" s="32" t="s">
+      <c r="L3" s="31" t="s">
         <v>295</v>
       </c>
-      <c r="M3" s="33" t="s">
+      <c r="M3" s="32" t="s">
         <v>296</v>
       </c>
-      <c r="N3" s="34" t="s">
+      <c r="N3" s="33" t="s">
         <v>297</v>
       </c>
-      <c r="O3" s="35"/>
-      <c r="P3" s="36" t="s">
+      <c r="O3" s="34"/>
+      <c r="P3" s="35" t="s">
         <v>298</v>
       </c>
-      <c r="Q3" s="37" t="s">
+      <c r="Q3" s="36" t="s">
         <v>299</v>
       </c>
-      <c r="R3" s="38" t="s">
+      <c r="R3" s="37" t="s">
         <v>337</v>
       </c>
-      <c r="S3" s="36" t="s">
+      <c r="S3" s="35" t="s">
         <v>300</v>
       </c>
-      <c r="T3" s="57" t="s">
+      <c r="T3" s="56" t="s">
         <v>367</v>
       </c>
-      <c r="U3" s="57" t="s">
+      <c r="U3" s="56" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>306</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="30">
         <v>1.5</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="30">
         <v>5</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="30">
         <v>40</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="30">
         <v>80</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="30">
         <v>10</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="30">
         <f t="shared" ref="G4:G12" si="0">AVERAGE(F4,H4)</f>
         <v>15</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="30">
         <v>20</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="30">
         <v>1.74</v>
       </c>
-      <c r="J4" s="31">
+      <c r="J4" s="30">
         <v>1.3859999999999999</v>
       </c>
-      <c r="K4" s="42">
+      <c r="K4" s="41">
         <f t="shared" ref="K4:M12" si="1">$J4*F4</f>
         <v>13.86</v>
       </c>
-      <c r="L4" s="42">
+      <c r="L4" s="41">
         <f t="shared" si="1"/>
         <v>20.79</v>
       </c>
-      <c r="M4" s="43">
+      <c r="M4" s="42">
         <f t="shared" si="1"/>
         <v>27.72</v>
       </c>
-      <c r="N4" s="44" t="s">
+      <c r="N4" s="43" t="s">
         <v>307</v>
       </c>
-      <c r="O4" s="45">
+      <c r="O4" s="44">
         <v>20</v>
       </c>
-      <c r="P4" s="46">
+      <c r="P4" s="45">
         <f t="shared" ref="P4:P12" si="2">($L4/rho_r)^(1/3)</f>
         <v>0.19996794358015296</v>
       </c>
-      <c r="Q4" s="46">
+      <c r="Q4" s="45">
         <f t="shared" ref="Q4:Q12" si="3">Lt*P4</f>
         <v>0.36394165731587841</v>
       </c>
-      <c r="R4" s="42">
+      <c r="R4" s="41">
         <f t="shared" ref="R4:R12" si="4">IF(weight_check="Minimal",$K4,IF(weight_check="Average",$L4," none"))</f>
         <v>13.86</v>
       </c>
-      <c r="S4" s="46">
+      <c r="S4" s="45">
         <f t="shared" ref="S4:S12" si="5">($K4/rho_r)^(1/3)</f>
         <v>0.17468808908511205</v>
       </c>
-      <c r="T4" s="58" t="s">
+      <c r="T4" s="57" t="s">
         <v>363</v>
       </c>
-      <c r="U4" s="59" t="s">
+      <c r="U4" s="58" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="30" t="s">
         <v>308</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="30">
         <v>2</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="30">
         <v>10</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="30">
         <v>60</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="30">
         <v>120</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="30">
         <v>20</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="30">
         <f t="shared" si="0"/>
         <v>27.5</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="30">
         <v>35</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="30">
         <v>2.02</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="30">
         <v>1.3520000000000001</v>
       </c>
-      <c r="K5" s="42">
+      <c r="K5" s="41">
         <f t="shared" si="1"/>
         <v>27.040000000000003</v>
       </c>
-      <c r="L5" s="42">
+      <c r="L5" s="41">
         <f t="shared" si="1"/>
         <v>37.18</v>
       </c>
-      <c r="M5" s="43">
+      <c r="M5" s="42">
         <f t="shared" si="1"/>
         <v>47.32</v>
       </c>
-      <c r="N5" s="44" t="s">
+      <c r="N5" s="43" t="s">
         <v>309</v>
       </c>
-      <c r="O5" s="45">
+      <c r="O5" s="44">
         <v>35</v>
       </c>
-      <c r="P5" s="46">
+      <c r="P5" s="45">
         <f t="shared" si="2"/>
         <v>0.24272360429169446</v>
       </c>
-      <c r="Q5" s="46">
+      <c r="Q5" s="45">
         <f t="shared" si="3"/>
         <v>0.44175695981088392</v>
       </c>
-      <c r="R5" s="42">
+      <c r="R5" s="41">
         <f t="shared" si="4"/>
         <v>27.040000000000003</v>
       </c>
-      <c r="S5" s="46">
+      <c r="S5" s="45">
         <f t="shared" si="5"/>
         <v>0.21827857661222116</v>
       </c>
-      <c r="T5" s="58" t="s">
+      <c r="T5" s="57" t="s">
         <v>363</v>
       </c>
-      <c r="U5" s="59" t="s">
+      <c r="U5" s="58" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>310</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="30">
         <v>15</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="30">
         <v>40</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="30">
         <v>200</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="30">
         <v>300</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="30">
         <v>80</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="30">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="30">
         <v>120</v>
       </c>
-      <c r="I6" s="31">
+      <c r="I6" s="30">
         <v>2.25</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="30">
         <v>1.2689999999999999</v>
       </c>
-      <c r="K6" s="42">
+      <c r="K6" s="41">
         <f t="shared" si="1"/>
         <v>101.52</v>
       </c>
-      <c r="L6" s="42">
+      <c r="L6" s="41">
         <f t="shared" si="1"/>
         <v>126.89999999999999</v>
       </c>
-      <c r="M6" s="43">
+      <c r="M6" s="42">
         <f t="shared" si="1"/>
         <v>152.28</v>
       </c>
-      <c r="N6" s="44" t="s">
+      <c r="N6" s="43" t="s">
         <v>311</v>
       </c>
-      <c r="O6" s="45">
+      <c r="O6" s="44">
         <v>120</v>
       </c>
-      <c r="P6" s="46">
+      <c r="P6" s="45">
         <f t="shared" si="2"/>
         <v>0.36545122729011309</v>
       </c>
-      <c r="Q6" s="46">
+      <c r="Q6" s="45">
         <f t="shared" si="3"/>
         <v>0.6651212336680058</v>
       </c>
-      <c r="R6" s="42">
+      <c r="R6" s="41">
         <f t="shared" si="4"/>
         <v>101.52</v>
       </c>
-      <c r="S6" s="46">
+      <c r="S6" s="45">
         <f t="shared" si="5"/>
         <v>0.33925486716397496</v>
       </c>
-      <c r="T6" s="58" t="s">
+      <c r="T6" s="57" t="s">
         <v>363</v>
       </c>
-      <c r="U6" s="59" t="s">
+      <c r="U6" s="58" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="30" t="s">
         <v>312</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="30">
         <v>30</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="30">
         <v>60</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="30">
         <v>300</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="30">
         <v>450</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="30">
         <v>120</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="30">
         <f t="shared" si="0"/>
         <v>155</v>
       </c>
-      <c r="H7" s="31">
+      <c r="H7" s="30">
         <v>190</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="30">
         <v>2.25</v>
       </c>
-      <c r="J7" s="31">
+      <c r="J7" s="30">
         <v>1.2430000000000001</v>
       </c>
-      <c r="K7" s="42">
+      <c r="K7" s="41">
         <f t="shared" si="1"/>
         <v>149.16000000000003</v>
       </c>
-      <c r="L7" s="42">
+      <c r="L7" s="41">
         <f t="shared" si="1"/>
         <v>192.66500000000002</v>
       </c>
-      <c r="M7" s="43">
+      <c r="M7" s="42">
         <f t="shared" si="1"/>
         <v>236.17000000000002</v>
       </c>
-      <c r="N7" s="44" t="s">
+      <c r="N7" s="43" t="s">
         <v>313</v>
       </c>
-      <c r="O7" s="45">
+      <c r="O7" s="44">
         <v>190</v>
       </c>
-      <c r="P7" s="46">
+      <c r="P7" s="45">
         <f t="shared" si="2"/>
         <v>0.4200263080212468</v>
       </c>
-      <c r="Q7" s="46">
+      <c r="Q7" s="45">
         <f t="shared" si="3"/>
         <v>0.76444788059866919</v>
       </c>
-      <c r="R7" s="42">
+      <c r="R7" s="41">
         <f t="shared" si="4"/>
         <v>149.16000000000003</v>
       </c>
-      <c r="S7" s="46">
+      <c r="S7" s="45">
         <f t="shared" si="5"/>
         <v>0.38567931065615685</v>
       </c>
-      <c r="T7" s="58" t="s">
+      <c r="T7" s="57" t="s">
         <v>363</v>
       </c>
-      <c r="U7" s="59" t="s">
+      <c r="U7" s="58" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="30" t="s">
         <v>380</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="30">
         <v>200</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="30">
         <v>300</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="30">
         <v>1000</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="30">
         <v>1500</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="30">
         <v>540</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="30">
         <f t="shared" si="0"/>
         <v>615</v>
       </c>
-      <c r="H8" s="31">
+      <c r="H8" s="30">
         <v>690</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="30">
         <v>3</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="30">
         <v>1.163</v>
       </c>
-      <c r="K8" s="42">
+      <c r="K8" s="41">
         <f t="shared" si="1"/>
         <v>628.02</v>
       </c>
-      <c r="L8" s="42">
+      <c r="L8" s="41">
         <f t="shared" si="1"/>
         <v>715.245</v>
       </c>
-      <c r="M8" s="43">
+      <c r="M8" s="42">
         <f t="shared" si="1"/>
         <v>802.47</v>
       </c>
-      <c r="N8" s="44" t="s">
+      <c r="N8" s="43" t="s">
         <v>314</v>
       </c>
-      <c r="O8" s="45">
+      <c r="O8" s="44">
         <v>690</v>
       </c>
-      <c r="P8" s="46">
+      <c r="P8" s="45">
         <f t="shared" si="2"/>
         <v>0.65036999114505645</v>
       </c>
-      <c r="Q8" s="46">
+      <c r="Q8" s="45">
         <f t="shared" si="3"/>
         <v>1.1836733838840028</v>
       </c>
-      <c r="R8" s="42">
+      <c r="R8" s="41">
         <f t="shared" si="4"/>
         <v>628.02</v>
       </c>
-      <c r="S8" s="46">
+      <c r="S8" s="45">
         <f t="shared" si="5"/>
         <v>0.62277816214005777</v>
       </c>
-      <c r="T8" s="58" t="s">
+      <c r="T8" s="57" t="s">
         <v>363</v>
       </c>
-      <c r="U8" s="59" t="s">
+      <c r="U8" s="58" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="B9" s="34">
+      <c r="B9" s="33">
         <v>700</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="30">
         <v>1000</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="30">
         <v>3000</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="30">
         <v>4500</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F9" s="30">
         <v>1700</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="30">
         <f t="shared" si="0"/>
         <v>1900</v>
       </c>
-      <c r="H9" s="31">
+      <c r="H9" s="30">
         <v>2100</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="30">
         <v>3.29</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="30">
         <v>1.099</v>
       </c>
-      <c r="K9" s="42">
+      <c r="K9" s="41">
         <f t="shared" si="1"/>
         <v>1868.3</v>
       </c>
-      <c r="L9" s="42">
+      <c r="L9" s="41">
         <f t="shared" si="1"/>
         <v>2088.1</v>
       </c>
-      <c r="M9" s="43">
+      <c r="M9" s="42">
         <f t="shared" si="1"/>
         <v>2307.9</v>
       </c>
-      <c r="N9" s="44" t="s">
+      <c r="N9" s="43" t="s">
         <v>316</v>
       </c>
-      <c r="O9" s="45">
+      <c r="O9" s="44">
         <v>2100</v>
       </c>
-      <c r="P9" s="46">
+      <c r="P9" s="45">
         <f t="shared" si="2"/>
         <v>0.92952123374931728</v>
       </c>
-      <c r="Q9" s="46">
+      <c r="Q9" s="45">
         <f t="shared" si="3"/>
         <v>1.6917286454237574</v>
       </c>
-      <c r="R9" s="42">
+      <c r="R9" s="41">
         <f t="shared" si="4"/>
         <v>1868.3</v>
       </c>
-      <c r="S9" s="46">
+      <c r="S9" s="45">
         <f t="shared" si="5"/>
         <v>0.89569006135575246</v>
       </c>
-      <c r="T9" s="58" t="s">
+      <c r="T9" s="57" t="s">
         <v>363</v>
       </c>
-      <c r="U9" s="55" t="s">
+      <c r="U9" s="54" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="30">
         <v>2000</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="30">
         <v>3000</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="30">
         <v>6000</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="30">
         <v>9000</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="30">
         <v>4200</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="30">
         <f t="shared" si="0"/>
         <v>4500</v>
       </c>
-      <c r="H10" s="31">
+      <c r="H10" s="30">
         <v>4800</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="30">
         <v>5.22</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="30">
         <v>1.054</v>
       </c>
-      <c r="K10" s="42">
+      <c r="K10" s="41">
         <f t="shared" si="1"/>
         <v>4426.8</v>
       </c>
-      <c r="L10" s="42">
+      <c r="L10" s="41">
         <f t="shared" si="1"/>
         <v>4743</v>
       </c>
-      <c r="M10" s="43">
+      <c r="M10" s="42">
         <f t="shared" si="1"/>
         <v>5059.2</v>
       </c>
-      <c r="N10" s="44" t="s">
+      <c r="N10" s="43" t="s">
         <v>318</v>
       </c>
-      <c r="O10" s="45">
+      <c r="O10" s="44">
         <v>4800</v>
       </c>
-      <c r="P10" s="46">
+      <c r="P10" s="45">
         <f t="shared" si="2"/>
         <v>1.2218744743060006</v>
       </c>
-      <c r="Q10" s="46">
+      <c r="Q10" s="45">
         <f t="shared" si="3"/>
         <v>2.2238115432369212</v>
       </c>
-      <c r="R10" s="42">
+      <c r="R10" s="41">
         <f t="shared" si="4"/>
         <v>4426.8</v>
       </c>
-      <c r="S10" s="46">
+      <c r="S10" s="45">
         <f t="shared" si="5"/>
         <v>1.1940949209898202</v>
       </c>
-      <c r="T10" s="55" t="s">
+      <c r="T10" s="54" t="s">
         <v>310</v>
       </c>
-      <c r="U10" s="55" t="s">
+      <c r="U10" s="54" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>319</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="30">
         <v>4000</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="30">
         <v>6000</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="30">
         <v>10000</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="30">
         <v>15000</v>
       </c>
-      <c r="F11" s="31">
+      <c r="F11" s="30">
         <v>7500</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="30">
         <f t="shared" si="0"/>
         <v>8000</v>
       </c>
-      <c r="H11" s="31">
+      <c r="H11" s="30">
         <v>8500</v>
       </c>
-      <c r="I11" s="31">
+      <c r="I11" s="30">
         <v>7.08</v>
       </c>
-      <c r="J11" s="31">
+      <c r="J11" s="30">
         <v>1.024</v>
       </c>
-      <c r="K11" s="42">
+      <c r="K11" s="41">
         <f t="shared" si="1"/>
         <v>7680</v>
       </c>
-      <c r="L11" s="42">
+      <c r="L11" s="41">
         <f t="shared" si="1"/>
         <v>8192</v>
       </c>
-      <c r="M11" s="43">
+      <c r="M11" s="42">
         <f t="shared" si="1"/>
         <v>8704</v>
       </c>
-      <c r="N11" s="44" t="s">
+      <c r="N11" s="43" t="s">
         <v>320</v>
       </c>
-      <c r="O11" s="45">
+      <c r="O11" s="44">
         <v>8500</v>
       </c>
-      <c r="P11" s="46">
+      <c r="P11" s="45">
         <f t="shared" si="2"/>
         <v>1.4660165233186864</v>
       </c>
-      <c r="Q11" s="46">
+      <c r="Q11" s="45">
         <f t="shared" si="3"/>
         <v>2.6681500724400093</v>
       </c>
-      <c r="R11" s="42">
+      <c r="R11" s="41">
         <f t="shared" si="4"/>
         <v>7680</v>
       </c>
-      <c r="S11" s="46">
+      <c r="S11" s="45">
         <f t="shared" si="5"/>
         <v>1.4348151621398011</v>
       </c>
-      <c r="T11" s="58"/>
-      <c r="U11" s="59"/>
+      <c r="T11" s="57"/>
+      <c r="U11" s="58"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="30" t="s">
         <v>321</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="30">
         <v>6500</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="30">
         <v>10000</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="30">
         <v>15000</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="30">
         <v>22500</v>
       </c>
-      <c r="F12" s="31">
+      <c r="F12" s="30">
         <v>12000</v>
       </c>
-      <c r="G12" s="31">
+      <c r="G12" s="30">
         <f t="shared" si="0"/>
         <v>12500</v>
       </c>
-      <c r="H12" s="31">
+      <c r="H12" s="30">
         <v>13000</v>
       </c>
-      <c r="I12" s="31">
+      <c r="I12" s="30">
         <v>8.92</v>
       </c>
-      <c r="J12" s="31">
+      <c r="J12" s="30">
         <v>1.002</v>
       </c>
-      <c r="K12" s="42">
+      <c r="K12" s="41">
         <f t="shared" si="1"/>
         <v>12024</v>
       </c>
-      <c r="L12" s="42">
+      <c r="L12" s="41">
         <f t="shared" si="1"/>
         <v>12525</v>
       </c>
-      <c r="M12" s="43">
+      <c r="M12" s="42">
         <f t="shared" si="1"/>
         <v>13026</v>
       </c>
-      <c r="N12" s="44" t="s">
+      <c r="N12" s="43" t="s">
         <v>322</v>
       </c>
-      <c r="O12" s="45">
+      <c r="O12" s="44">
         <v>13000</v>
       </c>
-      <c r="P12" s="46">
+      <c r="P12" s="45">
         <f t="shared" si="2"/>
         <v>1.6888903809640281</v>
       </c>
-      <c r="Q12" s="46">
+      <c r="Q12" s="45">
         <f t="shared" si="3"/>
         <v>3.0737804933545312</v>
       </c>
-      <c r="R12" s="42">
+      <c r="R12" s="41">
         <f t="shared" si="4"/>
         <v>12024</v>
       </c>
-      <c r="S12" s="46">
+      <c r="S12" s="45">
         <f t="shared" si="5"/>
         <v>1.6660647399016293</v>
       </c>
-      <c r="T12" s="58"/>
-      <c r="U12" s="59"/>
+      <c r="T12" s="57"/>
+      <c r="U12" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12137,7 +12180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BADE3C9-F1E8-4518-8FC3-9DDBC15FFDFD}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -12406,6 +12449,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008ABF17219AE49A4BA0BDD81D071BF678" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27f34586c84b8c90a2cb002f0f0fc035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fc9abb88-5dc8-4425-a823-e2986ac3f199" xmlns:ns4="13eb6276-85db-4ef3-a671-167ab07ac255" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ec505085f4519de6c764bdf3897c86a" ns3:_="" ns4:_="">
     <xsd:import namespace="fc9abb88-5dc8-4425-a823-e2986ac3f199"/>
@@ -12634,22 +12692,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A202D3EF-E74A-4B50-BD9D-588EBDA690CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="13eb6276-85db-4ef3-a671-167ab07ac255"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fc9abb88-5dc8-4425-a823-e2986ac3f199"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60595BF4-BDC7-43A9-9318-C73E99FECE97}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12666,29 +12734,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A202D3EF-E74A-4B50-BD9D-588EBDA690CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="13eb6276-85db-4ef3-a671-167ab07ac255"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fc9abb88-5dc8-4425-a823-e2986ac3f199"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add comments for single run
</commit_message>
<xml_diff>
--- a/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
+++ b/Notebooks/Constanta Phase III/Input data/test_data_phase_II.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JY6\github\breakwater\Notebooks\Constanta Phase III\Input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B49F237-E56C-4AAE-A627-9B36B4D8112B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{25E0FC4E-069F-4EED-AA71-9F127AF6FE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="709" firstSheet="1" activeTab="8" xr2:uid="{06ED436A-2CC0-4489-A506-29F94518B839}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="709" firstSheet="1" activeTab="2" xr2:uid="{06ED436A-2CC0-4489-A506-29F94518B839}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="384">
   <si>
     <t>Input</t>
   </si>
@@ -1644,6 +1644,46 @@
   </cellStyles>
   <dxfs count="48">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -1749,16 +1789,6 @@
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1968,16 +1998,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2122,16 +2142,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -2213,16 +2223,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2237,7 +2237,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{128A59F9-895D-4C60-8954-4F77FF691FFB}" name="Overview" displayName="Overview" ref="A2:G62" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{128A59F9-895D-4C60-8954-4F77FF691FFB}" name="Overview" displayName="Overview" ref="A2:G62" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45">
   <autoFilter ref="A2:G62" xr:uid="{C615D3FE-C5C3-4AC1-8573-2115046F6FC7}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{FDED3D30-FC03-4894-AAAE-7069E3558798}" name="Input"/>
@@ -2245,8 +2245,8 @@
     <tableColumn id="3" xr3:uid="{122DBA8D-3347-48F4-8A76-270615744B5D}" name="Unit"/>
     <tableColumn id="4" xr3:uid="{B4BA3D29-867B-4EF8-A808-EE6581BB8115}" name="Category"/>
     <tableColumn id="5" xr3:uid="{CB74FB27-39F6-4359-BAC6-C5DFAC8E01C0}" name="Used for"/>
-    <tableColumn id="6" xr3:uid="{266927E0-00C5-4D6A-BB41-21164D34B2CE}" name="Necessary input" dataDxfId="43"/>
-    <tableColumn id="7" xr3:uid="{30AC8882-C2A6-43C1-86B7-25C9ED481C62}" name="Remarks" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{266927E0-00C5-4D6A-BB41-21164D34B2CE}" name="Necessary input" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{30AC8882-C2A6-43C1-86B7-25C9ED481C62}" name="Remarks" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2301,63 +2301,63 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{51C39BE7-D5C7-40C5-A499-C0C1F391598A}" name="input_concrete_elements" displayName="input_concrete_elements" ref="A2:F4" totalsRowShown="0">
-  <autoFilter ref="A2:F4" xr:uid="{51C39BE7-D5C7-40C5-A499-C0C1F391598A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{51C39BE7-D5C7-40C5-A499-C0C1F391598A}" name="input_concrete_elements" displayName="input_concrete_elements" ref="A2:F5" totalsRowShown="0">
+  <autoFilter ref="A2:F5" xr:uid="{51C39BE7-D5C7-40C5-A499-C0C1F391598A}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{32645932-B206-41E7-B1E9-2A52D9AE0D60}" name="Limit State"/>
     <tableColumn id="1" xr3:uid="{B6826C86-D95D-4464-8196-B4E1CEBC5F0A}" name="Nod"/>
-    <tableColumn id="2" xr3:uid="{12FE237E-CE70-4E63-BE4C-9D0365BAB8AC}" name="Accropode II-trunk" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{3045C02B-DCDC-42A1-B50F-88D0E610E62A}" name="Accropode II-roundhead" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{0280B610-A0B2-48C8-AB40-3AE6F87EDE4A}" name="Xbloc-trunk" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{C26BCBB6-089E-47C5-9394-EA17687F6843}" name="Xbloc-roundhead" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{12FE237E-CE70-4E63-BE4C-9D0365BAB8AC}" name="Accropode II-trunk" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{3045C02B-DCDC-42A1-B50F-88D0E610E62A}" name="Accropode II-roundhead" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{0280B610-A0B2-48C8-AB40-3AE6F87EDE4A}" name="Xbloc-trunk" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{C26BCBB6-089E-47C5-9394-EA17687F6843}" name="Xbloc-roundhead" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{88915663-9067-4DC4-90A4-2D7CD517273B}" name="input_project" displayName="input_project" ref="A1:E29" totalsRowShown="0" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{88915663-9067-4DC4-90A4-2D7CD517273B}" name="input_project" displayName="input_project" ref="A1:E29" totalsRowShown="0" dataDxfId="38">
   <autoFilter ref="A1:E29" xr:uid="{8653FB80-28B1-42DD-ADDB-1F402573EE6E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{10575A1B-65C2-4D3D-A919-D5D631E15E73}" name="Parameter" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{9F5575C0-7208-43BD-86BC-6A3485FF384C}" name="Symbol" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{1CF28AEF-1CBA-48D2-A66A-EE6DC73C8CC9}" name="Unit " dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{FB5987BB-56D7-412F-8C95-1F5820C3E77A}" name="Explanation" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{5ABE4DA7-DB09-46BC-AF34-3D5B699627F3}" name="Value" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{10575A1B-65C2-4D3D-A919-D5D631E15E73}" name="Parameter" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{9F5575C0-7208-43BD-86BC-6A3485FF384C}" name="Symbol" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{1CF28AEF-1CBA-48D2-A66A-EE6DC73C8CC9}" name="Unit " dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{FB5987BB-56D7-412F-8C95-1F5820C3E77A}" name="Explanation" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{5ABE4DA7-DB09-46BC-AF34-3D5B699627F3}" name="Value" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6634BB44-66AA-43C5-94C9-21ADB80AD51A}" name="input_requirements" displayName="input_requirements" ref="A1:G6" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6634BB44-66AA-43C5-94C9-21ADB80AD51A}" name="input_requirements" displayName="input_requirements" ref="A1:G6" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="A1:G6" xr:uid="{AC8FC8D0-6474-4C46-AABC-7775C18E706C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{ED5624B9-4A0A-4F41-BA44-D0E02EE32577}" name="Parameter" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{2B068622-98F3-4E2A-BE8E-A97C121E3F4C}" name="Symbol" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{4BC1E5B1-1862-4E8F-8CC1-D2F05F356929}" name="Unit " dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{F431E098-CB44-4ACA-97A5-C64500DD9528}" name="Explanation" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{C6914755-DB47-4220-827C-0984890970A0}" name="ELS" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{D3A99EAE-B2C9-4E74-B3E2-A288F4532A21}" name="SLS" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{9350B3BA-690A-42F3-BB94-29E26F161B54}" name="ULS" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{ED5624B9-4A0A-4F41-BA44-D0E02EE32577}" name="Parameter" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{2B068622-98F3-4E2A-BE8E-A97C121E3F4C}" name="Symbol" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{4BC1E5B1-1862-4E8F-8CC1-D2F05F356929}" name="Unit " dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{F431E098-CB44-4ACA-97A5-C64500DD9528}" name="Explanation" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{C6914755-DB47-4220-827C-0984890970A0}" name="ELS" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{D3A99EAE-B2C9-4E74-B3E2-A288F4532A21}" name="SLS" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{9350B3BA-690A-42F3-BB94-29E26F161B54}" name="ULS" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5DFFFB11-DDA0-4FF0-A99C-C5B40B22BB0F}" name="input_cross_section" displayName="input_cross_section" ref="A2:N9" totalsRowShown="0" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5DFFFB11-DDA0-4FF0-A99C-C5B40B22BB0F}" name="input_cross_section" displayName="input_cross_section" ref="A2:N9" totalsRowShown="0" tableBorderDxfId="22">
   <autoFilter ref="A2:N9" xr:uid="{EDBA852A-A4D9-4055-8891-B74537BE60D1}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{65F89A4D-13BC-480A-9A54-9B5181E61222}" name="Structure" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{DD7D1624-C590-49ED-8883-96E10DDFDC57}" name="Chainage" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{56CAAB95-7C5D-4C77-9690-8C7E28E5E58F}" name="dir_structure" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{65F89A4D-13BC-480A-9A54-9B5181E61222}" name="Structure" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{DD7D1624-C590-49ED-8883-96E10DDFDC57}" name="Chainage" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{56CAAB95-7C5D-4C77-9690-8C7E28E5E58F}" name="dir_structure" dataDxfId="19"/>
     <tableColumn id="4" xr3:uid="{3211485F-4253-4196-9552-5388E1C18679}" name="z_bed"/>
     <tableColumn id="5" xr3:uid="{12FF2071-DB6F-4635-AAF2-7224DB03F7AF}" name="public"/>
     <tableColumn id="6" xr3:uid="{3C50E8D0-D9A3-4D42-9184-21A91AB97D26}" name="P"/>
-    <tableColumn id="7" xr3:uid="{67557D02-D417-4935-83D4-56C7A3EC4E57}" name="tan_a" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{67557D02-D417-4935-83D4-56C7A3EC4E57}" name="tan_a" dataDxfId="18"/>
     <tableColumn id="9" xr3:uid="{0A204ACD-A807-4615-BEB7-8F6AA353A3CD}" name="Gc"/>
-    <tableColumn id="10" xr3:uid="{0003E8D8-CC23-4555-A626-BC13BBABE9B8}" name="slope_foreshore" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{0003E8D8-CC23-4555-A626-BC13BBABE9B8}" name="slope_foreshore" dataDxfId="17"/>
     <tableColumn id="12" xr3:uid="{74307101-79D4-4197-A798-20BAE3C12767}" name="crest_roughness"/>
     <tableColumn id="13" xr3:uid="{30E9BE3D-820F-4565-AD86-93CC1E7A860F}" name="cot_a_rear"/>
     <tableColumn id="14" xr3:uid="{A3804960-2456-4577-852A-50CF47F120BD}" name="B"/>
@@ -2369,20 +2369,20 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A63CE4AC-CF5D-406B-B465-B4984FB45555}" name="input_hydrometeo" displayName="input_hydrometeo" ref="A2:K170" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A63CE4AC-CF5D-406B-B465-B4984FB45555}" name="input_hydrometeo" displayName="input_hydrometeo" ref="A2:K170" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A2:K170" xr:uid="{8EC5B0C1-E4CA-4C7B-AA39-695D226630E3}"/>
   <tableColumns count="11">
-    <tableColumn id="6" xr3:uid="{F9A5357A-5DE4-4408-A14A-E6698FD3755F}" name="Calculation_case" dataDxfId="10"/>
-    <tableColumn id="1" xr3:uid="{012C1F4F-AAC2-4FD0-A162-E004B1A207F9}" name="Structure" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{BE45E132-052E-4051-A5CC-2691B8D1D576}" name="Chainage" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{CE4FADC8-9574-4B7C-9E02-F0716073BF79}" name="Offshore bin" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{C0A99159-F33E-4796-BC72-CB4DE68B9FDE}" name="Limit State" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{240593D5-435F-4039-BD0D-5B8B3FDD3128}" name="wl" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{1A72D5A3-EEEE-48D4-B8C7-0BC7A1474131}" name="Hm0" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{937FF273-2A9A-4DA7-AC8F-B2F74F1681D7}" name="dir_wave" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{24ED7C68-4403-4BB0-A849-0C22B2AF55BB}" name="Tp" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{A397DA8E-DE81-4096-A083-356358DACD29}" name="Tm-1,0" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{17652E84-F087-4BBA-B4B9-CD36B5153566}" name="Tm0,2" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{F9A5357A-5DE4-4408-A14A-E6698FD3755F}" name="Calculation_case" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{012C1F4F-AAC2-4FD0-A162-E004B1A207F9}" name="Structure" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{BE45E132-052E-4051-A5CC-2691B8D1D576}" name="Chainage" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{CE4FADC8-9574-4B7C-9E02-F0716073BF79}" name="Offshore bin" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{C0A99159-F33E-4796-BC72-CB4DE68B9FDE}" name="Limit State" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{240593D5-435F-4039-BD0D-5B8B3FDD3128}" name="wl" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{1A72D5A3-EEEE-48D4-B8C7-0BC7A1474131}" name="Hm0" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{937FF273-2A9A-4DA7-AC8F-B2F74F1681D7}" name="dir_wave" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{24ED7C68-4403-4BB0-A849-0C22B2AF55BB}" name="Tp" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{A397DA8E-DE81-4096-A083-356358DACD29}" name="Tm-1,0" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{17652E84-F087-4BBA-B4B9-CD36B5153566}" name="Tm0,2" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2691,25 +2691,25 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
-    <col min="6" max="6" width="46.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="60.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="61.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" customWidth="1"/>
+    <col min="6" max="6" width="46.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="60.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="61.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B1" s="5"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>183</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>165</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>142</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>143</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>65</v>
       </c>
@@ -3249,7 +3249,7 @@
       </c>
       <c r="G26" s="22"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -3316,7 +3316,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>238</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>228</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>230</v>
       </c>
@@ -3549,7 +3549,7 @@
       </c>
       <c r="G40" s="22"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>107</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -3609,7 +3609,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>113</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>116</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>119</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>120</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>124</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>140</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>141</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>147</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>147</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>147</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>152</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>159</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>161</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>162</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>167</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>169</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>174</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>177</v>
       </c>
@@ -4040,7 +4040,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B1 B3:B1048576">
-    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4070,77 +4070,77 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>348</v>
       </c>
@@ -4157,23 +4157,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2A734E-EE5D-4E22-9A61-D491991AFF7E}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>270</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -4201,43 +4201,52 @@
         <v>275</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>209</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C4" s="27">
         <v>2.8</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D4" s="27">
         <v>2.5</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E4" s="28">
         <v>2.77</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F4" s="28">
         <v>2.57</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>210</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>0.5</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C5" s="27">
         <v>3.1</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D5" s="27">
         <v>2.8</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E5" s="27">
         <v>3.1</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F5" s="27">
         <v>2.9</v>
       </c>
     </row>
@@ -4257,16 +4266,16 @@
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" customWidth="1"/>
-    <col min="4" max="4" width="53.7109375" customWidth="1"/>
+    <col min="1" max="1" width="46.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" customWidth="1"/>
+    <col min="4" max="4" width="53.6640625" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>198</v>
       </c>
@@ -4283,7 +4292,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
         <v>6</v>
       </c>
@@ -4298,7 +4307,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>10</v>
       </c>
@@ -4313,7 +4322,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>183</v>
       </c>
@@ -4328,7 +4337,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>13</v>
       </c>
@@ -4343,7 +4352,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>245</v>
       </c>
@@ -4358,7 +4367,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>246</v>
       </c>
@@ -4373,7 +4382,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
         <v>247</v>
       </c>
@@ -4388,7 +4397,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
         <v>255</v>
       </c>
@@ -4403,7 +4412,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>256</v>
       </c>
@@ -4418,7 +4427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
         <v>257</v>
       </c>
@@ -4433,7 +4442,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="47" t="s">
         <v>258</v>
       </c>
@@ -4448,7 +4457,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="47" t="s">
         <v>152</v>
       </c>
@@ -4465,7 +4474,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="47" t="s">
         <v>338</v>
       </c>
@@ -4482,7 +4491,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="53" t="s">
         <v>264</v>
       </c>
@@ -4499,7 +4508,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="53" t="s">
         <v>277</v>
       </c>
@@ -4516,7 +4525,7 @@
         <v>1.077</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="53" t="s">
         <v>278</v>
       </c>
@@ -4533,7 +4542,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="53" t="s">
         <v>281</v>
       </c>
@@ -4550,7 +4559,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="53" t="s">
         <v>328</v>
       </c>
@@ -4567,7 +4576,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="53" t="s">
         <v>332</v>
       </c>
@@ -4584,7 +4593,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="53" t="s">
         <v>340</v>
       </c>
@@ -4601,7 +4610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="53" t="s">
         <v>342</v>
       </c>
@@ -4618,7 +4627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="53" t="s">
         <v>344</v>
       </c>
@@ -4635,7 +4644,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="53" t="s">
         <v>349</v>
       </c>
@@ -4652,7 +4661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="47" t="s">
         <v>359</v>
       </c>
@@ -4667,7 +4676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="53" t="s">
         <v>353</v>
       </c>
@@ -4684,7 +4693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="53" t="s">
         <v>356</v>
       </c>
@@ -4701,7 +4710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="53" t="s">
         <v>361</v>
       </c>
@@ -4716,7 +4725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="53" t="s">
         <v>381</v>
       </c>
@@ -4733,7 +4742,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B29">
-    <cfRule type="duplicateValues" dxfId="37" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4769,15 +4778,15 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
     <col min="5" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>198</v>
       </c>
@@ -4800,7 +4809,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>250</v>
       </c>
@@ -4821,7 +4830,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>251</v>
       </c>
@@ -4838,7 +4847,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>59</v>
       </c>
@@ -4857,7 +4866,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>62</v>
       </c>
@@ -4876,7 +4885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>165</v>
       </c>
@@ -4897,7 +4906,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="30" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4914,24 +4923,24 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.7109375" customWidth="1"/>
+    <col min="1" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C1" s="21" t="s">
         <v>252</v>
       </c>
@@ -4969,7 +4978,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>205</v>
       </c>
@@ -5013,7 +5022,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>212</v>
       </c>
@@ -5057,7 +5066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>212</v>
       </c>
@@ -5101,7 +5110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>212</v>
       </c>
@@ -5145,7 +5154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>212</v>
       </c>
@@ -5189,7 +5198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>212</v>
       </c>
@@ -5233,7 +5242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>212</v>
       </c>
@@ -5277,7 +5286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>212</v>
       </c>
@@ -5338,20 +5347,20 @@
       <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>249</v>
       </c>
@@ -5386,7 +5395,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="17">
         <v>1</v>
       </c>
@@ -5421,7 +5430,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>2</v>
       </c>
@@ -5456,7 +5465,7 @@
         <v>4.8499999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="17">
         <v>3</v>
       </c>
@@ -5491,7 +5500,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
         <v>4</v>
       </c>
@@ -5526,7 +5535,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>5</v>
       </c>
@@ -5561,7 +5570,7 @@
         <v>4.7699999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <v>6</v>
       </c>
@@ -5596,7 +5605,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <v>7</v>
       </c>
@@ -5631,7 +5640,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="17">
         <v>8</v>
       </c>
@@ -5666,7 +5675,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
         <v>9</v>
       </c>
@@ -5701,7 +5710,7 @@
         <v>2.74</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
         <v>10</v>
       </c>
@@ -5736,7 +5745,7 @@
         <v>4.79</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>11</v>
       </c>
@@ -5771,7 +5780,7 @@
         <v>6.61</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>12</v>
       </c>
@@ -5806,7 +5815,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
         <v>13</v>
       </c>
@@ -5841,7 +5850,7 @@
         <v>4.8899999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="17">
         <v>14</v>
       </c>
@@ -5876,7 +5885,7 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>15</v>
       </c>
@@ -5911,7 +5920,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="17">
         <v>16</v>
       </c>
@@ -5946,7 +5955,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="17">
         <v>17</v>
       </c>
@@ -5981,7 +5990,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="17">
         <v>18</v>
       </c>
@@ -6016,7 +6025,7 @@
         <v>4.91</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="17">
         <v>19</v>
       </c>
@@ -6051,7 +6060,7 @@
         <v>6.88</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="17">
         <v>20</v>
       </c>
@@ -6086,7 +6095,7 @@
         <v>6.52</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="17">
         <v>21</v>
       </c>
@@ -6121,7 +6130,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="17">
         <v>22</v>
       </c>
@@ -6156,7 +6165,7 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="17">
         <v>23</v>
       </c>
@@ -6191,7 +6200,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="17">
         <v>24</v>
       </c>
@@ -6226,7 +6235,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="17">
         <v>25</v>
       </c>
@@ -6261,7 +6270,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="17">
         <v>26</v>
       </c>
@@ -6296,7 +6305,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="17">
         <v>27</v>
       </c>
@@ -6331,7 +6340,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="17">
         <v>28</v>
       </c>
@@ -6366,7 +6375,7 @@
         <v>6.87</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="17">
         <v>29</v>
       </c>
@@ -6401,7 +6410,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="17">
         <v>30</v>
       </c>
@@ -6436,7 +6445,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="17">
         <v>31</v>
       </c>
@@ -6471,7 +6480,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="17">
         <v>32</v>
       </c>
@@ -6506,7 +6515,7 @@
         <v>2.76</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="17">
         <v>33</v>
       </c>
@@ -6541,7 +6550,7 @@
         <v>2.77</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="17">
         <v>34</v>
       </c>
@@ -6576,7 +6585,7 @@
         <v>5.77</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="17">
         <v>35</v>
       </c>
@@ -6611,7 +6620,7 @@
         <v>7.46</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="17">
         <v>36</v>
       </c>
@@ -6646,7 +6655,7 @@
         <v>7.11</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="17">
         <v>37</v>
       </c>
@@ -6681,7 +6690,7 @@
         <v>4.97</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="17">
         <v>38</v>
       </c>
@@ -6716,7 +6725,7 @@
         <v>4.08</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="17">
         <v>39</v>
       </c>
@@ -6751,7 +6760,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="17">
         <v>40</v>
       </c>
@@ -6786,7 +6795,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="17">
         <v>41</v>
       </c>
@@ -6821,7 +6830,7 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="17">
         <v>42</v>
       </c>
@@ -6856,7 +6865,7 @@
         <v>5.97</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="17">
         <v>43</v>
       </c>
@@ -6891,7 +6900,7 @@
         <v>7.56</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="17">
         <v>44</v>
       </c>
@@ -6926,7 +6935,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="17">
         <v>45</v>
       </c>
@@ -6961,7 +6970,7 @@
         <v>5.07</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="17">
         <v>46</v>
       </c>
@@ -6996,7 +7005,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="17">
         <v>47</v>
       </c>
@@ -7031,7 +7040,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="17">
         <v>48</v>
       </c>
@@ -7066,7 +7075,7 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="17">
         <v>49</v>
       </c>
@@ -7101,7 +7110,7 @@
         <v>3.37</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="17">
         <v>50</v>
       </c>
@@ -7136,7 +7145,7 @@
         <v>6.43</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="17">
         <v>51</v>
       </c>
@@ -7171,7 +7180,7 @@
         <v>7.83</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="17">
         <v>52</v>
       </c>
@@ -7206,7 +7215,7 @@
         <v>7.59</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="17">
         <v>53</v>
       </c>
@@ -7241,7 +7250,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="17">
         <v>54</v>
       </c>
@@ -7276,7 +7285,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="17">
         <v>55</v>
       </c>
@@ -7311,7 +7320,7 @@
         <v>4.22</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="17">
         <v>56</v>
       </c>
@@ -7346,7 +7355,7 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="17">
         <v>57</v>
       </c>
@@ -7381,7 +7390,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="17">
         <v>58</v>
       </c>
@@ -7416,7 +7425,7 @@
         <v>8.94</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="17">
         <v>59</v>
       </c>
@@ -7451,7 +7460,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="17">
         <v>60</v>
       </c>
@@ -7486,7 +7495,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="17">
         <v>61</v>
       </c>
@@ -7521,7 +7530,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="17">
         <v>62</v>
       </c>
@@ -7556,7 +7565,7 @@
         <v>6.71</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="17">
         <v>63</v>
       </c>
@@ -7591,7 +7600,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="17">
         <v>64</v>
       </c>
@@ -7626,7 +7635,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="17">
         <v>65</v>
       </c>
@@ -7661,7 +7670,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="17">
         <v>66</v>
       </c>
@@ -7696,7 +7705,7 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="17">
         <v>67</v>
       </c>
@@ -7731,7 +7740,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="17">
         <v>68</v>
       </c>
@@ -7766,7 +7775,7 @@
         <v>10.59</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="17">
         <v>69</v>
       </c>
@@ -7801,7 +7810,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="17">
         <v>70</v>
       </c>
@@ -7836,7 +7845,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="17">
         <v>71</v>
       </c>
@@ -7871,7 +7880,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" s="17">
         <v>72</v>
       </c>
@@ -7906,7 +7915,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="17">
         <v>73</v>
       </c>
@@ -7941,7 +7950,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="17">
         <v>74</v>
       </c>
@@ -7976,7 +7985,7 @@
         <v>9.2100000000000009</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="17">
         <v>75</v>
       </c>
@@ -8014,7 +8023,7 @@
       <c r="M77" s="7"/>
       <c r="N77" s="7"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="17">
         <v>76</v>
       </c>
@@ -8052,7 +8061,7 @@
       <c r="M78" s="7"/>
       <c r="N78" s="7"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" s="17">
         <v>77</v>
       </c>
@@ -8090,7 +8099,7 @@
       <c r="M79" s="7"/>
       <c r="N79" s="7"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" s="17">
         <v>78</v>
       </c>
@@ -8128,7 +8137,7 @@
       <c r="M80" s="7"/>
       <c r="N80" s="7"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="17">
         <v>79</v>
       </c>
@@ -8166,7 +8175,7 @@
       <c r="M81" s="7"/>
       <c r="N81" s="7"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="17">
         <v>80</v>
       </c>
@@ -8204,7 +8213,7 @@
       <c r="M82" s="7"/>
       <c r="N82" s="7"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="17">
         <v>81</v>
       </c>
@@ -8242,7 +8251,7 @@
       <c r="M83" s="7"/>
       <c r="N83" s="7"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="17">
         <v>82</v>
       </c>
@@ -8280,7 +8289,7 @@
       <c r="M84" s="7"/>
       <c r="N84" s="7"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" s="17">
         <v>83</v>
       </c>
@@ -8318,7 +8327,7 @@
       <c r="M85" s="7"/>
       <c r="N85" s="7"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" s="17">
         <v>84</v>
       </c>
@@ -8356,7 +8365,7 @@
       <c r="M86" s="7"/>
       <c r="N86" s="7"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" s="17">
         <v>85</v>
       </c>
@@ -8394,7 +8403,7 @@
       <c r="M87" s="7"/>
       <c r="N87" s="7"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" s="17">
         <v>86</v>
       </c>
@@ -8432,7 +8441,7 @@
       <c r="M88" s="7"/>
       <c r="N88" s="7"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" s="17">
         <v>87</v>
       </c>
@@ -8470,7 +8479,7 @@
       <c r="M89" s="7"/>
       <c r="N89" s="7"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" s="17">
         <v>88</v>
       </c>
@@ -8505,7 +8514,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" s="17">
         <v>89</v>
       </c>
@@ -8540,7 +8549,7 @@
         <v>5.61</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" s="17">
         <v>90</v>
       </c>
@@ -8575,7 +8584,7 @@
         <v>9.56</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" s="17">
         <v>91</v>
       </c>
@@ -8610,7 +8619,7 @@
         <v>10.29</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" s="17">
         <v>92</v>
       </c>
@@ -8645,7 +8654,7 @@
         <v>10.81</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" s="17">
         <v>93</v>
       </c>
@@ -8680,7 +8689,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" s="17">
         <v>94</v>
       </c>
@@ -8715,7 +8724,7 @@
         <v>7.44</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="17">
         <v>95</v>
       </c>
@@ -8750,7 +8759,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="17">
         <v>96</v>
       </c>
@@ -8785,7 +8794,7 @@
         <v>2.23</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="17">
         <v>97</v>
       </c>
@@ -8820,7 +8829,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="17">
         <v>98</v>
       </c>
@@ -8855,7 +8864,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="17">
         <v>99</v>
       </c>
@@ -8890,7 +8899,7 @@
         <v>10.32</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="17">
         <v>100</v>
       </c>
@@ -8925,7 +8934,7 @@
         <v>10.84</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="17">
         <v>101</v>
       </c>
@@ -8960,7 +8969,7 @@
         <v>8.51</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="17">
         <v>102</v>
       </c>
@@ -8995,7 +9004,7 @@
         <v>7.57</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="17">
         <v>103</v>
       </c>
@@ -9030,7 +9039,7 @@
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="17">
         <v>104</v>
       </c>
@@ -9065,7 +9074,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="17">
         <v>105</v>
       </c>
@@ -9100,7 +9109,7 @@
         <v>6.23</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="17">
         <v>106</v>
       </c>
@@ -9135,7 +9144,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="17">
         <v>107</v>
       </c>
@@ -9170,7 +9179,7 @@
         <v>10.43</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="17">
         <v>108</v>
       </c>
@@ -9205,7 +9214,7 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="17">
         <v>109</v>
       </c>
@@ -9240,7 +9249,7 @@
         <v>8.7200000000000006</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="17">
         <v>110</v>
       </c>
@@ -9275,7 +9284,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="17">
         <v>111</v>
       </c>
@@ -9310,7 +9319,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="17">
         <v>112</v>
       </c>
@@ -9345,7 +9354,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="17">
         <v>113</v>
       </c>
@@ -9380,7 +9389,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="17">
         <v>114</v>
       </c>
@@ -9415,7 +9424,7 @@
         <v>8.94</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="17">
         <v>115</v>
       </c>
@@ -9450,7 +9459,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="17">
         <v>116</v>
       </c>
@@ -9485,7 +9494,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="17">
         <v>117</v>
       </c>
@@ -9520,7 +9529,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="17">
         <v>118</v>
       </c>
@@ -9555,7 +9564,7 @@
         <v>6.71</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="17">
         <v>119</v>
       </c>
@@ -9590,7 +9599,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="17">
         <v>120</v>
       </c>
@@ -9625,7 +9634,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="17">
         <v>121</v>
       </c>
@@ -9660,7 +9669,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="17">
         <v>122</v>
       </c>
@@ -9695,7 +9704,7 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="17">
         <v>123</v>
       </c>
@@ -9730,7 +9739,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="17">
         <v>124</v>
       </c>
@@ -9765,7 +9774,7 @@
         <v>10.59</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="17">
         <v>125</v>
       </c>
@@ -9800,7 +9809,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="17">
         <v>126</v>
       </c>
@@ -9835,7 +9844,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="17">
         <v>127</v>
       </c>
@@ -9870,7 +9879,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="17">
         <v>128</v>
       </c>
@@ -9905,7 +9914,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="17">
         <v>129</v>
       </c>
@@ -9940,7 +9949,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" s="17">
         <v>130</v>
       </c>
@@ -9975,7 +9984,7 @@
         <v>9.2100000000000009</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" s="17">
         <v>131</v>
       </c>
@@ -10010,7 +10019,7 @@
         <v>10.11</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" s="17">
         <v>132</v>
       </c>
@@ -10045,7 +10054,7 @@
         <v>10.67</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" s="17">
         <v>133</v>
       </c>
@@ -10080,7 +10089,7 @@
         <v>8.11</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" s="17">
         <v>134</v>
       </c>
@@ -10115,7 +10124,7 @@
         <v>7.09</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137" s="17">
         <v>135</v>
       </c>
@@ -10150,7 +10159,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" s="17">
         <v>136</v>
       </c>
@@ -10185,7 +10194,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" s="17">
         <v>137</v>
       </c>
@@ -10220,7 +10229,7 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140" s="17">
         <v>138</v>
       </c>
@@ -10255,7 +10264,7 @@
         <v>9.4499999999999993</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141" s="17">
         <v>139</v>
       </c>
@@ -10290,7 +10299,7 @@
         <v>10.23</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142" s="17">
         <v>140</v>
       </c>
@@ -10325,7 +10334,7 @@
         <v>10.76</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" s="17">
         <v>141</v>
       </c>
@@ -10360,7 +10369,7 @@
         <v>8.31</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" s="17">
         <v>142</v>
       </c>
@@ -10395,7 +10404,7 @@
         <v>7.26</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" s="17">
         <v>143</v>
       </c>
@@ -10430,7 +10439,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" s="17">
         <v>144</v>
       </c>
@@ -10465,7 +10474,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" s="17">
         <v>145</v>
       </c>
@@ -10500,7 +10509,7 @@
         <v>5.61</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" s="17">
         <v>146</v>
       </c>
@@ -10535,7 +10544,7 @@
         <v>9.56</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149" s="17">
         <v>147</v>
       </c>
@@ -10570,7 +10579,7 @@
         <v>10.29</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150" s="17">
         <v>148</v>
       </c>
@@ -10605,7 +10614,7 @@
         <v>10.81</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151" s="17">
         <v>149</v>
       </c>
@@ -10640,7 +10649,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" s="17">
         <v>150</v>
       </c>
@@ -10675,7 +10684,7 @@
         <v>7.44</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" s="17">
         <v>151</v>
       </c>
@@ -10710,7 +10719,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154" s="17">
         <v>152</v>
       </c>
@@ -10745,7 +10754,7 @@
         <v>2.23</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" s="17">
         <v>153</v>
       </c>
@@ -10780,7 +10789,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" s="17">
         <v>154</v>
       </c>
@@ -10815,7 +10824,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157" s="17">
         <v>155</v>
       </c>
@@ -10850,7 +10859,7 @@
         <v>10.32</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" s="17">
         <v>156</v>
       </c>
@@ -10885,7 +10894,7 @@
         <v>10.84</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" s="17">
         <v>157</v>
       </c>
@@ -10920,7 +10929,7 @@
         <v>8.51</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" s="17">
         <v>158</v>
       </c>
@@ -10955,7 +10964,7 @@
         <v>7.57</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161" s="17">
         <v>159</v>
       </c>
@@ -10990,7 +10999,7 @@
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162" s="17">
         <v>160</v>
       </c>
@@ -11025,7 +11034,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163" s="17">
         <v>161</v>
       </c>
@@ -11060,7 +11069,7 @@
         <v>6.23</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164" s="17">
         <v>162</v>
       </c>
@@ -11095,7 +11104,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165" s="17">
         <v>163</v>
       </c>
@@ -11130,7 +11139,7 @@
         <v>10.43</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166" s="17">
         <v>164</v>
       </c>
@@ -11165,7 +11174,7 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167" s="17">
         <v>165</v>
       </c>
@@ -11200,7 +11209,7 @@
         <v>8.7200000000000006</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168" s="17">
         <v>166</v>
       </c>
@@ -11235,7 +11244,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169" s="17">
         <v>167</v>
       </c>
@@ -11270,7 +11279,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170" s="17">
         <v>168</v>
       </c>
@@ -11307,7 +11316,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11325,14 +11334,14 @@
       <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
-    <col min="20" max="20" width="19.85546875" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
+    <col min="20" max="20" width="19.88671875" customWidth="1"/>
+    <col min="21" max="21" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>284</v>
       </c>
@@ -11355,7 +11364,7 @@
       <c r="R1" s="30"/>
       <c r="S1" s="30"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>301</v>
       </c>
@@ -11417,7 +11426,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31"/>
       <c r="B3" s="32" t="s">
         <v>285</v>
@@ -11478,7 +11487,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>306</v>
       </c>
@@ -11551,7 +11560,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>308</v>
       </c>
@@ -11624,7 +11633,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>310</v>
       </c>
@@ -11697,7 +11706,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>312</v>
       </c>
@@ -11770,7 +11779,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>380</v>
       </c>
@@ -11843,7 +11852,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>315</v>
       </c>
@@ -11916,7 +11925,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>317</v>
       </c>
@@ -11989,7 +11998,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>319</v>
       </c>
@@ -12058,7 +12067,7 @@
       <c r="T11" s="58"/>
       <c r="U11" s="59"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>321</v>
       </c>
@@ -12137,22 +12146,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BADE3C9-F1E8-4518-8FC3-9DDBC15FFDFD}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="1" max="3" width="10.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="23.5546875" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
         <v>371</v>
       </c>
@@ -12163,7 +12172,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>205</v>
       </c>
@@ -12192,7 +12201,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>212</v>
       </c>
@@ -12218,7 +12227,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>212</v>
       </c>
@@ -12244,7 +12253,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>212</v>
       </c>
@@ -12270,7 +12279,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>212</v>
       </c>
@@ -12296,7 +12305,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>212</v>
       </c>
@@ -12322,7 +12331,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>212</v>
       </c>
@@ -12348,7 +12357,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>212</v>
       </c>
@@ -12374,7 +12383,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
@@ -12406,6 +12415,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008ABF17219AE49A4BA0BDD81D071BF678" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27f34586c84b8c90a2cb002f0f0fc035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fc9abb88-5dc8-4425-a823-e2986ac3f199" xmlns:ns4="13eb6276-85db-4ef3-a671-167ab07ac255" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ec505085f4519de6c764bdf3897c86a" ns3:_="" ns4:_="">
     <xsd:import namespace="fc9abb88-5dc8-4425-a823-e2986ac3f199"/>
@@ -12634,22 +12658,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A202D3EF-E74A-4B50-BD9D-588EBDA690CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="13eb6276-85db-4ef3-a671-167ab07ac255"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fc9abb88-5dc8-4425-a823-e2986ac3f199"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60595BF4-BDC7-43A9-9318-C73E99FECE97}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12666,29 +12700,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A202D3EF-E74A-4B50-BD9D-588EBDA690CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="13eb6276-85db-4ef3-a671-167ab07ac255"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fc9abb88-5dc8-4425-a823-e2986ac3f199"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>